<commit_message>
Update S_NV_CHUNG: remove permission.list, permission.structure
</commit_message>
<xml_diff>
--- a/apps/core/fixtures/core_permission.xlsx
+++ b/apps/core/fixtures/core_permission.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15660" tabRatio="894" firstSheet="10" activeTab="18"/>
+    <workbookView windowHeight="15660" tabRatio="894"/>
   </bookViews>
   <sheets>
     <sheet name="core_permission" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="1786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3675" uniqueCount="1786">
   <si>
     <t>code</t>
   </si>
@@ -126,6 +126,24 @@
     <t>Permission Management</t>
   </si>
   <si>
+    <t>permission.list</t>
+  </si>
+  <si>
+    <t>[Core] [Permission Management] Danh sách Quyền</t>
+  </si>
+  <si>
+    <t>Xem danh sách Quyền</t>
+  </si>
+  <si>
+    <t>permission.structure</t>
+  </si>
+  <si>
+    <t>[Core] [Permission Management] UNREGISTERED Structure Quyền</t>
+  </si>
+  <si>
+    <t>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Structure a Quyền</t>
+  </si>
+  <si>
     <t>role.create</t>
   </si>
   <si>
@@ -436,24 +454,6 @@
   </si>
   <si>
     <t>Xem chi tiết của Phiếu phạt</t>
-  </si>
-  <si>
-    <t>permission.list</t>
-  </si>
-  <si>
-    <t>[Core] [Permission Management] Danh sách Quyền</t>
-  </si>
-  <si>
-    <t>Xem danh sách Quyền</t>
-  </si>
-  <si>
-    <t>permission.structure</t>
-  </si>
-  <si>
-    <t>[Core] [Permission Management] UNREGISTERED Structure Quyền</t>
-  </si>
-  <si>
-    <t>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Structure a Quyền</t>
   </si>
   <si>
     <t>attendance_record.wifi_attendance</t>
@@ -6847,8 +6847,8 @@
   <sheetPr/>
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -6928,141 +6928,174 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="1"/>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B208" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C208" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D208" t="s">
         <v>8</v>
       </c>
       <c r="E208" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B209" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C209" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D209" t="s">
         <v>8</v>
       </c>
       <c r="E209" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B210" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C210" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D210" t="s">
         <v>8</v>
       </c>
       <c r="E210" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B211" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C211" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D211" t="s">
         <v>8</v>
       </c>
       <c r="E211" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B212" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C212" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D212" t="s">
         <v>8</v>
       </c>
       <c r="E212" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="213" customFormat="1" spans="1:5">
       <c r="A213" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B213" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C213" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D213" t="s">
         <v>8</v>
       </c>
       <c r="E213" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B214" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C214" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D214" t="s">
         <v>8</v>
       </c>
       <c r="E214" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="215" spans="1:5">
       <c r="A215" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B215" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C215" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D215" t="s">
         <v>8</v>
       </c>
       <c r="E215" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -7109,7 +7142,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7123,7 +7156,7 @@
         <v>1144</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>1145</v>
@@ -7143,7 +7176,7 @@
         <v>1149</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
         <v>1145</v>
@@ -7163,7 +7196,7 @@
         <v>1152</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>1145</v>
@@ -7183,7 +7216,7 @@
         <v>1155</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>1145</v>
@@ -7203,7 +7236,7 @@
         <v>1158</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>1145</v>
@@ -7223,7 +7256,7 @@
         <v>1161</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>1145</v>
@@ -7243,7 +7276,7 @@
         <v>1164</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>1145</v>
@@ -7263,7 +7296,7 @@
         <v>1167</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>1145</v>
@@ -7283,7 +7316,7 @@
         <v>1170</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>1145</v>
@@ -7303,7 +7336,7 @@
         <v>1173</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
         <v>1145</v>
@@ -7323,7 +7356,7 @@
         <v>1176</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>1145</v>
@@ -7343,7 +7376,7 @@
         <v>1179</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>1145</v>
@@ -7363,7 +7396,7 @@
         <v>1182</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
         <v>1145</v>
@@ -7383,7 +7416,7 @@
         <v>1144</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
         <v>1185</v>
@@ -7403,7 +7436,7 @@
         <v>1149</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
         <v>1185</v>
@@ -7423,7 +7456,7 @@
         <v>1152</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
         <v>1185</v>
@@ -7443,7 +7476,7 @@
         <v>1158</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
         <v>1185</v>
@@ -7463,7 +7496,7 @@
         <v>1161</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>1185</v>
@@ -7483,7 +7516,7 @@
         <v>1164</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
         <v>1185</v>
@@ -7503,7 +7536,7 @@
         <v>1167</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
         <v>1185</v>
@@ -7523,7 +7556,7 @@
         <v>1170</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
         <v>1185</v>
@@ -7543,7 +7576,7 @@
         <v>1173</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
         <v>1185</v>
@@ -7563,7 +7596,7 @@
         <v>1176</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>1185</v>
@@ -7583,7 +7616,7 @@
         <v>1179</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>1185</v>
@@ -7603,7 +7636,7 @@
         <v>1182</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
         <v>1185</v>
@@ -7623,7 +7656,7 @@
         <v>1210</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>1211</v>
@@ -7643,7 +7676,7 @@
         <v>1214</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
         <v>1211</v>
@@ -7663,7 +7696,7 @@
         <v>1217</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
         <v>1211</v>
@@ -7683,7 +7716,7 @@
         <v>1220</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>1211</v>
@@ -7703,7 +7736,7 @@
         <v>1223</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
         <v>1211</v>
@@ -7723,7 +7756,7 @@
         <v>1226</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
         <v>1211</v>
@@ -7743,7 +7776,7 @@
         <v>1229</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
         <v>1211</v>
@@ -7763,7 +7796,7 @@
         <v>1232</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
         <v>1211</v>
@@ -7783,7 +7816,7 @@
         <v>1235</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E35" t="s">
         <v>1211</v>
@@ -7837,7 +7870,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:6">
@@ -8014,7 +8047,7 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
         <v>1240</v>
@@ -8034,7 +8067,7 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
         <v>1240</v>
@@ -8405,7 +8438,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -8879,7 +8912,7 @@
         <v>1397</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>1398</v>
@@ -8899,7 +8932,7 @@
         <v>1401</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
         <v>1398</v>
@@ -8939,7 +8972,7 @@
         <v>1407</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
         <v>1398</v>
@@ -8959,7 +8992,7 @@
         <v>1410</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
         <v>1398</v>
@@ -8979,7 +9012,7 @@
         <v>1413</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>1398</v>
@@ -8999,7 +9032,7 @@
         <v>1416</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
         <v>1398</v>
@@ -9019,7 +9052,7 @@
         <v>1419</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
         <v>1398</v>
@@ -9039,7 +9072,7 @@
         <v>1422</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
         <v>1398</v>
@@ -9351,7 +9384,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -11593,7 +11626,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -12099,43 +12132,43 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" t="str">
-        <v>permission.list</v>
-      </c>
-      <c r="B27" t="str">
-        <v>[Core] [Permission Management] Danh sách Quyền</v>
-      </c>
-      <c r="C27" t="str">
-        <v>Xem danh sách Quyền</v>
-      </c>
-      <c r="D27" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E27" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F27" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="str">
-        <v>permission.structure</v>
-      </c>
-      <c r="B28" t="str">
-        <v>[Core] [Permission Management] UNREGISTERED Structure Quyền</v>
-      </c>
-      <c r="C28" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Structure a Quyền</v>
-      </c>
-      <c r="D28" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E28" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F28" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -12458,7 +12491,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -13358,7 +13391,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -13864,43 +13897,43 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" t="str">
-        <v>permission.list</v>
-      </c>
-      <c r="B27" t="str">
-        <v>[Core] [Permission Management] Danh sách Quyền</v>
-      </c>
-      <c r="C27" t="str">
-        <v>Xem danh sách Quyền</v>
-      </c>
-      <c r="D27" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E27" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F27" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="str">
-        <v>permission.structure</v>
-      </c>
-      <c r="B28" t="str">
-        <v>[Core] [Permission Management] UNREGISTERED Structure Quyền</v>
-      </c>
-      <c r="C28" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Structure a Quyền</v>
-      </c>
-      <c r="D28" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E28" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F28" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -16680,7 +16713,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -17467,43 +17500,43 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" t="str">
-        <v>permission.list</v>
-      </c>
-      <c r="B41" t="str">
-        <v>[Core] [Permission Management] Danh sách Quyền</v>
-      </c>
-      <c r="C41" t="str">
-        <v>Xem danh sách Quyền</v>
-      </c>
-      <c r="D41" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E41" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F41" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" t="str">
-        <v>permission.structure</v>
-      </c>
-      <c r="B42" t="str">
-        <v>[Core] [Permission Management] UNREGISTERED Structure Quyền</v>
-      </c>
-      <c r="C42" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Structure a Quyền</v>
-      </c>
-      <c r="D42" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E42" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F42" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -18882,7 +18915,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -19388,43 +19421,43 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" t="str">
-        <v>permission.list</v>
-      </c>
-      <c r="B27" t="str">
-        <v>[Core] [Permission Management] Danh sách Quyền</v>
-      </c>
-      <c r="C27" t="str">
-        <v>Xem danh sách Quyền</v>
-      </c>
-      <c r="D27" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E27" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F27" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="str">
-        <v>permission.structure</v>
-      </c>
-      <c r="B28" t="str">
-        <v>[Core] [Permission Management] UNREGISTERED Structure Quyền</v>
-      </c>
-      <c r="C28" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Structure a Quyền</v>
-      </c>
-      <c r="D28" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E28" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F28" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -28066,8 +28099,8 @@
   <sheetPr/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -28094,7 +28127,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -28881,43 +28914,43 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" t="str">
-        <v>permission.list</v>
-      </c>
-      <c r="B41" t="str">
-        <v>[Core] [Permission Management] Danh sách Quyền</v>
-      </c>
-      <c r="C41" t="str">
-        <v>Xem danh sách Quyền</v>
-      </c>
-      <c r="D41" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E41" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F41" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" t="str">
-        <v>permission.structure</v>
-      </c>
-      <c r="B42" t="str">
-        <v>[Core] [Permission Management] UNREGISTERED Structure Quyền</v>
-      </c>
-      <c r="C42" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Structure a Quyền</v>
-      </c>
-      <c r="D42" t="str">
-        <v>Core</v>
-      </c>
-      <c r="E42" t="str">
-        <v>Permission Management</v>
-      </c>
-      <c r="F42" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -29290,10 +29323,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A24" sqref="A24:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -29321,487 +29354,447 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:6">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
         <v>110</v>
       </c>
-      <c r="D20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" t="s">
-        <v>104</v>
-      </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -29846,7 +29839,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -29951,7 +29944,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -30279,7 +30272,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -30313,7 +30306,7 @@
         <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
         <v>186</v>
@@ -30333,7 +30326,7 @@
         <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>186</v>
@@ -30353,7 +30346,7 @@
         <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>186</v>
@@ -30373,7 +30366,7 @@
         <v>195</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>186</v>
@@ -30393,7 +30386,7 @@
         <v>198</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>186</v>
@@ -30413,7 +30406,7 @@
         <v>201</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>186</v>
@@ -30433,7 +30426,7 @@
         <v>204</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>186</v>
@@ -30453,7 +30446,7 @@
         <v>207</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>186</v>
@@ -30685,7 +30678,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -30699,7 +30692,7 @@
         <v>237</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>186</v>
@@ -30719,7 +30712,7 @@
         <v>241</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
         <v>186</v>
@@ -30739,7 +30732,7 @@
         <v>244</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>186</v>
@@ -30759,7 +30752,7 @@
         <v>247</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>186</v>
@@ -30779,7 +30772,7 @@
         <v>250</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>186</v>
@@ -30799,7 +30792,7 @@
         <v>253</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>186</v>
@@ -30819,7 +30812,7 @@
         <v>256</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>186</v>
@@ -30839,7 +30832,7 @@
         <v>259</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>186</v>
@@ -31099,7 +31092,7 @@
         <v>298</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
         <v>186</v>
@@ -31119,7 +31112,7 @@
         <v>301</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
         <v>186</v>
@@ -31139,7 +31132,7 @@
         <v>304</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>186</v>
@@ -31159,7 +31152,7 @@
         <v>307</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>186</v>
@@ -31179,7 +31172,7 @@
         <v>310</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
         <v>186</v>
@@ -31199,7 +31192,7 @@
         <v>313</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>186</v>
@@ -31219,7 +31212,7 @@
         <v>316</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
         <v>186</v>
@@ -31239,7 +31232,7 @@
         <v>319</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
         <v>186</v>
@@ -31259,7 +31252,7 @@
         <v>322</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>186</v>
@@ -31279,7 +31272,7 @@
         <v>325</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
         <v>186</v>
@@ -31299,7 +31292,7 @@
         <v>328</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
         <v>186</v>
@@ -31319,7 +31312,7 @@
         <v>331</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
         <v>186</v>
@@ -31339,7 +31332,7 @@
         <v>244</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
         <v>186</v>
@@ -31359,7 +31352,7 @@
         <v>247</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E35" t="s">
         <v>186</v>
@@ -31379,7 +31372,7 @@
         <v>336</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
         <v>186</v>
@@ -31399,7 +31392,7 @@
         <v>339</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
         <v>186</v>
@@ -31419,7 +31412,7 @@
         <v>342</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E38" t="s">
         <v>186</v>
@@ -31439,7 +31432,7 @@
         <v>345</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E39" t="s">
         <v>186</v>
@@ -31459,7 +31452,7 @@
         <v>348</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
         <v>186</v>
@@ -31479,7 +31472,7 @@
         <v>351</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
         <v>186</v>
@@ -31499,7 +31492,7 @@
         <v>354</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E42" t="s">
         <v>186</v>
@@ -31519,7 +31512,7 @@
         <v>357</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E43" t="s">
         <v>186</v>
@@ -31539,7 +31532,7 @@
         <v>360</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E44" t="s">
         <v>186</v>
@@ -31559,7 +31552,7 @@
         <v>363</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E45" t="s">
         <v>186</v>
@@ -31579,7 +31572,7 @@
         <v>366</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E46" t="s">
         <v>186</v>
@@ -31599,7 +31592,7 @@
         <v>369</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E47" t="s">
         <v>186</v>
@@ -31619,7 +31612,7 @@
         <v>372</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E48" t="s">
         <v>186</v>
@@ -31639,7 +31632,7 @@
         <v>375</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E49" t="s">
         <v>186</v>
@@ -31659,7 +31652,7 @@
         <v>378</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E50" t="s">
         <v>186</v>
@@ -31679,7 +31672,7 @@
         <v>381</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E51" t="s">
         <v>186</v>
@@ -31699,7 +31692,7 @@
         <v>384</v>
       </c>
       <c r="D52" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E52" t="s">
         <v>186</v>
@@ -31719,7 +31712,7 @@
         <v>387</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
         <v>186</v>
@@ -31739,7 +31732,7 @@
         <v>390</v>
       </c>
       <c r="D54" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E54" t="s">
         <v>186</v>
@@ -31759,7 +31752,7 @@
         <v>393</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E55" t="s">
         <v>186</v>
@@ -31779,7 +31772,7 @@
         <v>396</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E56" t="s">
         <v>186</v>
@@ -31799,7 +31792,7 @@
         <v>399</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E57" t="s">
         <v>186</v>
@@ -31819,7 +31812,7 @@
         <v>402</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E58" t="s">
         <v>186</v>
@@ -31839,7 +31832,7 @@
         <v>405</v>
       </c>
       <c r="D59" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E59" t="s">
         <v>186</v>
@@ -31859,7 +31852,7 @@
         <v>408</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E60" t="s">
         <v>186</v>
@@ -31879,7 +31872,7 @@
         <v>411</v>
       </c>
       <c r="D61" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E61" t="s">
         <v>186</v>
@@ -31899,7 +31892,7 @@
         <v>414</v>
       </c>
       <c r="D62" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E62" t="s">
         <v>186</v>
@@ -31919,7 +31912,7 @@
         <v>417</v>
       </c>
       <c r="D63" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E63" t="s">
         <v>186</v>
@@ -31939,7 +31932,7 @@
         <v>420</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E64" t="s">
         <v>186</v>
@@ -31959,7 +31952,7 @@
         <v>423</v>
       </c>
       <c r="D65" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E65" t="s">
         <v>186</v>
@@ -31979,7 +31972,7 @@
         <v>426</v>
       </c>
       <c r="D66" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E66" t="s">
         <v>186</v>
@@ -31999,7 +31992,7 @@
         <v>429</v>
       </c>
       <c r="D67" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E67" t="s">
         <v>186</v>
@@ -32019,7 +32012,7 @@
         <v>432</v>
       </c>
       <c r="D68" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E68" t="s">
         <v>186</v>
@@ -32039,7 +32032,7 @@
         <v>435</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E69" t="s">
         <v>186</v>
@@ -32059,7 +32052,7 @@
         <v>438</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E70" t="s">
         <v>186</v>
@@ -32079,7 +32072,7 @@
         <v>441</v>
       </c>
       <c r="D71" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E71" t="s">
         <v>186</v>
@@ -32099,7 +32092,7 @@
         <v>444</v>
       </c>
       <c r="D72" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E72" t="s">
         <v>186</v>
@@ -32119,7 +32112,7 @@
         <v>447</v>
       </c>
       <c r="D73" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E73" t="s">
         <v>186</v>
@@ -32139,7 +32132,7 @@
         <v>450</v>
       </c>
       <c r="D74" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E74" t="s">
         <v>186</v>
@@ -32159,7 +32152,7 @@
         <v>453</v>
       </c>
       <c r="D75" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E75" t="s">
         <v>186</v>
@@ -32299,7 +32292,7 @@
         <v>185</v>
       </c>
       <c r="D82" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E82" t="s">
         <v>186</v>
@@ -32319,7 +32312,7 @@
         <v>189</v>
       </c>
       <c r="D83" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E83" t="s">
         <v>186</v>
@@ -32339,7 +32332,7 @@
         <v>192</v>
       </c>
       <c r="D84" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E84" t="s">
         <v>186</v>
@@ -32359,7 +32352,7 @@
         <v>195</v>
       </c>
       <c r="D85" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E85" t="s">
         <v>186</v>
@@ -32379,7 +32372,7 @@
         <v>198</v>
       </c>
       <c r="D86" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E86" t="s">
         <v>186</v>
@@ -32399,7 +32392,7 @@
         <v>201</v>
       </c>
       <c r="D87" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E87" t="s">
         <v>186</v>
@@ -32419,7 +32412,7 @@
         <v>204</v>
       </c>
       <c r="D88" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E88" t="s">
         <v>186</v>
@@ -32439,7 +32432,7 @@
         <v>207</v>
       </c>
       <c r="D89" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E89" t="s">
         <v>186</v>
@@ -32459,7 +32452,7 @@
         <v>475</v>
       </c>
       <c r="D90" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E90" t="s">
         <v>186</v>
@@ -32479,7 +32472,7 @@
         <v>478</v>
       </c>
       <c r="D91" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E91" t="s">
         <v>186</v>
@@ -32499,7 +32492,7 @@
         <v>481</v>
       </c>
       <c r="D92" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E92" t="s">
         <v>186</v>
@@ -32519,7 +32512,7 @@
         <v>484</v>
       </c>
       <c r="D93" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E93" t="s">
         <v>186</v>
@@ -32539,7 +32532,7 @@
         <v>487</v>
       </c>
       <c r="D94" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E94" t="s">
         <v>186</v>
@@ -32559,7 +32552,7 @@
         <v>490</v>
       </c>
       <c r="D95" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E95" t="s">
         <v>186</v>
@@ -32579,7 +32572,7 @@
         <v>493</v>
       </c>
       <c r="D96" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E96" t="s">
         <v>186</v>
@@ -32599,7 +32592,7 @@
         <v>496</v>
       </c>
       <c r="D97" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E97" t="s">
         <v>186</v>
@@ -32619,7 +32612,7 @@
         <v>499</v>
       </c>
       <c r="D98" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E98" t="s">
         <v>186</v>
@@ -32672,7 +32665,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -32686,10 +32679,10 @@
         <v>502</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
         <v>503</v>
@@ -32706,10 +32699,10 @@
         <v>506</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
         <v>503</v>
@@ -32717,19 +32710,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
         <v>503</v>
@@ -32746,10 +32739,10 @@
         <v>509</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
         <v>503</v>
@@ -32766,7 +32759,7 @@
         <v>512</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>513</v>
@@ -32786,7 +32779,7 @@
         <v>516</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>513</v>
@@ -32806,7 +32799,7 @@
         <v>519</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>513</v>
@@ -32826,7 +32819,7 @@
         <v>522</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>513</v>
@@ -32846,7 +32839,7 @@
         <v>525</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>513</v>
@@ -32866,7 +32859,7 @@
         <v>528</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
         <v>513</v>
@@ -32886,7 +32879,7 @@
         <v>531</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>513</v>
@@ -32906,7 +32899,7 @@
         <v>534</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>513</v>
@@ -32926,10 +32919,10 @@
         <v>537</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F14" t="s">
         <v>503</v>
@@ -32946,10 +32939,10 @@
         <v>540</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F15" t="s">
         <v>503</v>
@@ -32966,10 +32959,10 @@
         <v>543</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
         <v>503</v>
@@ -32986,10 +32979,10 @@
         <v>546</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F17" t="s">
         <v>503</v>
@@ -32997,19 +32990,19 @@
     </row>
     <row r="18" customFormat="1" spans="1:6">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F18" t="s">
         <v>503</v>
@@ -33026,10 +33019,10 @@
         <v>549</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F19" t="s">
         <v>503</v>
@@ -33046,10 +33039,10 @@
         <v>552</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F20" t="s">
         <v>503</v>
@@ -33066,10 +33059,10 @@
         <v>555</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F21" t="s">
         <v>503</v>
@@ -33086,10 +33079,10 @@
         <v>558</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F22" t="s">
         <v>503</v>
@@ -33106,10 +33099,10 @@
         <v>561</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F23" t="s">
         <v>503</v>
@@ -33126,10 +33119,10 @@
         <v>564</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
         <v>503</v>
@@ -33146,10 +33139,10 @@
         <v>567</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F25" t="s">
         <v>503</v>
@@ -33157,19 +33150,19 @@
     </row>
     <row r="26" customFormat="1" spans="1:6">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F26" t="s">
         <v>503</v>
@@ -33186,10 +33179,10 @@
         <v>570</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F27" t="s">
         <v>503</v>
@@ -33206,10 +33199,10 @@
         <v>573</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F28" t="s">
         <v>503</v>
@@ -33226,10 +33219,10 @@
         <v>576</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F29" t="s">
         <v>503</v>
@@ -33246,10 +33239,10 @@
         <v>579</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F30" t="s">
         <v>503</v>
@@ -33266,10 +33259,10 @@
         <v>582</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F31" t="s">
         <v>503</v>
@@ -33286,10 +33279,10 @@
         <v>585</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F32" t="s">
         <v>503</v>
@@ -33306,10 +33299,10 @@
         <v>588</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F33" t="s">
         <v>503</v>
@@ -33326,10 +33319,10 @@
         <v>591</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F34" t="s">
         <v>503</v>
@@ -33346,10 +33339,10 @@
         <v>594</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F35" t="s">
         <v>503</v>
@@ -33366,10 +33359,10 @@
         <v>597</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F36" t="s">
         <v>503</v>
@@ -33386,10 +33379,10 @@
         <v>600</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F37" t="s">
         <v>503</v>
@@ -33406,10 +33399,10 @@
         <v>603</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F38" t="s">
         <v>503</v>
@@ -33426,10 +33419,10 @@
         <v>606</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F39" t="s">
         <v>503</v>
@@ -33446,10 +33439,10 @@
         <v>609</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F40" t="s">
         <v>503</v>
@@ -33466,10 +33459,10 @@
         <v>612</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F41" t="s">
         <v>503</v>
@@ -33486,10 +33479,10 @@
         <v>615</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F42" t="s">
         <v>503</v>
@@ -33497,19 +33490,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" t="s">
         <v>110</v>
-      </c>
-      <c r="D43" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" t="s">
-        <v>104</v>
       </c>
       <c r="F43" t="s">
         <v>503</v>
@@ -33526,10 +33519,10 @@
         <v>618</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F44" t="s">
         <v>503</v>
@@ -33546,10 +33539,10 @@
         <v>621</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F45" t="s">
         <v>503</v>
@@ -33566,10 +33559,10 @@
         <v>624</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F46" t="s">
         <v>503</v>
@@ -33586,10 +33579,10 @@
         <v>627</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F47" t="s">
         <v>503</v>
@@ -33606,10 +33599,10 @@
         <v>630</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F48" t="s">
         <v>503</v>
@@ -33626,7 +33619,7 @@
         <v>633</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E49" t="s">
         <v>634</v>
@@ -33646,7 +33639,7 @@
         <v>637</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E50" t="s">
         <v>634</v>
@@ -33666,7 +33659,7 @@
         <v>640</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E51" t="s">
         <v>634</v>
@@ -33686,7 +33679,7 @@
         <v>643</v>
       </c>
       <c r="D52" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E52" t="s">
         <v>634</v>
@@ -33706,7 +33699,7 @@
         <v>646</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
         <v>634</v>
@@ -33726,7 +33719,7 @@
         <v>649</v>
       </c>
       <c r="D54" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E54" t="s">
         <v>634</v>
@@ -33746,7 +33739,7 @@
         <v>652</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E55" t="s">
         <v>634</v>
@@ -33766,7 +33759,7 @@
         <v>655</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E56" t="s">
         <v>634</v>
@@ -33786,7 +33779,7 @@
         <v>658</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E57" t="s">
         <v>634</v>
@@ -33806,7 +33799,7 @@
         <v>661</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E58" t="s">
         <v>634</v>
@@ -33826,7 +33819,7 @@
         <v>664</v>
       </c>
       <c r="D59" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E59" t="s">
         <v>634</v>
@@ -33846,7 +33839,7 @@
         <v>667</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E60" t="s">
         <v>634</v>
@@ -33866,7 +33859,7 @@
         <v>670</v>
       </c>
       <c r="D61" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E61" t="s">
         <v>634</v>
@@ -33886,7 +33879,7 @@
         <v>673</v>
       </c>
       <c r="D62" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E62" t="s">
         <v>634</v>
@@ -33906,7 +33899,7 @@
         <v>676</v>
       </c>
       <c r="D63" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E63" t="s">
         <v>634</v>
@@ -33926,7 +33919,7 @@
         <v>679</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E64" t="s">
         <v>634</v>
@@ -33946,7 +33939,7 @@
         <v>682</v>
       </c>
       <c r="D65" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E65" t="s">
         <v>634</v>
@@ -33966,7 +33959,7 @@
         <v>685</v>
       </c>
       <c r="D66" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E66" t="s">
         <v>634</v>
@@ -33986,7 +33979,7 @@
         <v>688</v>
       </c>
       <c r="D67" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E67" t="s">
         <v>634</v>
@@ -34006,7 +33999,7 @@
         <v>691</v>
       </c>
       <c r="D68" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E68" t="s">
         <v>634</v>
@@ -34026,7 +34019,7 @@
         <v>694</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E69" t="s">
         <v>695</v>
@@ -34046,7 +34039,7 @@
         <v>698</v>
       </c>
       <c r="D70" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E70" t="s">
         <v>695</v>
@@ -34066,7 +34059,7 @@
         <v>701</v>
       </c>
       <c r="D71" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E71" t="s">
         <v>695</v>
@@ -34086,7 +34079,7 @@
         <v>704</v>
       </c>
       <c r="D72" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E72" t="s">
         <v>695</v>
@@ -34106,7 +34099,7 @@
         <v>707</v>
       </c>
       <c r="D73" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E73" t="s">
         <v>695</v>
@@ -34126,7 +34119,7 @@
         <v>710</v>
       </c>
       <c r="D74" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E74" t="s">
         <v>695</v>
@@ -34146,7 +34139,7 @@
         <v>713</v>
       </c>
       <c r="D75" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E75" t="s">
         <v>695</v>
@@ -34166,7 +34159,7 @@
         <v>716</v>
       </c>
       <c r="D76" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E76" t="s">
         <v>695</v>
@@ -34186,7 +34179,7 @@
         <v>719</v>
       </c>
       <c r="D77" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E77" t="s">
         <v>634</v>
@@ -34206,7 +34199,7 @@
         <v>722</v>
       </c>
       <c r="D78" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E78" t="s">
         <v>634</v>
@@ -34226,7 +34219,7 @@
         <v>725</v>
       </c>
       <c r="D79" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E79" t="s">
         <v>634</v>
@@ -34246,7 +34239,7 @@
         <v>728</v>
       </c>
       <c r="D80" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E80" t="s">
         <v>634</v>
@@ -34266,7 +34259,7 @@
         <v>731</v>
       </c>
       <c r="D81" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E81" t="s">
         <v>634</v>
@@ -34286,7 +34279,7 @@
         <v>734</v>
       </c>
       <c r="D82" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E82" t="s">
         <v>634</v>
@@ -34306,7 +34299,7 @@
         <v>737</v>
       </c>
       <c r="D83" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E83" t="s">
         <v>634</v>
@@ -34326,7 +34319,7 @@
         <v>740</v>
       </c>
       <c r="D84" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E84" t="s">
         <v>634</v>
@@ -34346,7 +34339,7 @@
         <v>743</v>
       </c>
       <c r="D85" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E85" t="s">
         <v>634</v>
@@ -34366,7 +34359,7 @@
         <v>746</v>
       </c>
       <c r="D86" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E86" t="s">
         <v>634</v>
@@ -34386,7 +34379,7 @@
         <v>749</v>
       </c>
       <c r="D87" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E87" t="s">
         <v>634</v>
@@ -34406,7 +34399,7 @@
         <v>752</v>
       </c>
       <c r="D88" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E88" t="s">
         <v>634</v>
@@ -34426,7 +34419,7 @@
         <v>755</v>
       </c>
       <c r="D89" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E89" t="s">
         <v>634</v>
@@ -34446,7 +34439,7 @@
         <v>758</v>
       </c>
       <c r="D90" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E90" t="s">
         <v>634</v>
@@ -34466,7 +34459,7 @@
         <v>761</v>
       </c>
       <c r="D91" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E91" t="s">
         <v>634</v>
@@ -34486,7 +34479,7 @@
         <v>764</v>
       </c>
       <c r="D92" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E92" t="s">
         <v>634</v>
@@ -34566,7 +34559,7 @@
         <v>777</v>
       </c>
       <c r="D96" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E96" t="s">
         <v>634</v>
@@ -34586,7 +34579,7 @@
         <v>780</v>
       </c>
       <c r="D97" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E97" t="s">
         <v>634</v>
@@ -34606,7 +34599,7 @@
         <v>783</v>
       </c>
       <c r="D98" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E98" t="s">
         <v>634</v>
@@ -34626,7 +34619,7 @@
         <v>786</v>
       </c>
       <c r="D99" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E99" t="s">
         <v>634</v>
@@ -34646,7 +34639,7 @@
         <v>789</v>
       </c>
       <c r="D100" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E100" t="s">
         <v>634</v>
@@ -34746,7 +34739,7 @@
         <v>805</v>
       </c>
       <c r="D105" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E105" t="s">
         <v>634</v>
@@ -34766,7 +34759,7 @@
         <v>808</v>
       </c>
       <c r="D106" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E106" t="s">
         <v>634</v>
@@ -34786,7 +34779,7 @@
         <v>811</v>
       </c>
       <c r="D107" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E107" t="s">
         <v>634</v>
@@ -34806,7 +34799,7 @@
         <v>814</v>
       </c>
       <c r="D108" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E108" t="s">
         <v>634</v>
@@ -34826,7 +34819,7 @@
         <v>817</v>
       </c>
       <c r="D109" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E109" t="s">
         <v>634</v>
@@ -34846,7 +34839,7 @@
         <v>820</v>
       </c>
       <c r="D110" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E110" t="s">
         <v>634</v>
@@ -34866,7 +34859,7 @@
         <v>823</v>
       </c>
       <c r="D111" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E111" t="s">
         <v>634</v>
@@ -34886,7 +34879,7 @@
         <v>826</v>
       </c>
       <c r="D112" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E112" t="s">
         <v>634</v>
@@ -34906,10 +34899,10 @@
         <v>829</v>
       </c>
       <c r="D113" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E113" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F113" t="s">
         <v>503</v>
@@ -34926,10 +34919,10 @@
         <v>832</v>
       </c>
       <c r="D114" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E114" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F114" t="s">
         <v>503</v>
@@ -34946,10 +34939,10 @@
         <v>835</v>
       </c>
       <c r="D115" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E115" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F115" t="s">
         <v>503</v>
@@ -34966,10 +34959,10 @@
         <v>838</v>
       </c>
       <c r="D116" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E116" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F116" t="s">
         <v>503</v>
@@ -34977,19 +34970,19 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C117" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D117" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E117" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F117" t="s">
         <v>503</v>
@@ -35006,10 +34999,10 @@
         <v>841</v>
       </c>
       <c r="D118" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E118" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F118" t="s">
         <v>503</v>
@@ -35026,10 +35019,10 @@
         <v>844</v>
       </c>
       <c r="D119" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E119" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F119" t="s">
         <v>503</v>
@@ -35046,10 +35039,10 @@
         <v>847</v>
       </c>
       <c r="D120" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E120" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F120" t="s">
         <v>503</v>
@@ -35100,7 +35093,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:6">
@@ -35134,10 +35127,10 @@
         <v>856</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F3" t="s">
         <v>853</v>
@@ -35154,10 +35147,10 @@
         <v>859</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
         <v>853</v>
@@ -35174,10 +35167,10 @@
         <v>862</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
         <v>853</v>
@@ -35194,10 +35187,10 @@
         <v>865</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
         <v>853</v>
@@ -35214,10 +35207,10 @@
         <v>868</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F7" t="s">
         <v>853</v>
@@ -35225,19 +35218,19 @@
     </row>
     <row r="8" customFormat="1" spans="1:6">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F8" t="s">
         <v>853</v>
@@ -35254,10 +35247,10 @@
         <v>871</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s">
         <v>853</v>
@@ -35265,19 +35258,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
         <v>853</v>
@@ -35294,10 +35287,10 @@
         <v>874</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F11" t="s">
         <v>853</v>
@@ -35314,7 +35307,7 @@
         <v>877</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E12" t="s">
         <v>878</v>
@@ -35334,7 +35327,7 @@
         <v>881</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E13" t="s">
         <v>878</v>
@@ -35354,7 +35347,7 @@
         <v>884</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
         <v>878</v>
@@ -35374,7 +35367,7 @@
         <v>887</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E15" t="s">
         <v>878</v>
@@ -35394,7 +35387,7 @@
         <v>890</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
         <v>878</v>
@@ -35414,7 +35407,7 @@
         <v>893</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
         <v>878</v>
@@ -35434,7 +35427,7 @@
         <v>896</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E18" t="s">
         <v>878</v>
@@ -35454,7 +35447,7 @@
         <v>899</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E19" t="s">
         <v>878</v>
@@ -35474,7 +35467,7 @@
         <v>902</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E20" t="s">
         <v>878</v>
@@ -35494,7 +35487,7 @@
         <v>905</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E21" t="s">
         <v>906</v>
@@ -35514,7 +35507,7 @@
         <v>909</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E22" t="s">
         <v>906</v>
@@ -35534,7 +35527,7 @@
         <v>912</v>
       </c>
       <c r="D23" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E23" t="s">
         <v>906</v>
@@ -35554,7 +35547,7 @@
         <v>915</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E24" t="s">
         <v>906</v>
@@ -35574,7 +35567,7 @@
         <v>918</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E25" t="s">
         <v>906</v>
@@ -35594,7 +35587,7 @@
         <v>921</v>
       </c>
       <c r="D26" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E26" t="s">
         <v>906</v>
@@ -35614,7 +35607,7 @@
         <v>924</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E27" t="s">
         <v>906</v>
@@ -35634,7 +35627,7 @@
         <v>927</v>
       </c>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E28" t="s">
         <v>906</v>
@@ -35654,7 +35647,7 @@
         <v>930</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E29" t="s">
         <v>906</v>
@@ -35694,7 +35687,7 @@
         <v>936</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E31" t="s">
         <v>933</v>
@@ -35714,7 +35707,7 @@
         <v>939</v>
       </c>
       <c r="D32" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E32" t="s">
         <v>940</v>
@@ -35734,7 +35727,7 @@
         <v>943</v>
       </c>
       <c r="D33" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E33" t="s">
         <v>940</v>
@@ -35754,7 +35747,7 @@
         <v>946</v>
       </c>
       <c r="D34" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E34" t="s">
         <v>940</v>
@@ -35774,7 +35767,7 @@
         <v>949</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E35" t="s">
         <v>940</v>
@@ -35794,7 +35787,7 @@
         <v>952</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E36" t="s">
         <v>940</v>
@@ -35814,7 +35807,7 @@
         <v>955</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E37" t="s">
         <v>940</v>
@@ -35834,7 +35827,7 @@
         <v>958</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
         <v>940</v>
@@ -35854,7 +35847,7 @@
         <v>961</v>
       </c>
       <c r="D39" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E39" t="s">
         <v>940</v>
@@ -35874,7 +35867,7 @@
         <v>964</v>
       </c>
       <c r="D40" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
         <v>940</v>
@@ -35894,7 +35887,7 @@
         <v>967</v>
       </c>
       <c r="D41" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E41" t="s">
         <v>940</v>
@@ -35914,7 +35907,7 @@
         <v>970</v>
       </c>
       <c r="D42" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E42" t="s">
         <v>940</v>
@@ -35967,7 +35960,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -36261,7 +36254,7 @@
         <v>1017</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
         <v>1018</v>
@@ -36281,7 +36274,7 @@
         <v>1021</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
         <v>1018</v>
@@ -36301,7 +36294,7 @@
         <v>1024</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
         <v>1018</v>
@@ -36321,7 +36314,7 @@
         <v>1027</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>1018</v>
@@ -36341,7 +36334,7 @@
         <v>1030</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
         <v>1018</v>
@@ -36361,7 +36354,7 @@
         <v>1033</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
         <v>1018</v>
@@ -36381,7 +36374,7 @@
         <v>1036</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
         <v>1018</v>
@@ -36401,7 +36394,7 @@
         <v>1039</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
         <v>1040</v>
@@ -36421,7 +36414,7 @@
         <v>1043</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>1040</v>
@@ -36441,7 +36434,7 @@
         <v>1046</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
         <v>1040</v>
@@ -36461,7 +36454,7 @@
         <v>1049</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
         <v>1040</v>
@@ -36481,7 +36474,7 @@
         <v>1052</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>1040</v>
@@ -36501,7 +36494,7 @@
         <v>1055</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
         <v>1040</v>
@@ -36521,7 +36514,7 @@
         <v>1058</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
         <v>1040</v>
@@ -36541,7 +36534,7 @@
         <v>1061</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>1040</v>
@@ -36561,7 +36554,7 @@
         <v>1064</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
         <v>1040</v>

</xml_diff>

<commit_message>
Add 11.1. Management Dashboard
</commit_message>
<xml_diff>
--- a/apps/core/fixtures/core_permission.xlsx
+++ b/apps/core/fixtures/core_permission.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16260" tabRatio="894" firstSheet="15" activeTab="19"/>
+    <workbookView windowHeight="16260" tabRatio="894" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="core_permission" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="1882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="1885">
   <si>
     <t>code</t>
   </si>
@@ -4211,9 +4211,6 @@
     <t>Quyền tạo mới một Quyết Định</t>
   </si>
   <si>
-    <t>S_NHANVIEN_CHUNG</t>
-  </si>
-  <si>
     <t>decision.destroy</t>
   </si>
   <si>
@@ -4266,6 +4263,18 @@
   </si>
   <si>
     <t>Quyền cập nhật Quyết Định</t>
+  </si>
+  <si>
+    <t>hrm.dashboard.common.realtime</t>
+  </si>
+  <si>
+    <t>[HCNS] [HRM Dashboard] View Common HRM realtime dashboard</t>
+  </si>
+  <si>
+    <t>View HRM stats for handling proposals, attendance, and penalties</t>
+  </si>
+  <si>
+    <t>HRM Dashboard</t>
   </si>
   <si>
     <t>proposal.mine</t>
@@ -7095,8 +7104,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="S_HRM_CHUNG" displayName="S_HRM_CHUNG" ref="A1:F36" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F36" etc:filterBottomFollowUsedRange="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="S_HRM_CHUNG" displayName="S_HRM_CHUNG" ref="A1:F37" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F37" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="6">
     <tableColumn id="1" name="code" dataDxfId="54"/>
     <tableColumn id="2" name="Tên" dataDxfId="55"/>
@@ -8095,10 +8104,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="A21:F21"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -8667,18 +8676,18 @@
         <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B29" t="s">
         <v>1375</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>1376</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1377</v>
       </c>
       <c r="D29" t="s">
         <v>77</v>
@@ -8687,18 +8696,18 @@
         <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B30" t="s">
         <v>1378</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>1379</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1380</v>
       </c>
       <c r="D30" t="s">
         <v>77</v>
@@ -8707,18 +8716,18 @@
         <v>78</v>
       </c>
       <c r="F30" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B31" t="s">
         <v>1381</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>1382</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1383</v>
       </c>
       <c r="D31" t="s">
         <v>77</v>
@@ -8727,18 +8736,18 @@
         <v>78</v>
       </c>
       <c r="F31" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B32" t="s">
         <v>1384</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>1385</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1386</v>
       </c>
       <c r="D32" t="s">
         <v>77</v>
@@ -8747,7 +8756,7 @@
         <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -8767,18 +8776,18 @@
         <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B34" t="s">
         <v>1387</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>1388</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1389</v>
       </c>
       <c r="D34" t="s">
         <v>77</v>
@@ -8787,7 +8796,7 @@
         <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -8807,18 +8816,18 @@
         <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>1374</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B36" t="s">
         <v>1390</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>1391</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1392</v>
       </c>
       <c r="D36" t="s">
         <v>77</v>
@@ -8827,7 +8836,27 @@
         <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>1374</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F37" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -8881,13 +8910,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>1393</v>
+        <v>1396</v>
       </c>
       <c r="B2" t="s">
-        <v>1394</v>
+        <v>1397</v>
       </c>
       <c r="C2" t="s">
-        <v>1395</v>
+        <v>1398</v>
       </c>
       <c r="D2" t="s">
         <v>145</v>
@@ -8896,7 +8925,7 @@
         <v>170</v>
       </c>
       <c r="F2" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -8916,7 +8945,7 @@
         <v>208</v>
       </c>
       <c r="F3" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -8936,7 +8965,7 @@
         <v>208</v>
       </c>
       <c r="F4" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8956,7 +8985,7 @@
         <v>208</v>
       </c>
       <c r="F5" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8976,7 +9005,7 @@
         <v>208</v>
       </c>
       <c r="F6" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8996,7 +9025,7 @@
         <v>208</v>
       </c>
       <c r="F7" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -9016,7 +9045,7 @@
         <v>208</v>
       </c>
       <c r="F8" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -9036,7 +9065,7 @@
         <v>208</v>
       </c>
       <c r="F9" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -9056,18 +9085,18 @@
         <v>208</v>
       </c>
       <c r="F10" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1397</v>
+        <v>1400</v>
       </c>
       <c r="B11" t="s">
-        <v>1398</v>
+        <v>1401</v>
       </c>
       <c r="C11" t="s">
-        <v>1399</v>
+        <v>1402</v>
       </c>
       <c r="D11" t="s">
         <v>145</v>
@@ -9076,18 +9105,18 @@
         <v>170</v>
       </c>
       <c r="F11" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1400</v>
+        <v>1403</v>
       </c>
       <c r="B12" t="s">
-        <v>1401</v>
+        <v>1404</v>
       </c>
       <c r="C12" t="s">
-        <v>1402</v>
+        <v>1405</v>
       </c>
       <c r="D12" t="s">
         <v>145</v>
@@ -9096,18 +9125,18 @@
         <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1403</v>
+        <v>1406</v>
       </c>
       <c r="B13" t="s">
-        <v>1404</v>
+        <v>1407</v>
       </c>
       <c r="C13" t="s">
-        <v>1405</v>
+        <v>1408</v>
       </c>
       <c r="D13" t="s">
         <v>145</v>
@@ -9116,18 +9145,18 @@
         <v>170</v>
       </c>
       <c r="F13" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>1406</v>
+        <v>1409</v>
       </c>
       <c r="B14" t="s">
-        <v>1407</v>
+        <v>1410</v>
       </c>
       <c r="C14" t="s">
-        <v>1408</v>
+        <v>1411</v>
       </c>
       <c r="D14" t="s">
         <v>145</v>
@@ -9136,18 +9165,18 @@
         <v>170</v>
       </c>
       <c r="F14" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>1409</v>
+        <v>1412</v>
       </c>
       <c r="B15" t="s">
-        <v>1410</v>
+        <v>1413</v>
       </c>
       <c r="C15" t="s">
-        <v>1411</v>
+        <v>1414</v>
       </c>
       <c r="D15" t="s">
         <v>145</v>
@@ -9156,18 +9185,18 @@
         <v>170</v>
       </c>
       <c r="F15" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1412</v>
+        <v>1415</v>
       </c>
       <c r="B16" t="s">
-        <v>1413</v>
+        <v>1416</v>
       </c>
       <c r="C16" t="s">
-        <v>1414</v>
+        <v>1417</v>
       </c>
       <c r="D16" t="s">
         <v>145</v>
@@ -9176,18 +9205,18 @@
         <v>170</v>
       </c>
       <c r="F16" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1415</v>
+        <v>1418</v>
       </c>
       <c r="B17" t="s">
-        <v>1416</v>
+        <v>1419</v>
       </c>
       <c r="C17" t="s">
-        <v>1417</v>
+        <v>1420</v>
       </c>
       <c r="D17" t="s">
         <v>145</v>
@@ -9196,18 +9225,18 @@
         <v>170</v>
       </c>
       <c r="F17" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1418</v>
+        <v>1421</v>
       </c>
       <c r="B18" t="s">
-        <v>1419</v>
+        <v>1422</v>
       </c>
       <c r="C18" t="s">
-        <v>1420</v>
+        <v>1423</v>
       </c>
       <c r="D18" t="s">
         <v>145</v>
@@ -9216,18 +9245,18 @@
         <v>170</v>
       </c>
       <c r="F18" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1421</v>
+        <v>1424</v>
       </c>
       <c r="B19" t="s">
-        <v>1422</v>
+        <v>1425</v>
       </c>
       <c r="C19" t="s">
-        <v>1423</v>
+        <v>1426</v>
       </c>
       <c r="D19" t="s">
         <v>145</v>
@@ -9236,7 +9265,7 @@
         <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -9256,18 +9285,18 @@
         <v>208</v>
       </c>
       <c r="F20" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>1424</v>
+        <v>1427</v>
       </c>
       <c r="B21" t="s">
-        <v>1425</v>
+        <v>1428</v>
       </c>
       <c r="C21" t="s">
-        <v>1426</v>
+        <v>1429</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
@@ -9276,18 +9305,18 @@
         <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>1427</v>
+        <v>1430</v>
       </c>
       <c r="B22" t="s">
-        <v>1428</v>
+        <v>1431</v>
       </c>
       <c r="C22" t="s">
-        <v>1429</v>
+        <v>1432</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -9296,18 +9325,18 @@
         <v>29</v>
       </c>
       <c r="F22" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1430</v>
+        <v>1433</v>
       </c>
       <c r="B23" t="s">
-        <v>1431</v>
+        <v>1434</v>
       </c>
       <c r="C23" t="s">
-        <v>1432</v>
+        <v>1435</v>
       </c>
       <c r="D23" t="s">
         <v>28</v>
@@ -9316,18 +9345,18 @@
         <v>29</v>
       </c>
       <c r="F23" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>1433</v>
+        <v>1436</v>
       </c>
       <c r="B24" t="s">
-        <v>1434</v>
+        <v>1437</v>
       </c>
       <c r="C24" t="s">
-        <v>1435</v>
+        <v>1438</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -9336,18 +9365,18 @@
         <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>1436</v>
+        <v>1439</v>
       </c>
       <c r="B25" t="s">
-        <v>1437</v>
+        <v>1440</v>
       </c>
       <c r="C25" t="s">
-        <v>1438</v>
+        <v>1441</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -9356,18 +9385,18 @@
         <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>1439</v>
+        <v>1442</v>
       </c>
       <c r="B26" t="s">
-        <v>1440</v>
+        <v>1443</v>
       </c>
       <c r="C26" t="s">
-        <v>1441</v>
+        <v>1444</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -9376,18 +9405,18 @@
         <v>29</v>
       </c>
       <c r="F26" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>1442</v>
+        <v>1445</v>
       </c>
       <c r="B27" t="s">
-        <v>1443</v>
+        <v>1446</v>
       </c>
       <c r="C27" t="s">
-        <v>1444</v>
+        <v>1447</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
@@ -9396,18 +9425,18 @@
         <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>1445</v>
+        <v>1448</v>
       </c>
       <c r="B28" t="s">
-        <v>1446</v>
+        <v>1449</v>
       </c>
       <c r="C28" t="s">
-        <v>1447</v>
+        <v>1450</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -9416,27 +9445,27 @@
         <v>29</v>
       </c>
       <c r="F28" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1448</v>
+        <v>1451</v>
       </c>
       <c r="B29" t="s">
-        <v>1449</v>
+        <v>1452</v>
       </c>
       <c r="C29" t="s">
-        <v>1450</v>
+        <v>1453</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F29" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -9456,187 +9485,187 @@
         <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>1452</v>
+        <v>1455</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1453</v>
+        <v>1456</v>
       </c>
       <c r="C31" t="s">
-        <v>1454</v>
+        <v>1457</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F31" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>1455</v>
+        <v>1458</v>
       </c>
       <c r="B32" t="s">
-        <v>1456</v>
+        <v>1459</v>
       </c>
       <c r="C32" t="s">
-        <v>1457</v>
+        <v>1460</v>
       </c>
       <c r="D32" t="s">
         <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F32" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>1458</v>
+        <v>1461</v>
       </c>
       <c r="B33" t="s">
-        <v>1459</v>
+        <v>1462</v>
       </c>
       <c r="C33" t="s">
-        <v>1460</v>
+        <v>1463</v>
       </c>
       <c r="D33" t="s">
         <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F33" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>1455</v>
+        <v>1458</v>
       </c>
       <c r="B34" t="s">
-        <v>1456</v>
+        <v>1459</v>
       </c>
       <c r="C34" t="s">
-        <v>1457</v>
+        <v>1460</v>
       </c>
       <c r="D34" t="s">
         <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F34" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>1461</v>
+        <v>1464</v>
       </c>
       <c r="B35" t="s">
-        <v>1462</v>
+        <v>1465</v>
       </c>
       <c r="C35" t="s">
-        <v>1463</v>
+        <v>1466</v>
       </c>
       <c r="D35" t="s">
         <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F35" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>1464</v>
+        <v>1467</v>
       </c>
       <c r="B36" t="s">
-        <v>1465</v>
+        <v>1468</v>
       </c>
       <c r="C36" t="s">
-        <v>1466</v>
+        <v>1469</v>
       </c>
       <c r="D36" t="s">
         <v>28</v>
       </c>
       <c r="E36" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F36" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>1448</v>
+        <v>1451</v>
       </c>
       <c r="B37" t="s">
-        <v>1449</v>
+        <v>1452</v>
       </c>
       <c r="C37" t="s">
-        <v>1450</v>
+        <v>1453</v>
       </c>
       <c r="D37" t="s">
         <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F37" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>1452</v>
+        <v>1455</v>
       </c>
       <c r="B38" t="s">
-        <v>1453</v>
+        <v>1456</v>
       </c>
       <c r="C38" t="s">
-        <v>1454</v>
+        <v>1457</v>
       </c>
       <c r="D38" t="s">
         <v>28</v>
       </c>
       <c r="E38" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F38" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>1467</v>
+        <v>1470</v>
       </c>
       <c r="B39" t="s">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="C39" t="s">
-        <v>1469</v>
+        <v>1472</v>
       </c>
       <c r="D39" t="s">
         <v>28</v>
       </c>
       <c r="E39" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="F39" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
     </row>
   </sheetData>
@@ -9689,13 +9718,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>1470</v>
+        <v>1473</v>
       </c>
       <c r="B2" t="s">
-        <v>1471</v>
+        <v>1474</v>
       </c>
       <c r="C2" t="s">
-        <v>1472</v>
+        <v>1475</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -9704,18 +9733,18 @@
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>1474</v>
+        <v>1477</v>
       </c>
       <c r="B3" t="s">
-        <v>1475</v>
+        <v>1478</v>
       </c>
       <c r="C3" t="s">
-        <v>1476</v>
+        <v>1479</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -9724,18 +9753,18 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>1430</v>
+        <v>1433</v>
       </c>
       <c r="B4" t="s">
-        <v>1431</v>
+        <v>1434</v>
       </c>
       <c r="C4" t="s">
-        <v>1432</v>
+        <v>1435</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
@@ -9744,18 +9773,18 @@
         <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>1433</v>
+        <v>1436</v>
       </c>
       <c r="B5" t="s">
-        <v>1434</v>
+        <v>1437</v>
       </c>
       <c r="C5" t="s">
-        <v>1435</v>
+        <v>1438</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
@@ -9764,18 +9793,18 @@
         <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>1436</v>
+        <v>1439</v>
       </c>
       <c r="B6" t="s">
-        <v>1437</v>
+        <v>1440</v>
       </c>
       <c r="C6" t="s">
-        <v>1438</v>
+        <v>1441</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -9784,18 +9813,18 @@
         <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>1439</v>
+        <v>1442</v>
       </c>
       <c r="B7" t="s">
-        <v>1440</v>
+        <v>1443</v>
       </c>
       <c r="C7" t="s">
-        <v>1441</v>
+        <v>1444</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
@@ -9804,18 +9833,18 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>1442</v>
+        <v>1445</v>
       </c>
       <c r="B8" t="s">
-        <v>1443</v>
+        <v>1446</v>
       </c>
       <c r="C8" t="s">
-        <v>1444</v>
+        <v>1447</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -9824,18 +9853,18 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>1445</v>
+        <v>1448</v>
       </c>
       <c r="B9" t="s">
-        <v>1446</v>
+        <v>1449</v>
       </c>
       <c r="C9" t="s">
-        <v>1447</v>
+        <v>1450</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
@@ -9844,18 +9873,18 @@
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
       <c r="B10" t="s">
-        <v>1478</v>
+        <v>1481</v>
       </c>
       <c r="C10" t="s">
-        <v>1479</v>
+        <v>1482</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
@@ -9864,18 +9893,18 @@
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1480</v>
+        <v>1483</v>
       </c>
       <c r="B11" t="s">
-        <v>1481</v>
+        <v>1484</v>
       </c>
       <c r="C11" t="s">
-        <v>1482</v>
+        <v>1485</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
@@ -9884,18 +9913,18 @@
         <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1483</v>
+        <v>1486</v>
       </c>
       <c r="B12" t="s">
-        <v>1484</v>
+        <v>1487</v>
       </c>
       <c r="C12" t="s">
-        <v>1485</v>
+        <v>1488</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
@@ -9904,18 +9933,18 @@
         <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1486</v>
+        <v>1489</v>
       </c>
       <c r="B13" t="s">
-        <v>1487</v>
+        <v>1490</v>
       </c>
       <c r="C13" t="s">
-        <v>1488</v>
+        <v>1491</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -9924,18 +9953,18 @@
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>1424</v>
+        <v>1427</v>
       </c>
       <c r="B14" t="s">
-        <v>1425</v>
+        <v>1428</v>
       </c>
       <c r="C14" t="s">
-        <v>1426</v>
+        <v>1429</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
@@ -9944,18 +9973,18 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>1427</v>
+        <v>1430</v>
       </c>
       <c r="B15" t="s">
-        <v>1428</v>
+        <v>1431</v>
       </c>
       <c r="C15" t="s">
-        <v>1429</v>
+        <v>1432</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -9964,198 +9993,198 @@
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1489</v>
+        <v>1492</v>
       </c>
       <c r="B16" t="s">
-        <v>1490</v>
+        <v>1493</v>
       </c>
       <c r="C16" t="s">
-        <v>1491</v>
+        <v>1494</v>
       </c>
       <c r="D16" t="s">
         <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F16" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1493</v>
+        <v>1496</v>
       </c>
       <c r="B17" t="s">
-        <v>1494</v>
+        <v>1497</v>
       </c>
       <c r="C17" t="s">
-        <v>1495</v>
+        <v>1498</v>
       </c>
       <c r="D17" t="s">
         <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F17" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1496</v>
+        <v>1499</v>
       </c>
       <c r="B18" t="s">
-        <v>1497</v>
+        <v>1500</v>
       </c>
       <c r="C18" t="s">
-        <v>1498</v>
+        <v>1501</v>
       </c>
       <c r="D18" t="s">
         <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F18" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1499</v>
+        <v>1502</v>
       </c>
       <c r="B19" t="s">
-        <v>1500</v>
+        <v>1503</v>
       </c>
       <c r="C19" t="s">
-        <v>1501</v>
+        <v>1504</v>
       </c>
       <c r="D19" t="s">
         <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F19" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>1502</v>
+        <v>1505</v>
       </c>
       <c r="B20" t="s">
-        <v>1503</v>
+        <v>1506</v>
       </c>
       <c r="C20" t="s">
-        <v>1504</v>
+        <v>1507</v>
       </c>
       <c r="D20" t="s">
         <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F20" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>1505</v>
+        <v>1508</v>
       </c>
       <c r="B21" t="s">
-        <v>1506</v>
+        <v>1509</v>
       </c>
       <c r="C21" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
       <c r="D21" t="s">
         <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F21" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>1508</v>
+        <v>1511</v>
       </c>
       <c r="B22" t="s">
-        <v>1509</v>
+        <v>1512</v>
       </c>
       <c r="C22" t="s">
-        <v>1510</v>
+        <v>1513</v>
       </c>
       <c r="D22" t="s">
         <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F22" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1511</v>
+        <v>1514</v>
       </c>
       <c r="B23" t="s">
-        <v>1512</v>
+        <v>1515</v>
       </c>
       <c r="C23" t="s">
-        <v>1513</v>
+        <v>1516</v>
       </c>
       <c r="D23" t="s">
         <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F23" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>1514</v>
+        <v>1517</v>
       </c>
       <c r="B24" t="s">
-        <v>1515</v>
+        <v>1518</v>
       </c>
       <c r="C24" t="s">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="D24" t="s">
         <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="F24" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>1517</v>
+        <v>1520</v>
       </c>
       <c r="B25" t="s">
-        <v>1518</v>
+        <v>1521</v>
       </c>
       <c r="C25" t="s">
-        <v>1519</v>
+        <v>1522</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -10164,18 +10193,18 @@
         <v>1048</v>
       </c>
       <c r="F25" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>1520</v>
+        <v>1523</v>
       </c>
       <c r="B26" t="s">
-        <v>1521</v>
+        <v>1524</v>
       </c>
       <c r="C26" t="s">
-        <v>1522</v>
+        <v>1525</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -10184,12 +10213,12 @@
         <v>1048</v>
       </c>
       <c r="F26" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>1523</v>
+        <v>1526</v>
       </c>
       <c r="B27" t="s">
         <v>1046</v>
@@ -10204,12 +10233,12 @@
         <v>1048</v>
       </c>
       <c r="F27" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>1524</v>
+        <v>1527</v>
       </c>
       <c r="B28" t="s">
         <v>1050</v>
@@ -10224,18 +10253,18 @@
         <v>1048</v>
       </c>
       <c r="F28" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="B29" t="s">
-        <v>1526</v>
+        <v>1529</v>
       </c>
       <c r="C29" t="s">
-        <v>1527</v>
+        <v>1530</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
@@ -10244,18 +10273,18 @@
         <v>1048</v>
       </c>
       <c r="F29" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
       <c r="B30" t="s">
-        <v>1529</v>
+        <v>1532</v>
       </c>
       <c r="C30" t="s">
-        <v>1530</v>
+        <v>1533</v>
       </c>
       <c r="D30" t="s">
         <v>28</v>
@@ -10264,18 +10293,18 @@
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>1531</v>
+        <v>1534</v>
       </c>
       <c r="B31" t="s">
-        <v>1532</v>
+        <v>1535</v>
       </c>
       <c r="C31" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -10284,18 +10313,18 @@
         <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>1534</v>
+        <v>1537</v>
       </c>
       <c r="B32" t="s">
-        <v>1535</v>
+        <v>1538</v>
       </c>
       <c r="C32" t="s">
-        <v>1536</v>
+        <v>1539</v>
       </c>
       <c r="D32" t="s">
         <v>28</v>
@@ -10304,18 +10333,18 @@
         <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>1537</v>
+        <v>1540</v>
       </c>
       <c r="B33" t="s">
-        <v>1538</v>
+        <v>1541</v>
       </c>
       <c r="C33" t="s">
-        <v>1539</v>
+        <v>1542</v>
       </c>
       <c r="D33" t="s">
         <v>28</v>
@@ -10324,18 +10353,18 @@
         <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>1540</v>
+        <v>1543</v>
       </c>
       <c r="B34" t="s">
-        <v>1541</v>
+        <v>1544</v>
       </c>
       <c r="C34" t="s">
-        <v>1542</v>
+        <v>1545</v>
       </c>
       <c r="D34" t="s">
         <v>28</v>
@@ -10344,18 +10373,18 @@
         <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>1543</v>
+        <v>1546</v>
       </c>
       <c r="B35" t="s">
-        <v>1544</v>
+        <v>1547</v>
       </c>
       <c r="C35" t="s">
-        <v>1545</v>
+        <v>1548</v>
       </c>
       <c r="D35" t="s">
         <v>28</v>
@@ -10364,18 +10393,18 @@
         <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>1546</v>
+        <v>1549</v>
       </c>
       <c r="B36" t="s">
-        <v>1547</v>
+        <v>1550</v>
       </c>
       <c r="C36" t="s">
-        <v>1548</v>
+        <v>1551</v>
       </c>
       <c r="D36" t="s">
         <v>28</v>
@@ -10384,18 +10413,18 @@
         <v>29</v>
       </c>
       <c r="F36" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>1549</v>
+        <v>1552</v>
       </c>
       <c r="B37" t="s">
-        <v>1550</v>
+        <v>1553</v>
       </c>
       <c r="C37" t="s">
-        <v>1551</v>
+        <v>1554</v>
       </c>
       <c r="D37" t="s">
         <v>28</v>
@@ -10455,13 +10484,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>1552</v>
+        <v>1555</v>
       </c>
       <c r="B2" t="s">
-        <v>1553</v>
+        <v>1556</v>
       </c>
       <c r="C2" t="s">
-        <v>1554</v>
+        <v>1557</v>
       </c>
       <c r="D2" t="s">
         <v>145</v>
@@ -10470,18 +10499,18 @@
         <v>170</v>
       </c>
       <c r="F2" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>1556</v>
+        <v>1559</v>
       </c>
       <c r="B3" t="s">
-        <v>1557</v>
+        <v>1560</v>
       </c>
       <c r="C3" t="s">
-        <v>1558</v>
+        <v>1561</v>
       </c>
       <c r="D3" t="s">
         <v>145</v>
@@ -10490,18 +10519,18 @@
         <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>1559</v>
+        <v>1562</v>
       </c>
       <c r="B4" t="s">
-        <v>1560</v>
+        <v>1563</v>
       </c>
       <c r="C4" t="s">
-        <v>1561</v>
+        <v>1564</v>
       </c>
       <c r="D4" t="s">
         <v>145</v>
@@ -10510,18 +10539,18 @@
         <v>170</v>
       </c>
       <c r="F4" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>1562</v>
+        <v>1565</v>
       </c>
       <c r="B5" t="s">
-        <v>1563</v>
+        <v>1566</v>
       </c>
       <c r="C5" t="s">
-        <v>1564</v>
+        <v>1567</v>
       </c>
       <c r="D5" t="s">
         <v>145</v>
@@ -10530,18 +10559,18 @@
         <v>170</v>
       </c>
       <c r="F5" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>1565</v>
+        <v>1568</v>
       </c>
       <c r="B6" t="s">
-        <v>1566</v>
+        <v>1569</v>
       </c>
       <c r="C6" t="s">
-        <v>1567</v>
+        <v>1570</v>
       </c>
       <c r="D6" t="s">
         <v>145</v>
@@ -10550,18 +10579,18 @@
         <v>170</v>
       </c>
       <c r="F6" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>1568</v>
+        <v>1571</v>
       </c>
       <c r="B7" t="s">
-        <v>1569</v>
+        <v>1572</v>
       </c>
       <c r="C7" t="s">
-        <v>1570</v>
+        <v>1573</v>
       </c>
       <c r="D7" t="s">
         <v>145</v>
@@ -10570,18 +10599,18 @@
         <v>170</v>
       </c>
       <c r="F7" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>1571</v>
+        <v>1574</v>
       </c>
       <c r="B8" t="s">
-        <v>1572</v>
+        <v>1575</v>
       </c>
       <c r="C8" t="s">
-        <v>1573</v>
+        <v>1576</v>
       </c>
       <c r="D8" t="s">
         <v>145</v>
@@ -10590,23 +10619,23 @@
         <v>170</v>
       </c>
       <c r="F8" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="9" spans="6:6">
       <c r="F9" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1574</v>
+        <v>1577</v>
       </c>
       <c r="B10" t="s">
-        <v>1575</v>
+        <v>1578</v>
       </c>
       <c r="C10" t="s">
-        <v>1576</v>
+        <v>1579</v>
       </c>
       <c r="D10" t="s">
         <v>145</v>
@@ -10615,18 +10644,18 @@
         <v>170</v>
       </c>
       <c r="F10" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1577</v>
+        <v>1580</v>
       </c>
       <c r="B11" t="s">
-        <v>1578</v>
+        <v>1581</v>
       </c>
       <c r="C11" t="s">
-        <v>1579</v>
+        <v>1582</v>
       </c>
       <c r="D11" t="s">
         <v>145</v>
@@ -10635,18 +10664,18 @@
         <v>170</v>
       </c>
       <c r="F11" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1580</v>
+        <v>1583</v>
       </c>
       <c r="B12" t="s">
-        <v>1581</v>
+        <v>1584</v>
       </c>
       <c r="C12" t="s">
-        <v>1582</v>
+        <v>1585</v>
       </c>
       <c r="D12" t="s">
         <v>145</v>
@@ -10655,18 +10684,18 @@
         <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1583</v>
+        <v>1586</v>
       </c>
       <c r="B13" t="s">
-        <v>1584</v>
+        <v>1587</v>
       </c>
       <c r="C13" t="s">
-        <v>1585</v>
+        <v>1588</v>
       </c>
       <c r="D13" t="s">
         <v>145</v>
@@ -10675,18 +10704,18 @@
         <v>170</v>
       </c>
       <c r="F13" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>1586</v>
+        <v>1589</v>
       </c>
       <c r="B14" t="s">
-        <v>1587</v>
+        <v>1590</v>
       </c>
       <c r="C14" t="s">
-        <v>1588</v>
+        <v>1591</v>
       </c>
       <c r="D14" t="s">
         <v>145</v>
@@ -10695,18 +10724,18 @@
         <v>170</v>
       </c>
       <c r="F14" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>1589</v>
+        <v>1592</v>
       </c>
       <c r="B15" t="s">
-        <v>1590</v>
+        <v>1593</v>
       </c>
       <c r="C15" t="s">
-        <v>1591</v>
+        <v>1594</v>
       </c>
       <c r="D15" t="s">
         <v>145</v>
@@ -10715,18 +10744,18 @@
         <v>170</v>
       </c>
       <c r="F15" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1592</v>
+        <v>1595</v>
       </c>
       <c r="B16" t="s">
-        <v>1593</v>
+        <v>1596</v>
       </c>
       <c r="C16" t="s">
-        <v>1594</v>
+        <v>1597</v>
       </c>
       <c r="D16" t="s">
         <v>145</v>
@@ -10735,18 +10764,18 @@
         <v>170</v>
       </c>
       <c r="F16" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1595</v>
+        <v>1598</v>
       </c>
       <c r="B17" t="s">
-        <v>1596</v>
+        <v>1599</v>
       </c>
       <c r="C17" t="s">
-        <v>1597</v>
+        <v>1600</v>
       </c>
       <c r="D17" t="s">
         <v>145</v>
@@ -10755,18 +10784,18 @@
         <v>170</v>
       </c>
       <c r="F17" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1598</v>
+        <v>1601</v>
       </c>
       <c r="B18" t="s">
-        <v>1599</v>
+        <v>1602</v>
       </c>
       <c r="C18" t="s">
-        <v>1600</v>
+        <v>1603</v>
       </c>
       <c r="D18" t="s">
         <v>145</v>
@@ -10775,18 +10804,18 @@
         <v>170</v>
       </c>
       <c r="F18" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="B19" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="C19" t="s">
-        <v>1603</v>
+        <v>1606</v>
       </c>
       <c r="D19" t="s">
         <v>145</v>
@@ -10795,23 +10824,23 @@
         <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="20" spans="6:6">
       <c r="F20" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>1604</v>
+        <v>1607</v>
       </c>
       <c r="B21" t="s">
-        <v>1605</v>
+        <v>1608</v>
       </c>
       <c r="C21" t="s">
-        <v>1606</v>
+        <v>1609</v>
       </c>
       <c r="D21" t="s">
         <v>145</v>
@@ -10820,18 +10849,18 @@
         <v>170</v>
       </c>
       <c r="F21" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>1607</v>
+        <v>1610</v>
       </c>
       <c r="B22" t="s">
-        <v>1608</v>
+        <v>1611</v>
       </c>
       <c r="C22" t="s">
-        <v>1609</v>
+        <v>1612</v>
       </c>
       <c r="D22" t="s">
         <v>145</v>
@@ -10840,18 +10869,18 @@
         <v>170</v>
       </c>
       <c r="F22" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1610</v>
+        <v>1613</v>
       </c>
       <c r="B23" t="s">
-        <v>1611</v>
+        <v>1614</v>
       </c>
       <c r="C23" t="s">
-        <v>1612</v>
+        <v>1615</v>
       </c>
       <c r="D23" t="s">
         <v>145</v>
@@ -10860,18 +10889,18 @@
         <v>170</v>
       </c>
       <c r="F23" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>1613</v>
+        <v>1616</v>
       </c>
       <c r="B24" t="s">
-        <v>1614</v>
+        <v>1617</v>
       </c>
       <c r="C24" t="s">
-        <v>1615</v>
+        <v>1618</v>
       </c>
       <c r="D24" t="s">
         <v>145</v>
@@ -10880,18 +10909,18 @@
         <v>170</v>
       </c>
       <c r="F24" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>1616</v>
+        <v>1619</v>
       </c>
       <c r="B25" t="s">
-        <v>1617</v>
+        <v>1620</v>
       </c>
       <c r="C25" t="s">
-        <v>1618</v>
+        <v>1621</v>
       </c>
       <c r="D25" t="s">
         <v>145</v>
@@ -10900,18 +10929,18 @@
         <v>170</v>
       </c>
       <c r="F25" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>1619</v>
+        <v>1622</v>
       </c>
       <c r="B26" t="s">
-        <v>1620</v>
+        <v>1623</v>
       </c>
       <c r="C26" t="s">
-        <v>1621</v>
+        <v>1624</v>
       </c>
       <c r="D26" t="s">
         <v>145</v>
@@ -10920,18 +10949,18 @@
         <v>170</v>
       </c>
       <c r="F26" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>1622</v>
+        <v>1625</v>
       </c>
       <c r="B27" t="s">
-        <v>1623</v>
+        <v>1626</v>
       </c>
       <c r="C27" t="s">
-        <v>1624</v>
+        <v>1627</v>
       </c>
       <c r="D27" t="s">
         <v>145</v>
@@ -10940,18 +10969,18 @@
         <v>170</v>
       </c>
       <c r="F27" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>1625</v>
+        <v>1628</v>
       </c>
       <c r="B28" t="s">
-        <v>1626</v>
+        <v>1629</v>
       </c>
       <c r="C28" t="s">
-        <v>1627</v>
+        <v>1630</v>
       </c>
       <c r="D28" t="s">
         <v>145</v>
@@ -10960,18 +10989,18 @@
         <v>170</v>
       </c>
       <c r="F28" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1628</v>
+        <v>1631</v>
       </c>
       <c r="B29" t="s">
-        <v>1629</v>
+        <v>1632</v>
       </c>
       <c r="C29" t="s">
-        <v>1630</v>
+        <v>1633</v>
       </c>
       <c r="D29" t="s">
         <v>145</v>
@@ -10980,18 +11009,18 @@
         <v>170</v>
       </c>
       <c r="F29" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>1631</v>
+        <v>1634</v>
       </c>
       <c r="B30" t="s">
-        <v>1632</v>
+        <v>1635</v>
       </c>
       <c r="C30" t="s">
-        <v>1633</v>
+        <v>1636</v>
       </c>
       <c r="D30" t="s">
         <v>145</v>
@@ -11000,23 +11029,23 @@
         <v>170</v>
       </c>
       <c r="F30" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="31" spans="6:6">
       <c r="F31" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>1634</v>
+        <v>1637</v>
       </c>
       <c r="B32" t="s">
-        <v>1635</v>
+        <v>1638</v>
       </c>
       <c r="C32" t="s">
-        <v>1636</v>
+        <v>1639</v>
       </c>
       <c r="D32" t="s">
         <v>145</v>
@@ -11025,18 +11054,18 @@
         <v>170</v>
       </c>
       <c r="F32" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>1637</v>
+        <v>1640</v>
       </c>
       <c r="B33" t="s">
-        <v>1638</v>
+        <v>1641</v>
       </c>
       <c r="C33" t="s">
-        <v>1639</v>
+        <v>1642</v>
       </c>
       <c r="D33" t="s">
         <v>145</v>
@@ -11045,18 +11074,18 @@
         <v>170</v>
       </c>
       <c r="F33" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>1640</v>
+        <v>1643</v>
       </c>
       <c r="B34" t="s">
-        <v>1641</v>
+        <v>1644</v>
       </c>
       <c r="C34" t="s">
-        <v>1642</v>
+        <v>1645</v>
       </c>
       <c r="D34" t="s">
         <v>145</v>
@@ -11065,18 +11094,18 @@
         <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>1643</v>
+        <v>1646</v>
       </c>
       <c r="B35" t="s">
-        <v>1644</v>
+        <v>1647</v>
       </c>
       <c r="C35" t="s">
-        <v>1645</v>
+        <v>1648</v>
       </c>
       <c r="D35" t="s">
         <v>145</v>
@@ -11085,18 +11114,18 @@
         <v>170</v>
       </c>
       <c r="F35" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>1646</v>
+        <v>1649</v>
       </c>
       <c r="B36" t="s">
-        <v>1647</v>
+        <v>1650</v>
       </c>
       <c r="C36" t="s">
-        <v>1648</v>
+        <v>1651</v>
       </c>
       <c r="D36" t="s">
         <v>145</v>
@@ -11105,18 +11134,18 @@
         <v>170</v>
       </c>
       <c r="F36" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>1649</v>
+        <v>1652</v>
       </c>
       <c r="B37" t="s">
-        <v>1650</v>
+        <v>1653</v>
       </c>
       <c r="C37" t="s">
-        <v>1651</v>
+        <v>1654</v>
       </c>
       <c r="D37" t="s">
         <v>145</v>
@@ -11125,18 +11154,18 @@
         <v>170</v>
       </c>
       <c r="F37" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>1652</v>
+        <v>1655</v>
       </c>
       <c r="B38" t="s">
-        <v>1653</v>
+        <v>1656</v>
       </c>
       <c r="C38" t="s">
-        <v>1654</v>
+        <v>1657</v>
       </c>
       <c r="D38" t="s">
         <v>145</v>
@@ -11145,18 +11174,18 @@
         <v>170</v>
       </c>
       <c r="F38" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>1655</v>
+        <v>1658</v>
       </c>
       <c r="B39" t="s">
-        <v>1656</v>
+        <v>1659</v>
       </c>
       <c r="C39" t="s">
-        <v>1657</v>
+        <v>1660</v>
       </c>
       <c r="D39" t="s">
         <v>145</v>
@@ -11165,18 +11194,18 @@
         <v>170</v>
       </c>
       <c r="F39" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>1658</v>
+        <v>1661</v>
       </c>
       <c r="B40" t="s">
-        <v>1659</v>
+        <v>1662</v>
       </c>
       <c r="C40" t="s">
-        <v>1660</v>
+        <v>1663</v>
       </c>
       <c r="D40" t="s">
         <v>145</v>
@@ -11185,18 +11214,18 @@
         <v>170</v>
       </c>
       <c r="F40" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>1661</v>
+        <v>1664</v>
       </c>
       <c r="B41" t="s">
-        <v>1662</v>
+        <v>1665</v>
       </c>
       <c r="C41" t="s">
-        <v>1663</v>
+        <v>1666</v>
       </c>
       <c r="D41" t="s">
         <v>145</v>
@@ -11205,23 +11234,23 @@
         <v>170</v>
       </c>
       <c r="F41" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="42" spans="6:6">
       <c r="F42" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>1664</v>
+        <v>1667</v>
       </c>
       <c r="B43" t="s">
-        <v>1665</v>
+        <v>1668</v>
       </c>
       <c r="C43" t="s">
-        <v>1666</v>
+        <v>1669</v>
       </c>
       <c r="D43" t="s">
         <v>145</v>
@@ -11230,18 +11259,18 @@
         <v>170</v>
       </c>
       <c r="F43" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>1667</v>
+        <v>1670</v>
       </c>
       <c r="B44" t="s">
-        <v>1668</v>
+        <v>1671</v>
       </c>
       <c r="C44" t="s">
-        <v>1669</v>
+        <v>1672</v>
       </c>
       <c r="D44" t="s">
         <v>145</v>
@@ -11250,18 +11279,18 @@
         <v>170</v>
       </c>
       <c r="F44" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>1670</v>
+        <v>1673</v>
       </c>
       <c r="B45" t="s">
-        <v>1671</v>
+        <v>1674</v>
       </c>
       <c r="C45" t="s">
-        <v>1672</v>
+        <v>1675</v>
       </c>
       <c r="D45" t="s">
         <v>145</v>
@@ -11270,18 +11299,18 @@
         <v>170</v>
       </c>
       <c r="F45" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>1673</v>
+        <v>1676</v>
       </c>
       <c r="B46" t="s">
-        <v>1674</v>
+        <v>1677</v>
       </c>
       <c r="C46" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="D46" t="s">
         <v>145</v>
@@ -11290,18 +11319,18 @@
         <v>170</v>
       </c>
       <c r="F46" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>1676</v>
+        <v>1679</v>
       </c>
       <c r="B47" t="s">
-        <v>1677</v>
+        <v>1680</v>
       </c>
       <c r="C47" t="s">
-        <v>1678</v>
+        <v>1681</v>
       </c>
       <c r="D47" t="s">
         <v>145</v>
@@ -11310,18 +11339,18 @@
         <v>170</v>
       </c>
       <c r="F47" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>1679</v>
+        <v>1682</v>
       </c>
       <c r="B48" t="s">
-        <v>1680</v>
+        <v>1683</v>
       </c>
       <c r="C48" t="s">
-        <v>1681</v>
+        <v>1684</v>
       </c>
       <c r="D48" t="s">
         <v>145</v>
@@ -11330,18 +11359,18 @@
         <v>170</v>
       </c>
       <c r="F48" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>1682</v>
+        <v>1685</v>
       </c>
       <c r="B49" t="s">
-        <v>1683</v>
+        <v>1686</v>
       </c>
       <c r="C49" t="s">
-        <v>1684</v>
+        <v>1687</v>
       </c>
       <c r="D49" t="s">
         <v>145</v>
@@ -11350,18 +11379,18 @@
         <v>170</v>
       </c>
       <c r="F49" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>1685</v>
+        <v>1688</v>
       </c>
       <c r="B50" t="s">
-        <v>1686</v>
+        <v>1689</v>
       </c>
       <c r="C50" t="s">
-        <v>1687</v>
+        <v>1690</v>
       </c>
       <c r="D50" t="s">
         <v>145</v>
@@ -11370,18 +11399,18 @@
         <v>170</v>
       </c>
       <c r="F50" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>1688</v>
+        <v>1691</v>
       </c>
       <c r="B51" t="s">
-        <v>1689</v>
+        <v>1692</v>
       </c>
       <c r="C51" t="s">
-        <v>1690</v>
+        <v>1693</v>
       </c>
       <c r="D51" t="s">
         <v>145</v>
@@ -11390,18 +11419,18 @@
         <v>170</v>
       </c>
       <c r="F51" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>1691</v>
+        <v>1694</v>
       </c>
       <c r="B52" t="s">
-        <v>1692</v>
+        <v>1695</v>
       </c>
       <c r="C52" t="s">
-        <v>1693</v>
+        <v>1696</v>
       </c>
       <c r="D52" t="s">
         <v>145</v>
@@ -11410,23 +11439,23 @@
         <v>170</v>
       </c>
       <c r="F52" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="53" spans="6:6">
       <c r="F53" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>1694</v>
+        <v>1697</v>
       </c>
       <c r="B54" t="s">
-        <v>1695</v>
+        <v>1698</v>
       </c>
       <c r="C54" t="s">
-        <v>1696</v>
+        <v>1699</v>
       </c>
       <c r="D54" t="s">
         <v>145</v>
@@ -11435,18 +11464,18 @@
         <v>170</v>
       </c>
       <c r="F54" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>1697</v>
+        <v>1700</v>
       </c>
       <c r="B55" t="s">
-        <v>1698</v>
+        <v>1701</v>
       </c>
       <c r="C55" t="s">
-        <v>1699</v>
+        <v>1702</v>
       </c>
       <c r="D55" t="s">
         <v>145</v>
@@ -11455,18 +11484,18 @@
         <v>170</v>
       </c>
       <c r="F55" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>1700</v>
+        <v>1703</v>
       </c>
       <c r="B56" t="s">
-        <v>1701</v>
+        <v>1704</v>
       </c>
       <c r="C56" t="s">
-        <v>1702</v>
+        <v>1705</v>
       </c>
       <c r="D56" t="s">
         <v>145</v>
@@ -11475,18 +11504,18 @@
         <v>170</v>
       </c>
       <c r="F56" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>1703</v>
+        <v>1706</v>
       </c>
       <c r="B57" t="s">
-        <v>1704</v>
+        <v>1707</v>
       </c>
       <c r="C57" t="s">
-        <v>1705</v>
+        <v>1708</v>
       </c>
       <c r="D57" t="s">
         <v>145</v>
@@ -11495,18 +11524,18 @@
         <v>170</v>
       </c>
       <c r="F57" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>1706</v>
+        <v>1709</v>
       </c>
       <c r="B58" t="s">
-        <v>1707</v>
+        <v>1710</v>
       </c>
       <c r="C58" t="s">
-        <v>1708</v>
+        <v>1711</v>
       </c>
       <c r="D58" t="s">
         <v>145</v>
@@ -11515,18 +11544,18 @@
         <v>170</v>
       </c>
       <c r="F58" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>1709</v>
+        <v>1712</v>
       </c>
       <c r="B59" t="s">
-        <v>1710</v>
+        <v>1713</v>
       </c>
       <c r="C59" t="s">
-        <v>1711</v>
+        <v>1714</v>
       </c>
       <c r="D59" t="s">
         <v>145</v>
@@ -11535,18 +11564,18 @@
         <v>170</v>
       </c>
       <c r="F59" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>1712</v>
+        <v>1715</v>
       </c>
       <c r="B60" t="s">
-        <v>1713</v>
+        <v>1716</v>
       </c>
       <c r="C60" t="s">
-        <v>1714</v>
+        <v>1717</v>
       </c>
       <c r="D60" t="s">
         <v>145</v>
@@ -11555,18 +11584,18 @@
         <v>170</v>
       </c>
       <c r="F60" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>1715</v>
+        <v>1718</v>
       </c>
       <c r="B61" t="s">
-        <v>1716</v>
+        <v>1719</v>
       </c>
       <c r="C61" t="s">
-        <v>1717</v>
+        <v>1720</v>
       </c>
       <c r="D61" t="s">
         <v>145</v>
@@ -11575,18 +11604,18 @@
         <v>170</v>
       </c>
       <c r="F61" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>1718</v>
+        <v>1721</v>
       </c>
       <c r="B62" t="s">
-        <v>1719</v>
+        <v>1722</v>
       </c>
       <c r="C62" t="s">
-        <v>1720</v>
+        <v>1723</v>
       </c>
       <c r="D62" t="s">
         <v>145</v>
@@ -11595,18 +11624,18 @@
         <v>170</v>
       </c>
       <c r="F62" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>1721</v>
+        <v>1724</v>
       </c>
       <c r="B63" t="s">
-        <v>1722</v>
+        <v>1725</v>
       </c>
       <c r="C63" t="s">
-        <v>1723</v>
+        <v>1726</v>
       </c>
       <c r="D63" t="s">
         <v>145</v>
@@ -11615,23 +11644,23 @@
         <v>170</v>
       </c>
       <c r="F63" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="64" spans="6:6">
       <c r="F64" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>1724</v>
+        <v>1727</v>
       </c>
       <c r="B65" t="s">
-        <v>1725</v>
+        <v>1728</v>
       </c>
       <c r="C65" t="s">
-        <v>1726</v>
+        <v>1729</v>
       </c>
       <c r="D65" t="s">
         <v>145</v>
@@ -11640,18 +11669,18 @@
         <v>170</v>
       </c>
       <c r="F65" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>1727</v>
+        <v>1730</v>
       </c>
       <c r="B66" t="s">
-        <v>1728</v>
+        <v>1731</v>
       </c>
       <c r="C66" t="s">
-        <v>1729</v>
+        <v>1732</v>
       </c>
       <c r="D66" t="s">
         <v>145</v>
@@ -11660,18 +11689,18 @@
         <v>170</v>
       </c>
       <c r="F66" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>1730</v>
+        <v>1733</v>
       </c>
       <c r="B67" t="s">
-        <v>1731</v>
+        <v>1734</v>
       </c>
       <c r="C67" t="s">
-        <v>1732</v>
+        <v>1735</v>
       </c>
       <c r="D67" t="s">
         <v>145</v>
@@ -11680,18 +11709,18 @@
         <v>170</v>
       </c>
       <c r="F67" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>1733</v>
+        <v>1736</v>
       </c>
       <c r="B68" t="s">
-        <v>1734</v>
+        <v>1737</v>
       </c>
       <c r="C68" t="s">
-        <v>1735</v>
+        <v>1738</v>
       </c>
       <c r="D68" t="s">
         <v>145</v>
@@ -11700,18 +11729,18 @@
         <v>170</v>
       </c>
       <c r="F68" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>1736</v>
+        <v>1739</v>
       </c>
       <c r="B69" t="s">
-        <v>1737</v>
+        <v>1740</v>
       </c>
       <c r="C69" t="s">
-        <v>1738</v>
+        <v>1741</v>
       </c>
       <c r="D69" t="s">
         <v>145</v>
@@ -11720,18 +11749,18 @@
         <v>170</v>
       </c>
       <c r="F69" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>1739</v>
+        <v>1742</v>
       </c>
       <c r="B70" t="s">
-        <v>1740</v>
+        <v>1743</v>
       </c>
       <c r="C70" t="s">
-        <v>1741</v>
+        <v>1744</v>
       </c>
       <c r="D70" t="s">
         <v>145</v>
@@ -11740,18 +11769,18 @@
         <v>170</v>
       </c>
       <c r="F70" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>1742</v>
+        <v>1745</v>
       </c>
       <c r="B71" t="s">
-        <v>1743</v>
+        <v>1746</v>
       </c>
       <c r="C71" t="s">
-        <v>1744</v>
+        <v>1747</v>
       </c>
       <c r="D71" t="s">
         <v>145</v>
@@ -11760,18 +11789,18 @@
         <v>170</v>
       </c>
       <c r="F71" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>1745</v>
+        <v>1748</v>
       </c>
       <c r="B72" t="s">
-        <v>1746</v>
+        <v>1749</v>
       </c>
       <c r="C72" t="s">
-        <v>1747</v>
+        <v>1750</v>
       </c>
       <c r="D72" t="s">
         <v>145</v>
@@ -11780,18 +11809,18 @@
         <v>170</v>
       </c>
       <c r="F72" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>1748</v>
+        <v>1751</v>
       </c>
       <c r="B73" t="s">
-        <v>1749</v>
+        <v>1752</v>
       </c>
       <c r="C73" t="s">
-        <v>1750</v>
+        <v>1753</v>
       </c>
       <c r="D73" t="s">
         <v>145</v>
@@ -11800,18 +11829,18 @@
         <v>170</v>
       </c>
       <c r="F73" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>1751</v>
+        <v>1754</v>
       </c>
       <c r="B74" t="s">
-        <v>1752</v>
+        <v>1755</v>
       </c>
       <c r="C74" t="s">
-        <v>1753</v>
+        <v>1756</v>
       </c>
       <c r="D74" t="s">
         <v>145</v>
@@ -11820,23 +11849,23 @@
         <v>170</v>
       </c>
       <c r="F74" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="75" spans="6:6">
       <c r="F75" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>1754</v>
+        <v>1757</v>
       </c>
       <c r="B76" t="s">
-        <v>1755</v>
+        <v>1758</v>
       </c>
       <c r="C76" t="s">
-        <v>1756</v>
+        <v>1759</v>
       </c>
       <c r="D76" t="s">
         <v>145</v>
@@ -11845,18 +11874,18 @@
         <v>170</v>
       </c>
       <c r="F76" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>1757</v>
+        <v>1760</v>
       </c>
       <c r="B77" t="s">
-        <v>1758</v>
+        <v>1761</v>
       </c>
       <c r="C77" t="s">
-        <v>1759</v>
+        <v>1762</v>
       </c>
       <c r="D77" t="s">
         <v>145</v>
@@ -11865,18 +11894,18 @@
         <v>170</v>
       </c>
       <c r="F77" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>1760</v>
+        <v>1763</v>
       </c>
       <c r="B78" t="s">
-        <v>1761</v>
+        <v>1764</v>
       </c>
       <c r="C78" t="s">
-        <v>1762</v>
+        <v>1765</v>
       </c>
       <c r="D78" t="s">
         <v>145</v>
@@ -11885,18 +11914,18 @@
         <v>170</v>
       </c>
       <c r="F78" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>1763</v>
+        <v>1766</v>
       </c>
       <c r="B79" t="s">
-        <v>1764</v>
+        <v>1767</v>
       </c>
       <c r="C79" t="s">
-        <v>1765</v>
+        <v>1768</v>
       </c>
       <c r="D79" t="s">
         <v>145</v>
@@ -11905,18 +11934,18 @@
         <v>170</v>
       </c>
       <c r="F79" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>1766</v>
+        <v>1769</v>
       </c>
       <c r="B80" t="s">
-        <v>1767</v>
+        <v>1770</v>
       </c>
       <c r="C80" t="s">
-        <v>1768</v>
+        <v>1771</v>
       </c>
       <c r="D80" t="s">
         <v>145</v>
@@ -11925,18 +11954,18 @@
         <v>170</v>
       </c>
       <c r="F80" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>1769</v>
+        <v>1772</v>
       </c>
       <c r="B81" t="s">
-        <v>1770</v>
+        <v>1773</v>
       </c>
       <c r="C81" t="s">
-        <v>1771</v>
+        <v>1774</v>
       </c>
       <c r="D81" t="s">
         <v>145</v>
@@ -11945,18 +11974,18 @@
         <v>170</v>
       </c>
       <c r="F81" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>1772</v>
+        <v>1775</v>
       </c>
       <c r="B82" t="s">
-        <v>1773</v>
+        <v>1776</v>
       </c>
       <c r="C82" t="s">
-        <v>1774</v>
+        <v>1777</v>
       </c>
       <c r="D82" t="s">
         <v>145</v>
@@ -11965,18 +11994,18 @@
         <v>170</v>
       </c>
       <c r="F82" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>1775</v>
+        <v>1778</v>
       </c>
       <c r="B83" t="s">
-        <v>1776</v>
+        <v>1779</v>
       </c>
       <c r="C83" t="s">
-        <v>1777</v>
+        <v>1780</v>
       </c>
       <c r="D83" t="s">
         <v>145</v>
@@ -11985,18 +12014,18 @@
         <v>170</v>
       </c>
       <c r="F83" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>1778</v>
+        <v>1781</v>
       </c>
       <c r="B84" t="s">
-        <v>1779</v>
+        <v>1782</v>
       </c>
       <c r="C84" t="s">
-        <v>1780</v>
+        <v>1783</v>
       </c>
       <c r="D84" t="s">
         <v>145</v>
@@ -12005,18 +12034,18 @@
         <v>170</v>
       </c>
       <c r="F84" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>1781</v>
+        <v>1784</v>
       </c>
       <c r="B85" t="s">
-        <v>1782</v>
+        <v>1785</v>
       </c>
       <c r="C85" t="s">
-        <v>1783</v>
+        <v>1786</v>
       </c>
       <c r="D85" t="s">
         <v>145</v>
@@ -12025,18 +12054,18 @@
         <v>170</v>
       </c>
       <c r="F85" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>1784</v>
+        <v>1787</v>
       </c>
       <c r="B86" t="s">
-        <v>1785</v>
+        <v>1788</v>
       </c>
       <c r="C86" t="s">
-        <v>1786</v>
+        <v>1789</v>
       </c>
       <c r="D86" t="s">
         <v>145</v>
@@ -12045,18 +12074,18 @@
         <v>170</v>
       </c>
       <c r="F86" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>1787</v>
+        <v>1790</v>
       </c>
       <c r="B87" t="s">
-        <v>1788</v>
+        <v>1791</v>
       </c>
       <c r="C87" t="s">
-        <v>1789</v>
+        <v>1792</v>
       </c>
       <c r="D87" t="s">
         <v>145</v>
@@ -12065,18 +12094,18 @@
         <v>170</v>
       </c>
       <c r="F87" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>1790</v>
+        <v>1793</v>
       </c>
       <c r="B88" t="s">
-        <v>1791</v>
+        <v>1794</v>
       </c>
       <c r="C88" t="s">
-        <v>1792</v>
+        <v>1795</v>
       </c>
       <c r="D88" t="s">
         <v>145</v>
@@ -12085,18 +12114,18 @@
         <v>170</v>
       </c>
       <c r="F88" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>1793</v>
+        <v>1796</v>
       </c>
       <c r="B89" t="s">
-        <v>1794</v>
+        <v>1797</v>
       </c>
       <c r="C89" t="s">
-        <v>1795</v>
+        <v>1798</v>
       </c>
       <c r="D89" t="s">
         <v>145</v>
@@ -12105,18 +12134,18 @@
         <v>170</v>
       </c>
       <c r="F89" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>1796</v>
+        <v>1799</v>
       </c>
       <c r="B90" t="s">
-        <v>1797</v>
+        <v>1800</v>
       </c>
       <c r="C90" t="s">
-        <v>1798</v>
+        <v>1801</v>
       </c>
       <c r="D90" t="s">
         <v>145</v>
@@ -12125,18 +12154,18 @@
         <v>170</v>
       </c>
       <c r="F90" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>1799</v>
+        <v>1802</v>
       </c>
       <c r="B91" t="s">
-        <v>1800</v>
+        <v>1803</v>
       </c>
       <c r="C91" t="s">
-        <v>1801</v>
+        <v>1804</v>
       </c>
       <c r="D91" t="s">
         <v>145</v>
@@ -12145,18 +12174,18 @@
         <v>170</v>
       </c>
       <c r="F91" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>1802</v>
+        <v>1805</v>
       </c>
       <c r="B92" t="s">
-        <v>1803</v>
+        <v>1806</v>
       </c>
       <c r="C92" t="s">
-        <v>1804</v>
+        <v>1807</v>
       </c>
       <c r="D92" t="s">
         <v>145</v>
@@ -12165,18 +12194,18 @@
         <v>170</v>
       </c>
       <c r="F92" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>1805</v>
+        <v>1808</v>
       </c>
       <c r="B93" t="s">
-        <v>1806</v>
+        <v>1809</v>
       </c>
       <c r="C93" t="s">
-        <v>1807</v>
+        <v>1810</v>
       </c>
       <c r="D93" t="s">
         <v>145</v>
@@ -12185,18 +12214,18 @@
         <v>170</v>
       </c>
       <c r="F93" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>1808</v>
+        <v>1811</v>
       </c>
       <c r="B94" t="s">
-        <v>1809</v>
+        <v>1812</v>
       </c>
       <c r="C94" t="s">
-        <v>1810</v>
+        <v>1813</v>
       </c>
       <c r="D94" t="s">
         <v>145</v>
@@ -12205,18 +12234,18 @@
         <v>170</v>
       </c>
       <c r="F94" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>1811</v>
+        <v>1814</v>
       </c>
       <c r="B95" t="s">
-        <v>1812</v>
+        <v>1815</v>
       </c>
       <c r="C95" t="s">
-        <v>1813</v>
+        <v>1816</v>
       </c>
       <c r="D95" t="s">
         <v>145</v>
@@ -12225,18 +12254,18 @@
         <v>170</v>
       </c>
       <c r="F95" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>1814</v>
+        <v>1817</v>
       </c>
       <c r="B96" t="s">
-        <v>1815</v>
+        <v>1818</v>
       </c>
       <c r="C96" t="s">
-        <v>1816</v>
+        <v>1819</v>
       </c>
       <c r="D96" t="s">
         <v>145</v>
@@ -12245,18 +12274,18 @@
         <v>170</v>
       </c>
       <c r="F96" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>1817</v>
+        <v>1820</v>
       </c>
       <c r="B97" t="s">
-        <v>1818</v>
+        <v>1821</v>
       </c>
       <c r="C97" t="s">
-        <v>1819</v>
+        <v>1822</v>
       </c>
       <c r="D97" t="s">
         <v>145</v>
@@ -12265,18 +12294,18 @@
         <v>170</v>
       </c>
       <c r="F97" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>1820</v>
+        <v>1823</v>
       </c>
       <c r="B98" t="s">
-        <v>1821</v>
+        <v>1824</v>
       </c>
       <c r="C98" t="s">
-        <v>1822</v>
+        <v>1825</v>
       </c>
       <c r="D98" t="s">
         <v>145</v>
@@ -12285,18 +12314,18 @@
         <v>170</v>
       </c>
       <c r="F98" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>1823</v>
+        <v>1826</v>
       </c>
       <c r="B99" t="s">
-        <v>1824</v>
+        <v>1827</v>
       </c>
       <c r="C99" t="s">
-        <v>1825</v>
+        <v>1828</v>
       </c>
       <c r="D99" t="s">
         <v>145</v>
@@ -12305,18 +12334,18 @@
         <v>170</v>
       </c>
       <c r="F99" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>1826</v>
+        <v>1829</v>
       </c>
       <c r="B100" t="s">
-        <v>1827</v>
+        <v>1830</v>
       </c>
       <c r="C100" t="s">
-        <v>1828</v>
+        <v>1831</v>
       </c>
       <c r="D100" t="s">
         <v>145</v>
@@ -12325,18 +12354,18 @@
         <v>170</v>
       </c>
       <c r="F100" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>1829</v>
+        <v>1832</v>
       </c>
       <c r="B101" t="s">
-        <v>1830</v>
+        <v>1833</v>
       </c>
       <c r="C101" t="s">
-        <v>1831</v>
+        <v>1834</v>
       </c>
       <c r="D101" t="s">
         <v>145</v>
@@ -12345,18 +12374,18 @@
         <v>170</v>
       </c>
       <c r="F101" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>1832</v>
+        <v>1835</v>
       </c>
       <c r="B102" t="s">
-        <v>1833</v>
+        <v>1836</v>
       </c>
       <c r="C102" t="s">
-        <v>1834</v>
+        <v>1837</v>
       </c>
       <c r="D102" t="s">
         <v>145</v>
@@ -12365,18 +12394,18 @@
         <v>170</v>
       </c>
       <c r="F102" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>1835</v>
+        <v>1838</v>
       </c>
       <c r="B103" t="s">
-        <v>1836</v>
+        <v>1839</v>
       </c>
       <c r="C103" t="s">
-        <v>1837</v>
+        <v>1840</v>
       </c>
       <c r="D103" t="s">
         <v>145</v>
@@ -12385,18 +12414,18 @@
         <v>170</v>
       </c>
       <c r="F103" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B104" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="C104" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="D104" t="s">
         <v>145</v>
@@ -12405,18 +12434,18 @@
         <v>170</v>
       </c>
       <c r="F104" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>1841</v>
+        <v>1844</v>
       </c>
       <c r="B105" t="s">
-        <v>1842</v>
+        <v>1845</v>
       </c>
       <c r="C105" t="s">
-        <v>1843</v>
+        <v>1846</v>
       </c>
       <c r="D105" t="s">
         <v>145</v>
@@ -12425,18 +12454,18 @@
         <v>170</v>
       </c>
       <c r="F105" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>1844</v>
+        <v>1847</v>
       </c>
       <c r="B106" t="s">
-        <v>1845</v>
+        <v>1848</v>
       </c>
       <c r="C106" t="s">
-        <v>1846</v>
+        <v>1849</v>
       </c>
       <c r="D106" t="s">
         <v>145</v>
@@ -12445,18 +12474,18 @@
         <v>170</v>
       </c>
       <c r="F106" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>1847</v>
+        <v>1850</v>
       </c>
       <c r="B107" t="s">
-        <v>1848</v>
+        <v>1851</v>
       </c>
       <c r="C107" t="s">
-        <v>1849</v>
+        <v>1852</v>
       </c>
       <c r="D107" t="s">
         <v>145</v>
@@ -12465,18 +12494,18 @@
         <v>170</v>
       </c>
       <c r="F107" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>1850</v>
+        <v>1853</v>
       </c>
       <c r="B108" t="s">
-        <v>1851</v>
+        <v>1854</v>
       </c>
       <c r="C108" t="s">
-        <v>1852</v>
+        <v>1855</v>
       </c>
       <c r="D108" t="s">
         <v>145</v>
@@ -12485,18 +12514,18 @@
         <v>170</v>
       </c>
       <c r="F108" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>1853</v>
+        <v>1856</v>
       </c>
       <c r="B109" t="s">
-        <v>1854</v>
+        <v>1857</v>
       </c>
       <c r="C109" t="s">
-        <v>1855</v>
+        <v>1858</v>
       </c>
       <c r="D109" t="s">
         <v>145</v>
@@ -12505,18 +12534,18 @@
         <v>170</v>
       </c>
       <c r="F109" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>1856</v>
+        <v>1859</v>
       </c>
       <c r="B110" t="s">
-        <v>1857</v>
+        <v>1860</v>
       </c>
       <c r="C110" t="s">
-        <v>1858</v>
+        <v>1861</v>
       </c>
       <c r="D110" t="s">
         <v>145</v>
@@ -12525,18 +12554,18 @@
         <v>170</v>
       </c>
       <c r="F110" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>1859</v>
+        <v>1862</v>
       </c>
       <c r="B111" t="s">
-        <v>1860</v>
+        <v>1863</v>
       </c>
       <c r="C111" t="s">
-        <v>1861</v>
+        <v>1864</v>
       </c>
       <c r="D111" t="s">
         <v>145</v>
@@ -12545,18 +12574,18 @@
         <v>170</v>
       </c>
       <c r="F111" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>1862</v>
+        <v>1865</v>
       </c>
       <c r="B112" t="s">
-        <v>1863</v>
+        <v>1866</v>
       </c>
       <c r="C112" t="s">
-        <v>1864</v>
+        <v>1867</v>
       </c>
       <c r="D112" t="s">
         <v>145</v>
@@ -12565,18 +12594,18 @@
         <v>170</v>
       </c>
       <c r="F112" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>1865</v>
+        <v>1868</v>
       </c>
       <c r="B113" t="s">
-        <v>1866</v>
+        <v>1869</v>
       </c>
       <c r="C113" t="s">
-        <v>1867</v>
+        <v>1870</v>
       </c>
       <c r="D113" t="s">
         <v>145</v>
@@ -12585,18 +12614,18 @@
         <v>170</v>
       </c>
       <c r="F113" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>1868</v>
+        <v>1871</v>
       </c>
       <c r="B114" t="s">
-        <v>1869</v>
+        <v>1872</v>
       </c>
       <c r="C114" t="s">
-        <v>1870</v>
+        <v>1873</v>
       </c>
       <c r="D114" t="s">
         <v>145</v>
@@ -12605,7 +12634,7 @@
         <v>170</v>
       </c>
       <c r="F114" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
   </sheetData>
@@ -13460,7 +13489,7 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>1871</v>
+        <v>1874</v>
       </c>
     </row>
   </sheetData>
@@ -14445,7 +14474,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F54" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -14465,7 +14494,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F55" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -14485,7 +14514,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F56" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -14505,7 +14534,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F57" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -14525,7 +14554,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F58" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -14545,7 +14574,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F59" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -14565,7 +14594,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F60" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -14585,7 +14614,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F61" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -14605,7 +14634,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F62" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
   </sheetData>
@@ -15986,7 +16015,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F77" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -16006,7 +16035,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F78" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -16026,7 +16055,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F79" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -16046,7 +16075,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F80" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -16066,7 +16095,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F81" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -16086,7 +16115,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F82" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -16106,7 +16135,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F83" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -16126,7 +16155,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F84" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -16146,7 +16175,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F85" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -19468,7 +19497,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F79" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -19488,7 +19517,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F80" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -19508,7 +19537,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F81" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -19528,7 +19557,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F82" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -19548,7 +19577,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F83" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -19568,7 +19597,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F84" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -19588,7 +19617,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F85" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -19608,7 +19637,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F86" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -19628,7 +19657,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F87" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -26618,7 +26647,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F343" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="344" spans="1:6">
@@ -26638,7 +26667,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F344" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="345" spans="1:6">
@@ -26658,7 +26687,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F345" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="346" spans="1:6">
@@ -26678,7 +26707,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F346" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="347" spans="1:6">
@@ -26698,7 +26727,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F347" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="348" spans="1:6">
@@ -26718,7 +26747,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F348" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="349" spans="1:6">
@@ -26738,7 +26767,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F349" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="350" spans="1:6">
@@ -26758,7 +26787,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F350" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="351" spans="1:6">
@@ -26778,7 +26807,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F351" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="366" spans="1:6">
@@ -32019,7 +32048,7 @@
   <sheetPr/>
   <dimension ref="A1:F530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
+    <sheetView topLeftCell="A345" workbookViewId="0">
       <selection activeCell="A528" sqref="A528:F530"/>
     </sheetView>
   </sheetViews>
@@ -33390,7 +33419,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F73" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -33410,7 +33439,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F74" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -33430,7 +33459,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F75" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -33450,7 +33479,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F76" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -33470,7 +33499,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F77" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -33490,7 +33519,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F78" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -33510,7 +33539,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F79" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -33530,7 +33559,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F80" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -33550,7 +33579,7 @@
         <v>Quản lý Quyết Định</v>
       </c>
       <c r="F81" t="str">
-        <v>S_NHANVIEN_CHUNG</v>
+        <v>S_HRM_CHUNG</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -41762,19 +41791,19 @@
     </row>
     <row r="528" spans="1:6">
       <c r="A528" t="s">
-        <v>1872</v>
+        <v>1875</v>
       </c>
       <c r="B528" t="s">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="C528" t="s">
-        <v>1874</v>
+        <v>1877</v>
       </c>
       <c r="D528" t="s">
         <v>118</v>
       </c>
       <c r="E528" t="s">
-        <v>1875</v>
+        <v>1878</v>
       </c>
       <c r="F528" t="s">
         <v>59</v>
@@ -41782,19 +41811,19 @@
     </row>
     <row r="529" spans="1:6">
       <c r="A529" t="s">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="B529" t="s">
-        <v>1877</v>
+        <v>1880</v>
       </c>
       <c r="C529" t="s">
-        <v>1878</v>
+        <v>1881</v>
       </c>
       <c r="D529" t="s">
         <v>118</v>
       </c>
       <c r="E529" t="s">
-        <v>1875</v>
+        <v>1878</v>
       </c>
       <c r="F529" t="s">
         <v>59</v>
@@ -41802,19 +41831,19 @@
     </row>
     <row r="530" spans="1:6">
       <c r="A530" t="s">
-        <v>1879</v>
+        <v>1882</v>
       </c>
       <c r="B530" t="s">
-        <v>1880</v>
+        <v>1883</v>
       </c>
       <c r="C530" t="s">
-        <v>1881</v>
+        <v>1884</v>
       </c>
       <c r="D530" t="s">
         <v>118</v>
       </c>
       <c r="E530" t="s">
-        <v>1875</v>
+        <v>1878</v>
       </c>
       <c r="F530" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Add UC11.1.4, UC11.1.3; pytest --nomigrations
</commit_message>
<xml_diff>
--- a/apps/core/fixtures/core_permission.xlsx
+++ b/apps/core/fixtures/core_permission.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16260" tabRatio="894" firstSheet="2" activeTab="9"/>
+    <workbookView windowHeight="16260" tabRatio="894" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="core_permission" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="1885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4052" uniqueCount="1889">
   <si>
     <t>code</t>
   </si>
@@ -4506,6 +4506,18 @@
   </si>
   <si>
     <t>Quyền cập nhật ManagerAssessment</t>
+  </si>
+  <si>
+    <t>hrm.dashboard.manager.realtime</t>
+  </si>
+  <si>
+    <t>[HCNS] [Manager Dashboard] Xem thống kê các vấn đề HCNS cần xử lý</t>
+  </si>
+  <si>
+    <t>Xem thống kê các đề xuất cần xác nhận và đánh giá KPI</t>
+  </si>
+  <si>
+    <t>Manager Dashboard</t>
   </si>
   <si>
     <t>employee_kpi_assessment.create</t>
@@ -7119,8 +7131,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="S_TRUONGPHONG" displayName="S_TRUONGPHONG" ref="A1:F39" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F39" etc:filterBottomFollowUsedRange="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="S_TRUONGPHONG" displayName="S_TRUONGPHONG" ref="A1:F40" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F40" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="6">
     <tableColumn id="1" name="code" dataDxfId="60"/>
     <tableColumn id="2" name="Tên" dataDxfId="61"/>
@@ -8106,7 +8118,7 @@
   <sheetPr/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -8872,10 +8884,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -9665,6 +9677,26 @@
         <v>1454</v>
       </c>
       <c r="F39" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F40" t="s">
         <v>1399</v>
       </c>
     </row>
@@ -9718,13 +9750,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>1473</v>
+        <v>1477</v>
       </c>
       <c r="B2" t="s">
-        <v>1474</v>
+        <v>1478</v>
       </c>
       <c r="C2" t="s">
-        <v>1475</v>
+        <v>1479</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -9733,18 +9765,18 @@
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>1477</v>
+        <v>1481</v>
       </c>
       <c r="B3" t="s">
-        <v>1478</v>
+        <v>1482</v>
       </c>
       <c r="C3" t="s">
-        <v>1479</v>
+        <v>1483</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -9753,7 +9785,7 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -9773,7 +9805,7 @@
         <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9793,7 +9825,7 @@
         <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -9813,7 +9845,7 @@
         <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -9833,7 +9865,7 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -9853,7 +9885,7 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -9873,18 +9905,18 @@
         <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1480</v>
+        <v>1484</v>
       </c>
       <c r="B10" t="s">
-        <v>1481</v>
+        <v>1485</v>
       </c>
       <c r="C10" t="s">
-        <v>1482</v>
+        <v>1486</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
@@ -9893,18 +9925,18 @@
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1483</v>
+        <v>1487</v>
       </c>
       <c r="B11" t="s">
-        <v>1484</v>
+        <v>1488</v>
       </c>
       <c r="C11" t="s">
-        <v>1485</v>
+        <v>1489</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
@@ -9913,18 +9945,18 @@
         <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1486</v>
+        <v>1490</v>
       </c>
       <c r="B12" t="s">
-        <v>1487</v>
+        <v>1491</v>
       </c>
       <c r="C12" t="s">
-        <v>1488</v>
+        <v>1492</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
@@ -9933,18 +9965,18 @@
         <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1489</v>
+        <v>1493</v>
       </c>
       <c r="B13" t="s">
-        <v>1490</v>
+        <v>1494</v>
       </c>
       <c r="C13" t="s">
-        <v>1491</v>
+        <v>1495</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -9953,7 +9985,7 @@
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -9973,7 +10005,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -9993,198 +10025,198 @@
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1492</v>
+        <v>1496</v>
       </c>
       <c r="B16" t="s">
-        <v>1493</v>
+        <v>1497</v>
       </c>
       <c r="C16" t="s">
-        <v>1494</v>
+        <v>1498</v>
       </c>
       <c r="D16" t="s">
         <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F16" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1496</v>
+        <v>1500</v>
       </c>
       <c r="B17" t="s">
-        <v>1497</v>
+        <v>1501</v>
       </c>
       <c r="C17" t="s">
-        <v>1498</v>
+        <v>1502</v>
       </c>
       <c r="D17" t="s">
         <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F17" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1499</v>
+        <v>1503</v>
       </c>
       <c r="B18" t="s">
-        <v>1500</v>
+        <v>1504</v>
       </c>
       <c r="C18" t="s">
-        <v>1501</v>
+        <v>1505</v>
       </c>
       <c r="D18" t="s">
         <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F18" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1502</v>
+        <v>1506</v>
       </c>
       <c r="B19" t="s">
-        <v>1503</v>
+        <v>1507</v>
       </c>
       <c r="C19" t="s">
-        <v>1504</v>
+        <v>1508</v>
       </c>
       <c r="D19" t="s">
         <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F19" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>1505</v>
+        <v>1509</v>
       </c>
       <c r="B20" t="s">
-        <v>1506</v>
+        <v>1510</v>
       </c>
       <c r="C20" t="s">
-        <v>1507</v>
+        <v>1511</v>
       </c>
       <c r="D20" t="s">
         <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F20" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>1508</v>
+        <v>1512</v>
       </c>
       <c r="B21" t="s">
-        <v>1509</v>
+        <v>1513</v>
       </c>
       <c r="C21" t="s">
-        <v>1510</v>
+        <v>1514</v>
       </c>
       <c r="D21" t="s">
         <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F21" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>1511</v>
+        <v>1515</v>
       </c>
       <c r="B22" t="s">
-        <v>1512</v>
+        <v>1516</v>
       </c>
       <c r="C22" t="s">
-        <v>1513</v>
+        <v>1517</v>
       </c>
       <c r="D22" t="s">
         <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F22" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1514</v>
+        <v>1518</v>
       </c>
       <c r="B23" t="s">
-        <v>1515</v>
+        <v>1519</v>
       </c>
       <c r="C23" t="s">
-        <v>1516</v>
+        <v>1520</v>
       </c>
       <c r="D23" t="s">
         <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F23" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>1517</v>
+        <v>1521</v>
       </c>
       <c r="B24" t="s">
-        <v>1518</v>
+        <v>1522</v>
       </c>
       <c r="C24" t="s">
-        <v>1519</v>
+        <v>1523</v>
       </c>
       <c r="D24" t="s">
         <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="F24" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>1520</v>
+        <v>1524</v>
       </c>
       <c r="B25" t="s">
-        <v>1521</v>
+        <v>1525</v>
       </c>
       <c r="C25" t="s">
-        <v>1522</v>
+        <v>1526</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -10193,18 +10225,18 @@
         <v>1048</v>
       </c>
       <c r="F25" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>1523</v>
+        <v>1527</v>
       </c>
       <c r="B26" t="s">
-        <v>1524</v>
+        <v>1528</v>
       </c>
       <c r="C26" t="s">
-        <v>1525</v>
+        <v>1529</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -10213,12 +10245,12 @@
         <v>1048</v>
       </c>
       <c r="F26" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>1526</v>
+        <v>1530</v>
       </c>
       <c r="B27" t="s">
         <v>1046</v>
@@ -10233,12 +10265,12 @@
         <v>1048</v>
       </c>
       <c r="F27" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>1527</v>
+        <v>1531</v>
       </c>
       <c r="B28" t="s">
         <v>1050</v>
@@ -10253,18 +10285,18 @@
         <v>1048</v>
       </c>
       <c r="F28" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1528</v>
+        <v>1532</v>
       </c>
       <c r="B29" t="s">
-        <v>1529</v>
+        <v>1533</v>
       </c>
       <c r="C29" t="s">
-        <v>1530</v>
+        <v>1534</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
@@ -10273,18 +10305,18 @@
         <v>1048</v>
       </c>
       <c r="F29" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>1531</v>
+        <v>1535</v>
       </c>
       <c r="B30" t="s">
-        <v>1532</v>
+        <v>1536</v>
       </c>
       <c r="C30" t="s">
-        <v>1533</v>
+        <v>1537</v>
       </c>
       <c r="D30" t="s">
         <v>28</v>
@@ -10293,18 +10325,18 @@
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>1534</v>
+        <v>1538</v>
       </c>
       <c r="B31" t="s">
-        <v>1535</v>
+        <v>1539</v>
       </c>
       <c r="C31" t="s">
-        <v>1536</v>
+        <v>1540</v>
       </c>
       <c r="D31" t="s">
         <v>28</v>
@@ -10313,18 +10345,18 @@
         <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>1537</v>
+        <v>1541</v>
       </c>
       <c r="B32" t="s">
-        <v>1538</v>
+        <v>1542</v>
       </c>
       <c r="C32" t="s">
-        <v>1539</v>
+        <v>1543</v>
       </c>
       <c r="D32" t="s">
         <v>28</v>
@@ -10333,18 +10365,18 @@
         <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>1540</v>
+        <v>1544</v>
       </c>
       <c r="B33" t="s">
-        <v>1541</v>
+        <v>1545</v>
       </c>
       <c r="C33" t="s">
-        <v>1542</v>
+        <v>1546</v>
       </c>
       <c r="D33" t="s">
         <v>28</v>
@@ -10353,18 +10385,18 @@
         <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>1543</v>
+        <v>1547</v>
       </c>
       <c r="B34" t="s">
-        <v>1544</v>
+        <v>1548</v>
       </c>
       <c r="C34" t="s">
-        <v>1545</v>
+        <v>1549</v>
       </c>
       <c r="D34" t="s">
         <v>28</v>
@@ -10373,18 +10405,18 @@
         <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>1546</v>
+        <v>1550</v>
       </c>
       <c r="B35" t="s">
-        <v>1547</v>
+        <v>1551</v>
       </c>
       <c r="C35" t="s">
-        <v>1548</v>
+        <v>1552</v>
       </c>
       <c r="D35" t="s">
         <v>28</v>
@@ -10393,18 +10425,18 @@
         <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>1549</v>
+        <v>1553</v>
       </c>
       <c r="B36" t="s">
-        <v>1550</v>
+        <v>1554</v>
       </c>
       <c r="C36" t="s">
-        <v>1551</v>
+        <v>1555</v>
       </c>
       <c r="D36" t="s">
         <v>28</v>
@@ -10413,18 +10445,18 @@
         <v>29</v>
       </c>
       <c r="F36" t="s">
-        <v>1476</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>1552</v>
+        <v>1556</v>
       </c>
       <c r="B37" t="s">
-        <v>1553</v>
+        <v>1557</v>
       </c>
       <c r="C37" t="s">
-        <v>1554</v>
+        <v>1558</v>
       </c>
       <c r="D37" t="s">
         <v>28</v>
@@ -10484,13 +10516,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>1555</v>
+        <v>1559</v>
       </c>
       <c r="B2" t="s">
-        <v>1556</v>
+        <v>1560</v>
       </c>
       <c r="C2" t="s">
-        <v>1557</v>
+        <v>1561</v>
       </c>
       <c r="D2" t="s">
         <v>145</v>
@@ -10499,18 +10531,18 @@
         <v>170</v>
       </c>
       <c r="F2" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>1559</v>
+        <v>1563</v>
       </c>
       <c r="B3" t="s">
-        <v>1560</v>
+        <v>1564</v>
       </c>
       <c r="C3" t="s">
-        <v>1561</v>
+        <v>1565</v>
       </c>
       <c r="D3" t="s">
         <v>145</v>
@@ -10519,18 +10551,18 @@
         <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>1562</v>
+        <v>1566</v>
       </c>
       <c r="B4" t="s">
-        <v>1563</v>
+        <v>1567</v>
       </c>
       <c r="C4" t="s">
-        <v>1564</v>
+        <v>1568</v>
       </c>
       <c r="D4" t="s">
         <v>145</v>
@@ -10539,18 +10571,18 @@
         <v>170</v>
       </c>
       <c r="F4" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>1565</v>
+        <v>1569</v>
       </c>
       <c r="B5" t="s">
-        <v>1566</v>
+        <v>1570</v>
       </c>
       <c r="C5" t="s">
-        <v>1567</v>
+        <v>1571</v>
       </c>
       <c r="D5" t="s">
         <v>145</v>
@@ -10559,18 +10591,18 @@
         <v>170</v>
       </c>
       <c r="F5" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>1568</v>
+        <v>1572</v>
       </c>
       <c r="B6" t="s">
-        <v>1569</v>
+        <v>1573</v>
       </c>
       <c r="C6" t="s">
-        <v>1570</v>
+        <v>1574</v>
       </c>
       <c r="D6" t="s">
         <v>145</v>
@@ -10579,18 +10611,18 @@
         <v>170</v>
       </c>
       <c r="F6" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>1571</v>
+        <v>1575</v>
       </c>
       <c r="B7" t="s">
-        <v>1572</v>
+        <v>1576</v>
       </c>
       <c r="C7" t="s">
-        <v>1573</v>
+        <v>1577</v>
       </c>
       <c r="D7" t="s">
         <v>145</v>
@@ -10599,18 +10631,18 @@
         <v>170</v>
       </c>
       <c r="F7" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>1574</v>
+        <v>1578</v>
       </c>
       <c r="B8" t="s">
-        <v>1575</v>
+        <v>1579</v>
       </c>
       <c r="C8" t="s">
-        <v>1576</v>
+        <v>1580</v>
       </c>
       <c r="D8" t="s">
         <v>145</v>
@@ -10619,23 +10651,23 @@
         <v>170</v>
       </c>
       <c r="F8" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="9" spans="6:6">
       <c r="F9" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1577</v>
+        <v>1581</v>
       </c>
       <c r="B10" t="s">
-        <v>1578</v>
+        <v>1582</v>
       </c>
       <c r="C10" t="s">
-        <v>1579</v>
+        <v>1583</v>
       </c>
       <c r="D10" t="s">
         <v>145</v>
@@ -10644,18 +10676,18 @@
         <v>170</v>
       </c>
       <c r="F10" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1580</v>
+        <v>1584</v>
       </c>
       <c r="B11" t="s">
-        <v>1581</v>
+        <v>1585</v>
       </c>
       <c r="C11" t="s">
-        <v>1582</v>
+        <v>1586</v>
       </c>
       <c r="D11" t="s">
         <v>145</v>
@@ -10664,18 +10696,18 @@
         <v>170</v>
       </c>
       <c r="F11" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1583</v>
+        <v>1587</v>
       </c>
       <c r="B12" t="s">
-        <v>1584</v>
+        <v>1588</v>
       </c>
       <c r="C12" t="s">
-        <v>1585</v>
+        <v>1589</v>
       </c>
       <c r="D12" t="s">
         <v>145</v>
@@ -10684,18 +10716,18 @@
         <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1586</v>
+        <v>1590</v>
       </c>
       <c r="B13" t="s">
-        <v>1587</v>
+        <v>1591</v>
       </c>
       <c r="C13" t="s">
-        <v>1588</v>
+        <v>1592</v>
       </c>
       <c r="D13" t="s">
         <v>145</v>
@@ -10704,18 +10736,18 @@
         <v>170</v>
       </c>
       <c r="F13" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>1589</v>
+        <v>1593</v>
       </c>
       <c r="B14" t="s">
-        <v>1590</v>
+        <v>1594</v>
       </c>
       <c r="C14" t="s">
-        <v>1591</v>
+        <v>1595</v>
       </c>
       <c r="D14" t="s">
         <v>145</v>
@@ -10724,18 +10756,18 @@
         <v>170</v>
       </c>
       <c r="F14" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>1592</v>
+        <v>1596</v>
       </c>
       <c r="B15" t="s">
-        <v>1593</v>
+        <v>1597</v>
       </c>
       <c r="C15" t="s">
-        <v>1594</v>
+        <v>1598</v>
       </c>
       <c r="D15" t="s">
         <v>145</v>
@@ -10744,18 +10776,18 @@
         <v>170</v>
       </c>
       <c r="F15" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1595</v>
+        <v>1599</v>
       </c>
       <c r="B16" t="s">
-        <v>1596</v>
+        <v>1600</v>
       </c>
       <c r="C16" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D16" t="s">
         <v>145</v>
@@ -10764,18 +10796,18 @@
         <v>170</v>
       </c>
       <c r="F16" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="B17" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="C17" t="s">
-        <v>1600</v>
+        <v>1604</v>
       </c>
       <c r="D17" t="s">
         <v>145</v>
@@ -10784,18 +10816,18 @@
         <v>170</v>
       </c>
       <c r="F17" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1601</v>
+        <v>1605</v>
       </c>
       <c r="B18" t="s">
-        <v>1602</v>
+        <v>1606</v>
       </c>
       <c r="C18" t="s">
-        <v>1603</v>
+        <v>1607</v>
       </c>
       <c r="D18" t="s">
         <v>145</v>
@@ -10804,18 +10836,18 @@
         <v>170</v>
       </c>
       <c r="F18" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1604</v>
+        <v>1608</v>
       </c>
       <c r="B19" t="s">
-        <v>1605</v>
+        <v>1609</v>
       </c>
       <c r="C19" t="s">
-        <v>1606</v>
+        <v>1610</v>
       </c>
       <c r="D19" t="s">
         <v>145</v>
@@ -10824,23 +10856,23 @@
         <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="20" spans="6:6">
       <c r="F20" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>1607</v>
+        <v>1611</v>
       </c>
       <c r="B21" t="s">
-        <v>1608</v>
+        <v>1612</v>
       </c>
       <c r="C21" t="s">
-        <v>1609</v>
+        <v>1613</v>
       </c>
       <c r="D21" t="s">
         <v>145</v>
@@ -10849,18 +10881,18 @@
         <v>170</v>
       </c>
       <c r="F21" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>1610</v>
+        <v>1614</v>
       </c>
       <c r="B22" t="s">
-        <v>1611</v>
+        <v>1615</v>
       </c>
       <c r="C22" t="s">
-        <v>1612</v>
+        <v>1616</v>
       </c>
       <c r="D22" t="s">
         <v>145</v>
@@ -10869,18 +10901,18 @@
         <v>170</v>
       </c>
       <c r="F22" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1613</v>
+        <v>1617</v>
       </c>
       <c r="B23" t="s">
-        <v>1614</v>
+        <v>1618</v>
       </c>
       <c r="C23" t="s">
-        <v>1615</v>
+        <v>1619</v>
       </c>
       <c r="D23" t="s">
         <v>145</v>
@@ -10889,18 +10921,18 @@
         <v>170</v>
       </c>
       <c r="F23" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>1616</v>
+        <v>1620</v>
       </c>
       <c r="B24" t="s">
-        <v>1617</v>
+        <v>1621</v>
       </c>
       <c r="C24" t="s">
-        <v>1618</v>
+        <v>1622</v>
       </c>
       <c r="D24" t="s">
         <v>145</v>
@@ -10909,18 +10941,18 @@
         <v>170</v>
       </c>
       <c r="F24" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>1619</v>
+        <v>1623</v>
       </c>
       <c r="B25" t="s">
-        <v>1620</v>
+        <v>1624</v>
       </c>
       <c r="C25" t="s">
-        <v>1621</v>
+        <v>1625</v>
       </c>
       <c r="D25" t="s">
         <v>145</v>
@@ -10929,18 +10961,18 @@
         <v>170</v>
       </c>
       <c r="F25" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>1622</v>
+        <v>1626</v>
       </c>
       <c r="B26" t="s">
-        <v>1623</v>
+        <v>1627</v>
       </c>
       <c r="C26" t="s">
-        <v>1624</v>
+        <v>1628</v>
       </c>
       <c r="D26" t="s">
         <v>145</v>
@@ -10949,18 +10981,18 @@
         <v>170</v>
       </c>
       <c r="F26" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>1625</v>
+        <v>1629</v>
       </c>
       <c r="B27" t="s">
-        <v>1626</v>
+        <v>1630</v>
       </c>
       <c r="C27" t="s">
-        <v>1627</v>
+        <v>1631</v>
       </c>
       <c r="D27" t="s">
         <v>145</v>
@@ -10969,18 +11001,18 @@
         <v>170</v>
       </c>
       <c r="F27" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>1628</v>
+        <v>1632</v>
       </c>
       <c r="B28" t="s">
-        <v>1629</v>
+        <v>1633</v>
       </c>
       <c r="C28" t="s">
-        <v>1630</v>
+        <v>1634</v>
       </c>
       <c r="D28" t="s">
         <v>145</v>
@@ -10989,18 +11021,18 @@
         <v>170</v>
       </c>
       <c r="F28" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1631</v>
+        <v>1635</v>
       </c>
       <c r="B29" t="s">
-        <v>1632</v>
+        <v>1636</v>
       </c>
       <c r="C29" t="s">
-        <v>1633</v>
+        <v>1637</v>
       </c>
       <c r="D29" t="s">
         <v>145</v>
@@ -11009,18 +11041,18 @@
         <v>170</v>
       </c>
       <c r="F29" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>1634</v>
+        <v>1638</v>
       </c>
       <c r="B30" t="s">
-        <v>1635</v>
+        <v>1639</v>
       </c>
       <c r="C30" t="s">
-        <v>1636</v>
+        <v>1640</v>
       </c>
       <c r="D30" t="s">
         <v>145</v>
@@ -11029,23 +11061,23 @@
         <v>170</v>
       </c>
       <c r="F30" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="31" spans="6:6">
       <c r="F31" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>1637</v>
+        <v>1641</v>
       </c>
       <c r="B32" t="s">
-        <v>1638</v>
+        <v>1642</v>
       </c>
       <c r="C32" t="s">
-        <v>1639</v>
+        <v>1643</v>
       </c>
       <c r="D32" t="s">
         <v>145</v>
@@ -11054,18 +11086,18 @@
         <v>170</v>
       </c>
       <c r="F32" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>1640</v>
+        <v>1644</v>
       </c>
       <c r="B33" t="s">
-        <v>1641</v>
+        <v>1645</v>
       </c>
       <c r="C33" t="s">
-        <v>1642</v>
+        <v>1646</v>
       </c>
       <c r="D33" t="s">
         <v>145</v>
@@ -11074,18 +11106,18 @@
         <v>170</v>
       </c>
       <c r="F33" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>1643</v>
+        <v>1647</v>
       </c>
       <c r="B34" t="s">
-        <v>1644</v>
+        <v>1648</v>
       </c>
       <c r="C34" t="s">
-        <v>1645</v>
+        <v>1649</v>
       </c>
       <c r="D34" t="s">
         <v>145</v>
@@ -11094,18 +11126,18 @@
         <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>1646</v>
+        <v>1650</v>
       </c>
       <c r="B35" t="s">
-        <v>1647</v>
+        <v>1651</v>
       </c>
       <c r="C35" t="s">
-        <v>1648</v>
+        <v>1652</v>
       </c>
       <c r="D35" t="s">
         <v>145</v>
@@ -11114,18 +11146,18 @@
         <v>170</v>
       </c>
       <c r="F35" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>1649</v>
+        <v>1653</v>
       </c>
       <c r="B36" t="s">
-        <v>1650</v>
+        <v>1654</v>
       </c>
       <c r="C36" t="s">
-        <v>1651</v>
+        <v>1655</v>
       </c>
       <c r="D36" t="s">
         <v>145</v>
@@ -11134,18 +11166,18 @@
         <v>170</v>
       </c>
       <c r="F36" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>1652</v>
+        <v>1656</v>
       </c>
       <c r="B37" t="s">
-        <v>1653</v>
+        <v>1657</v>
       </c>
       <c r="C37" t="s">
-        <v>1654</v>
+        <v>1658</v>
       </c>
       <c r="D37" t="s">
         <v>145</v>
@@ -11154,18 +11186,18 @@
         <v>170</v>
       </c>
       <c r="F37" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>1655</v>
+        <v>1659</v>
       </c>
       <c r="B38" t="s">
-        <v>1656</v>
+        <v>1660</v>
       </c>
       <c r="C38" t="s">
-        <v>1657</v>
+        <v>1661</v>
       </c>
       <c r="D38" t="s">
         <v>145</v>
@@ -11174,18 +11206,18 @@
         <v>170</v>
       </c>
       <c r="F38" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>1658</v>
+        <v>1662</v>
       </c>
       <c r="B39" t="s">
-        <v>1659</v>
+        <v>1663</v>
       </c>
       <c r="C39" t="s">
-        <v>1660</v>
+        <v>1664</v>
       </c>
       <c r="D39" t="s">
         <v>145</v>
@@ -11194,18 +11226,18 @@
         <v>170</v>
       </c>
       <c r="F39" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>1661</v>
+        <v>1665</v>
       </c>
       <c r="B40" t="s">
-        <v>1662</v>
+        <v>1666</v>
       </c>
       <c r="C40" t="s">
-        <v>1663</v>
+        <v>1667</v>
       </c>
       <c r="D40" t="s">
         <v>145</v>
@@ -11214,18 +11246,18 @@
         <v>170</v>
       </c>
       <c r="F40" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>1664</v>
+        <v>1668</v>
       </c>
       <c r="B41" t="s">
-        <v>1665</v>
+        <v>1669</v>
       </c>
       <c r="C41" t="s">
-        <v>1666</v>
+        <v>1670</v>
       </c>
       <c r="D41" t="s">
         <v>145</v>
@@ -11234,23 +11266,23 @@
         <v>170</v>
       </c>
       <c r="F41" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="42" spans="6:6">
       <c r="F42" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>1667</v>
+        <v>1671</v>
       </c>
       <c r="B43" t="s">
-        <v>1668</v>
+        <v>1672</v>
       </c>
       <c r="C43" t="s">
-        <v>1669</v>
+        <v>1673</v>
       </c>
       <c r="D43" t="s">
         <v>145</v>
@@ -11259,18 +11291,18 @@
         <v>170</v>
       </c>
       <c r="F43" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>1670</v>
+        <v>1674</v>
       </c>
       <c r="B44" t="s">
-        <v>1671</v>
+        <v>1675</v>
       </c>
       <c r="C44" t="s">
-        <v>1672</v>
+        <v>1676</v>
       </c>
       <c r="D44" t="s">
         <v>145</v>
@@ -11279,18 +11311,18 @@
         <v>170</v>
       </c>
       <c r="F44" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>1673</v>
+        <v>1677</v>
       </c>
       <c r="B45" t="s">
-        <v>1674</v>
+        <v>1678</v>
       </c>
       <c r="C45" t="s">
-        <v>1675</v>
+        <v>1679</v>
       </c>
       <c r="D45" t="s">
         <v>145</v>
@@ -11299,18 +11331,18 @@
         <v>170</v>
       </c>
       <c r="F45" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>1676</v>
+        <v>1680</v>
       </c>
       <c r="B46" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="C46" t="s">
-        <v>1678</v>
+        <v>1682</v>
       </c>
       <c r="D46" t="s">
         <v>145</v>
@@ -11319,18 +11351,18 @@
         <v>170</v>
       </c>
       <c r="F46" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>1679</v>
+        <v>1683</v>
       </c>
       <c r="B47" t="s">
-        <v>1680</v>
+        <v>1684</v>
       </c>
       <c r="C47" t="s">
-        <v>1681</v>
+        <v>1685</v>
       </c>
       <c r="D47" t="s">
         <v>145</v>
@@ -11339,18 +11371,18 @@
         <v>170</v>
       </c>
       <c r="F47" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>1682</v>
+        <v>1686</v>
       </c>
       <c r="B48" t="s">
-        <v>1683</v>
+        <v>1687</v>
       </c>
       <c r="C48" t="s">
-        <v>1684</v>
+        <v>1688</v>
       </c>
       <c r="D48" t="s">
         <v>145</v>
@@ -11359,18 +11391,18 @@
         <v>170</v>
       </c>
       <c r="F48" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>1685</v>
+        <v>1689</v>
       </c>
       <c r="B49" t="s">
-        <v>1686</v>
+        <v>1690</v>
       </c>
       <c r="C49" t="s">
-        <v>1687</v>
+        <v>1691</v>
       </c>
       <c r="D49" t="s">
         <v>145</v>
@@ -11379,18 +11411,18 @@
         <v>170</v>
       </c>
       <c r="F49" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>1688</v>
+        <v>1692</v>
       </c>
       <c r="B50" t="s">
-        <v>1689</v>
+        <v>1693</v>
       </c>
       <c r="C50" t="s">
-        <v>1690</v>
+        <v>1694</v>
       </c>
       <c r="D50" t="s">
         <v>145</v>
@@ -11399,18 +11431,18 @@
         <v>170</v>
       </c>
       <c r="F50" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>1691</v>
+        <v>1695</v>
       </c>
       <c r="B51" t="s">
-        <v>1692</v>
+        <v>1696</v>
       </c>
       <c r="C51" t="s">
-        <v>1693</v>
+        <v>1697</v>
       </c>
       <c r="D51" t="s">
         <v>145</v>
@@ -11419,18 +11451,18 @@
         <v>170</v>
       </c>
       <c r="F51" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>1694</v>
+        <v>1698</v>
       </c>
       <c r="B52" t="s">
-        <v>1695</v>
+        <v>1699</v>
       </c>
       <c r="C52" t="s">
-        <v>1696</v>
+        <v>1700</v>
       </c>
       <c r="D52" t="s">
         <v>145</v>
@@ -11439,23 +11471,23 @@
         <v>170</v>
       </c>
       <c r="F52" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="53" spans="6:6">
       <c r="F53" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>1697</v>
+        <v>1701</v>
       </c>
       <c r="B54" t="s">
-        <v>1698</v>
+        <v>1702</v>
       </c>
       <c r="C54" t="s">
-        <v>1699</v>
+        <v>1703</v>
       </c>
       <c r="D54" t="s">
         <v>145</v>
@@ -11464,18 +11496,18 @@
         <v>170</v>
       </c>
       <c r="F54" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>1700</v>
+        <v>1704</v>
       </c>
       <c r="B55" t="s">
-        <v>1701</v>
+        <v>1705</v>
       </c>
       <c r="C55" t="s">
-        <v>1702</v>
+        <v>1706</v>
       </c>
       <c r="D55" t="s">
         <v>145</v>
@@ -11484,18 +11516,18 @@
         <v>170</v>
       </c>
       <c r="F55" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>1703</v>
+        <v>1707</v>
       </c>
       <c r="B56" t="s">
-        <v>1704</v>
+        <v>1708</v>
       </c>
       <c r="C56" t="s">
-        <v>1705</v>
+        <v>1709</v>
       </c>
       <c r="D56" t="s">
         <v>145</v>
@@ -11504,18 +11536,18 @@
         <v>170</v>
       </c>
       <c r="F56" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>1706</v>
+        <v>1710</v>
       </c>
       <c r="B57" t="s">
-        <v>1707</v>
+        <v>1711</v>
       </c>
       <c r="C57" t="s">
-        <v>1708</v>
+        <v>1712</v>
       </c>
       <c r="D57" t="s">
         <v>145</v>
@@ -11524,18 +11556,18 @@
         <v>170</v>
       </c>
       <c r="F57" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>1709</v>
+        <v>1713</v>
       </c>
       <c r="B58" t="s">
-        <v>1710</v>
+        <v>1714</v>
       </c>
       <c r="C58" t="s">
-        <v>1711</v>
+        <v>1715</v>
       </c>
       <c r="D58" t="s">
         <v>145</v>
@@ -11544,18 +11576,18 @@
         <v>170</v>
       </c>
       <c r="F58" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>1712</v>
+        <v>1716</v>
       </c>
       <c r="B59" t="s">
-        <v>1713</v>
+        <v>1717</v>
       </c>
       <c r="C59" t="s">
-        <v>1714</v>
+        <v>1718</v>
       </c>
       <c r="D59" t="s">
         <v>145</v>
@@ -11564,18 +11596,18 @@
         <v>170</v>
       </c>
       <c r="F59" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>1715</v>
+        <v>1719</v>
       </c>
       <c r="B60" t="s">
-        <v>1716</v>
+        <v>1720</v>
       </c>
       <c r="C60" t="s">
-        <v>1717</v>
+        <v>1721</v>
       </c>
       <c r="D60" t="s">
         <v>145</v>
@@ -11584,18 +11616,18 @@
         <v>170</v>
       </c>
       <c r="F60" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>1718</v>
+        <v>1722</v>
       </c>
       <c r="B61" t="s">
-        <v>1719</v>
+        <v>1723</v>
       </c>
       <c r="C61" t="s">
-        <v>1720</v>
+        <v>1724</v>
       </c>
       <c r="D61" t="s">
         <v>145</v>
@@ -11604,18 +11636,18 @@
         <v>170</v>
       </c>
       <c r="F61" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>1721</v>
+        <v>1725</v>
       </c>
       <c r="B62" t="s">
-        <v>1722</v>
+        <v>1726</v>
       </c>
       <c r="C62" t="s">
-        <v>1723</v>
+        <v>1727</v>
       </c>
       <c r="D62" t="s">
         <v>145</v>
@@ -11624,18 +11656,18 @@
         <v>170</v>
       </c>
       <c r="F62" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>1724</v>
+        <v>1728</v>
       </c>
       <c r="B63" t="s">
-        <v>1725</v>
+        <v>1729</v>
       </c>
       <c r="C63" t="s">
-        <v>1726</v>
+        <v>1730</v>
       </c>
       <c r="D63" t="s">
         <v>145</v>
@@ -11644,23 +11676,23 @@
         <v>170</v>
       </c>
       <c r="F63" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="64" spans="6:6">
       <c r="F64" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>1727</v>
+        <v>1731</v>
       </c>
       <c r="B65" t="s">
-        <v>1728</v>
+        <v>1732</v>
       </c>
       <c r="C65" t="s">
-        <v>1729</v>
+        <v>1733</v>
       </c>
       <c r="D65" t="s">
         <v>145</v>
@@ -11669,18 +11701,18 @@
         <v>170</v>
       </c>
       <c r="F65" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>1730</v>
+        <v>1734</v>
       </c>
       <c r="B66" t="s">
-        <v>1731</v>
+        <v>1735</v>
       </c>
       <c r="C66" t="s">
-        <v>1732</v>
+        <v>1736</v>
       </c>
       <c r="D66" t="s">
         <v>145</v>
@@ -11689,18 +11721,18 @@
         <v>170</v>
       </c>
       <c r="F66" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>1733</v>
+        <v>1737</v>
       </c>
       <c r="B67" t="s">
-        <v>1734</v>
+        <v>1738</v>
       </c>
       <c r="C67" t="s">
-        <v>1735</v>
+        <v>1739</v>
       </c>
       <c r="D67" t="s">
         <v>145</v>
@@ -11709,18 +11741,18 @@
         <v>170</v>
       </c>
       <c r="F67" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>1736</v>
+        <v>1740</v>
       </c>
       <c r="B68" t="s">
-        <v>1737</v>
+        <v>1741</v>
       </c>
       <c r="C68" t="s">
-        <v>1738</v>
+        <v>1742</v>
       </c>
       <c r="D68" t="s">
         <v>145</v>
@@ -11729,18 +11761,18 @@
         <v>170</v>
       </c>
       <c r="F68" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>1739</v>
+        <v>1743</v>
       </c>
       <c r="B69" t="s">
-        <v>1740</v>
+        <v>1744</v>
       </c>
       <c r="C69" t="s">
-        <v>1741</v>
+        <v>1745</v>
       </c>
       <c r="D69" t="s">
         <v>145</v>
@@ -11749,18 +11781,18 @@
         <v>170</v>
       </c>
       <c r="F69" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>1742</v>
+        <v>1746</v>
       </c>
       <c r="B70" t="s">
-        <v>1743</v>
+        <v>1747</v>
       </c>
       <c r="C70" t="s">
-        <v>1744</v>
+        <v>1748</v>
       </c>
       <c r="D70" t="s">
         <v>145</v>
@@ -11769,18 +11801,18 @@
         <v>170</v>
       </c>
       <c r="F70" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>1745</v>
+        <v>1749</v>
       </c>
       <c r="B71" t="s">
-        <v>1746</v>
+        <v>1750</v>
       </c>
       <c r="C71" t="s">
-        <v>1747</v>
+        <v>1751</v>
       </c>
       <c r="D71" t="s">
         <v>145</v>
@@ -11789,18 +11821,18 @@
         <v>170</v>
       </c>
       <c r="F71" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>1748</v>
+        <v>1752</v>
       </c>
       <c r="B72" t="s">
-        <v>1749</v>
+        <v>1753</v>
       </c>
       <c r="C72" t="s">
-        <v>1750</v>
+        <v>1754</v>
       </c>
       <c r="D72" t="s">
         <v>145</v>
@@ -11809,18 +11841,18 @@
         <v>170</v>
       </c>
       <c r="F72" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>1751</v>
+        <v>1755</v>
       </c>
       <c r="B73" t="s">
-        <v>1752</v>
+        <v>1756</v>
       </c>
       <c r="C73" t="s">
-        <v>1753</v>
+        <v>1757</v>
       </c>
       <c r="D73" t="s">
         <v>145</v>
@@ -11829,18 +11861,18 @@
         <v>170</v>
       </c>
       <c r="F73" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>1754</v>
+        <v>1758</v>
       </c>
       <c r="B74" t="s">
-        <v>1755</v>
+        <v>1759</v>
       </c>
       <c r="C74" t="s">
-        <v>1756</v>
+        <v>1760</v>
       </c>
       <c r="D74" t="s">
         <v>145</v>
@@ -11849,23 +11881,23 @@
         <v>170</v>
       </c>
       <c r="F74" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="75" spans="6:6">
       <c r="F75" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>1757</v>
+        <v>1761</v>
       </c>
       <c r="B76" t="s">
-        <v>1758</v>
+        <v>1762</v>
       </c>
       <c r="C76" t="s">
-        <v>1759</v>
+        <v>1763</v>
       </c>
       <c r="D76" t="s">
         <v>145</v>
@@ -11874,18 +11906,18 @@
         <v>170</v>
       </c>
       <c r="F76" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>1760</v>
+        <v>1764</v>
       </c>
       <c r="B77" t="s">
-        <v>1761</v>
+        <v>1765</v>
       </c>
       <c r="C77" t="s">
-        <v>1762</v>
+        <v>1766</v>
       </c>
       <c r="D77" t="s">
         <v>145</v>
@@ -11894,18 +11926,18 @@
         <v>170</v>
       </c>
       <c r="F77" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>1763</v>
+        <v>1767</v>
       </c>
       <c r="B78" t="s">
-        <v>1764</v>
+        <v>1768</v>
       </c>
       <c r="C78" t="s">
-        <v>1765</v>
+        <v>1769</v>
       </c>
       <c r="D78" t="s">
         <v>145</v>
@@ -11914,18 +11946,18 @@
         <v>170</v>
       </c>
       <c r="F78" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>1766</v>
+        <v>1770</v>
       </c>
       <c r="B79" t="s">
-        <v>1767</v>
+        <v>1771</v>
       </c>
       <c r="C79" t="s">
-        <v>1768</v>
+        <v>1772</v>
       </c>
       <c r="D79" t="s">
         <v>145</v>
@@ -11934,18 +11966,18 @@
         <v>170</v>
       </c>
       <c r="F79" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>1769</v>
+        <v>1773</v>
       </c>
       <c r="B80" t="s">
-        <v>1770</v>
+        <v>1774</v>
       </c>
       <c r="C80" t="s">
-        <v>1771</v>
+        <v>1775</v>
       </c>
       <c r="D80" t="s">
         <v>145</v>
@@ -11954,18 +11986,18 @@
         <v>170</v>
       </c>
       <c r="F80" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>1772</v>
+        <v>1776</v>
       </c>
       <c r="B81" t="s">
-        <v>1773</v>
+        <v>1777</v>
       </c>
       <c r="C81" t="s">
-        <v>1774</v>
+        <v>1778</v>
       </c>
       <c r="D81" t="s">
         <v>145</v>
@@ -11974,18 +12006,18 @@
         <v>170</v>
       </c>
       <c r="F81" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>1775</v>
+        <v>1779</v>
       </c>
       <c r="B82" t="s">
-        <v>1776</v>
+        <v>1780</v>
       </c>
       <c r="C82" t="s">
-        <v>1777</v>
+        <v>1781</v>
       </c>
       <c r="D82" t="s">
         <v>145</v>
@@ -11994,18 +12026,18 @@
         <v>170</v>
       </c>
       <c r="F82" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>1778</v>
+        <v>1782</v>
       </c>
       <c r="B83" t="s">
-        <v>1779</v>
+        <v>1783</v>
       </c>
       <c r="C83" t="s">
-        <v>1780</v>
+        <v>1784</v>
       </c>
       <c r="D83" t="s">
         <v>145</v>
@@ -12014,18 +12046,18 @@
         <v>170</v>
       </c>
       <c r="F83" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>1781</v>
+        <v>1785</v>
       </c>
       <c r="B84" t="s">
-        <v>1782</v>
+        <v>1786</v>
       </c>
       <c r="C84" t="s">
-        <v>1783</v>
+        <v>1787</v>
       </c>
       <c r="D84" t="s">
         <v>145</v>
@@ -12034,18 +12066,18 @@
         <v>170</v>
       </c>
       <c r="F84" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>1784</v>
+        <v>1788</v>
       </c>
       <c r="B85" t="s">
-        <v>1785</v>
+        <v>1789</v>
       </c>
       <c r="C85" t="s">
-        <v>1786</v>
+        <v>1790</v>
       </c>
       <c r="D85" t="s">
         <v>145</v>
@@ -12054,18 +12086,18 @@
         <v>170</v>
       </c>
       <c r="F85" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>1787</v>
+        <v>1791</v>
       </c>
       <c r="B86" t="s">
-        <v>1788</v>
+        <v>1792</v>
       </c>
       <c r="C86" t="s">
-        <v>1789</v>
+        <v>1793</v>
       </c>
       <c r="D86" t="s">
         <v>145</v>
@@ -12074,18 +12106,18 @@
         <v>170</v>
       </c>
       <c r="F86" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>1790</v>
+        <v>1794</v>
       </c>
       <c r="B87" t="s">
-        <v>1791</v>
+        <v>1795</v>
       </c>
       <c r="C87" t="s">
-        <v>1792</v>
+        <v>1796</v>
       </c>
       <c r="D87" t="s">
         <v>145</v>
@@ -12094,18 +12126,18 @@
         <v>170</v>
       </c>
       <c r="F87" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>1793</v>
+        <v>1797</v>
       </c>
       <c r="B88" t="s">
-        <v>1794</v>
+        <v>1798</v>
       </c>
       <c r="C88" t="s">
-        <v>1795</v>
+        <v>1799</v>
       </c>
       <c r="D88" t="s">
         <v>145</v>
@@ -12114,18 +12146,18 @@
         <v>170</v>
       </c>
       <c r="F88" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>1796</v>
+        <v>1800</v>
       </c>
       <c r="B89" t="s">
-        <v>1797</v>
+        <v>1801</v>
       </c>
       <c r="C89" t="s">
-        <v>1798</v>
+        <v>1802</v>
       </c>
       <c r="D89" t="s">
         <v>145</v>
@@ -12134,18 +12166,18 @@
         <v>170</v>
       </c>
       <c r="F89" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>1799</v>
+        <v>1803</v>
       </c>
       <c r="B90" t="s">
-        <v>1800</v>
+        <v>1804</v>
       </c>
       <c r="C90" t="s">
-        <v>1801</v>
+        <v>1805</v>
       </c>
       <c r="D90" t="s">
         <v>145</v>
@@ -12154,18 +12186,18 @@
         <v>170</v>
       </c>
       <c r="F90" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>1802</v>
+        <v>1806</v>
       </c>
       <c r="B91" t="s">
-        <v>1803</v>
+        <v>1807</v>
       </c>
       <c r="C91" t="s">
-        <v>1804</v>
+        <v>1808</v>
       </c>
       <c r="D91" t="s">
         <v>145</v>
@@ -12174,18 +12206,18 @@
         <v>170</v>
       </c>
       <c r="F91" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>1805</v>
+        <v>1809</v>
       </c>
       <c r="B92" t="s">
-        <v>1806</v>
+        <v>1810</v>
       </c>
       <c r="C92" t="s">
-        <v>1807</v>
+        <v>1811</v>
       </c>
       <c r="D92" t="s">
         <v>145</v>
@@ -12194,18 +12226,18 @@
         <v>170</v>
       </c>
       <c r="F92" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>1808</v>
+        <v>1812</v>
       </c>
       <c r="B93" t="s">
-        <v>1809</v>
+        <v>1813</v>
       </c>
       <c r="C93" t="s">
-        <v>1810</v>
+        <v>1814</v>
       </c>
       <c r="D93" t="s">
         <v>145</v>
@@ -12214,18 +12246,18 @@
         <v>170</v>
       </c>
       <c r="F93" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>1811</v>
+        <v>1815</v>
       </c>
       <c r="B94" t="s">
-        <v>1812</v>
+        <v>1816</v>
       </c>
       <c r="C94" t="s">
-        <v>1813</v>
+        <v>1817</v>
       </c>
       <c r="D94" t="s">
         <v>145</v>
@@ -12234,18 +12266,18 @@
         <v>170</v>
       </c>
       <c r="F94" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>1814</v>
+        <v>1818</v>
       </c>
       <c r="B95" t="s">
-        <v>1815</v>
+        <v>1819</v>
       </c>
       <c r="C95" t="s">
-        <v>1816</v>
+        <v>1820</v>
       </c>
       <c r="D95" t="s">
         <v>145</v>
@@ -12254,18 +12286,18 @@
         <v>170</v>
       </c>
       <c r="F95" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>1817</v>
+        <v>1821</v>
       </c>
       <c r="B96" t="s">
-        <v>1818</v>
+        <v>1822</v>
       </c>
       <c r="C96" t="s">
-        <v>1819</v>
+        <v>1823</v>
       </c>
       <c r="D96" t="s">
         <v>145</v>
@@ -12274,18 +12306,18 @@
         <v>170</v>
       </c>
       <c r="F96" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>1820</v>
+        <v>1824</v>
       </c>
       <c r="B97" t="s">
-        <v>1821</v>
+        <v>1825</v>
       </c>
       <c r="C97" t="s">
-        <v>1822</v>
+        <v>1826</v>
       </c>
       <c r="D97" t="s">
         <v>145</v>
@@ -12294,18 +12326,18 @@
         <v>170</v>
       </c>
       <c r="F97" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>1823</v>
+        <v>1827</v>
       </c>
       <c r="B98" t="s">
-        <v>1824</v>
+        <v>1828</v>
       </c>
       <c r="C98" t="s">
-        <v>1825</v>
+        <v>1829</v>
       </c>
       <c r="D98" t="s">
         <v>145</v>
@@ -12314,18 +12346,18 @@
         <v>170</v>
       </c>
       <c r="F98" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>1826</v>
+        <v>1830</v>
       </c>
       <c r="B99" t="s">
-        <v>1827</v>
+        <v>1831</v>
       </c>
       <c r="C99" t="s">
-        <v>1828</v>
+        <v>1832</v>
       </c>
       <c r="D99" t="s">
         <v>145</v>
@@ -12334,18 +12366,18 @@
         <v>170</v>
       </c>
       <c r="F99" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>1829</v>
+        <v>1833</v>
       </c>
       <c r="B100" t="s">
-        <v>1830</v>
+        <v>1834</v>
       </c>
       <c r="C100" t="s">
-        <v>1831</v>
+        <v>1835</v>
       </c>
       <c r="D100" t="s">
         <v>145</v>
@@ -12354,18 +12386,18 @@
         <v>170</v>
       </c>
       <c r="F100" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>1832</v>
+        <v>1836</v>
       </c>
       <c r="B101" t="s">
-        <v>1833</v>
+        <v>1837</v>
       </c>
       <c r="C101" t="s">
-        <v>1834</v>
+        <v>1838</v>
       </c>
       <c r="D101" t="s">
         <v>145</v>
@@ -12374,18 +12406,18 @@
         <v>170</v>
       </c>
       <c r="F101" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>1835</v>
+        <v>1839</v>
       </c>
       <c r="B102" t="s">
-        <v>1836</v>
+        <v>1840</v>
       </c>
       <c r="C102" t="s">
-        <v>1837</v>
+        <v>1841</v>
       </c>
       <c r="D102" t="s">
         <v>145</v>
@@ -12394,18 +12426,18 @@
         <v>170</v>
       </c>
       <c r="F102" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>1838</v>
+        <v>1842</v>
       </c>
       <c r="B103" t="s">
-        <v>1839</v>
+        <v>1843</v>
       </c>
       <c r="C103" t="s">
-        <v>1840</v>
+        <v>1844</v>
       </c>
       <c r="D103" t="s">
         <v>145</v>
@@ -12414,18 +12446,18 @@
         <v>170</v>
       </c>
       <c r="F103" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>1841</v>
+        <v>1845</v>
       </c>
       <c r="B104" t="s">
-        <v>1842</v>
+        <v>1846</v>
       </c>
       <c r="C104" t="s">
-        <v>1843</v>
+        <v>1847</v>
       </c>
       <c r="D104" t="s">
         <v>145</v>
@@ -12434,18 +12466,18 @@
         <v>170</v>
       </c>
       <c r="F104" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>1844</v>
+        <v>1848</v>
       </c>
       <c r="B105" t="s">
-        <v>1845</v>
+        <v>1849</v>
       </c>
       <c r="C105" t="s">
-        <v>1846</v>
+        <v>1850</v>
       </c>
       <c r="D105" t="s">
         <v>145</v>
@@ -12454,18 +12486,18 @@
         <v>170</v>
       </c>
       <c r="F105" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>1847</v>
+        <v>1851</v>
       </c>
       <c r="B106" t="s">
-        <v>1848</v>
+        <v>1852</v>
       </c>
       <c r="C106" t="s">
-        <v>1849</v>
+        <v>1853</v>
       </c>
       <c r="D106" t="s">
         <v>145</v>
@@ -12474,18 +12506,18 @@
         <v>170</v>
       </c>
       <c r="F106" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>1850</v>
+        <v>1854</v>
       </c>
       <c r="B107" t="s">
-        <v>1851</v>
+        <v>1855</v>
       </c>
       <c r="C107" t="s">
-        <v>1852</v>
+        <v>1856</v>
       </c>
       <c r="D107" t="s">
         <v>145</v>
@@ -12494,18 +12526,18 @@
         <v>170</v>
       </c>
       <c r="F107" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>1853</v>
+        <v>1857</v>
       </c>
       <c r="B108" t="s">
-        <v>1854</v>
+        <v>1858</v>
       </c>
       <c r="C108" t="s">
-        <v>1855</v>
+        <v>1859</v>
       </c>
       <c r="D108" t="s">
         <v>145</v>
@@ -12514,18 +12546,18 @@
         <v>170</v>
       </c>
       <c r="F108" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>1856</v>
+        <v>1860</v>
       </c>
       <c r="B109" t="s">
-        <v>1857</v>
+        <v>1861</v>
       </c>
       <c r="C109" t="s">
-        <v>1858</v>
+        <v>1862</v>
       </c>
       <c r="D109" t="s">
         <v>145</v>
@@ -12534,18 +12566,18 @@
         <v>170</v>
       </c>
       <c r="F109" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>1859</v>
+        <v>1863</v>
       </c>
       <c r="B110" t="s">
-        <v>1860</v>
+        <v>1864</v>
       </c>
       <c r="C110" t="s">
-        <v>1861</v>
+        <v>1865</v>
       </c>
       <c r="D110" t="s">
         <v>145</v>
@@ -12554,18 +12586,18 @@
         <v>170</v>
       </c>
       <c r="F110" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>1862</v>
+        <v>1866</v>
       </c>
       <c r="B111" t="s">
-        <v>1863</v>
+        <v>1867</v>
       </c>
       <c r="C111" t="s">
-        <v>1864</v>
+        <v>1868</v>
       </c>
       <c r="D111" t="s">
         <v>145</v>
@@ -12574,18 +12606,18 @@
         <v>170</v>
       </c>
       <c r="F111" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>1865</v>
+        <v>1869</v>
       </c>
       <c r="B112" t="s">
-        <v>1866</v>
+        <v>1870</v>
       </c>
       <c r="C112" t="s">
-        <v>1867</v>
+        <v>1871</v>
       </c>
       <c r="D112" t="s">
         <v>145</v>
@@ -12594,18 +12626,18 @@
         <v>170</v>
       </c>
       <c r="F112" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>1868</v>
+        <v>1872</v>
       </c>
       <c r="B113" t="s">
-        <v>1869</v>
+        <v>1873</v>
       </c>
       <c r="C113" t="s">
-        <v>1870</v>
+        <v>1874</v>
       </c>
       <c r="D113" t="s">
         <v>145</v>
@@ -12614,18 +12646,18 @@
         <v>170</v>
       </c>
       <c r="F113" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>1871</v>
+        <v>1875</v>
       </c>
       <c r="B114" t="s">
-        <v>1872</v>
+        <v>1876</v>
       </c>
       <c r="C114" t="s">
-        <v>1873</v>
+        <v>1877</v>
       </c>
       <c r="D114" t="s">
         <v>145</v>
@@ -12634,7 +12666,7 @@
         <v>170</v>
       </c>
       <c r="F114" t="s">
-        <v>1558</v>
+        <v>1562</v>
       </c>
     </row>
   </sheetData>
@@ -13489,7 +13521,7 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>1874</v>
+        <v>1878</v>
       </c>
     </row>
   </sheetData>
@@ -41791,19 +41823,19 @@
     </row>
     <row r="528" spans="1:6">
       <c r="A528" t="s">
-        <v>1875</v>
+        <v>1879</v>
       </c>
       <c r="B528" t="s">
-        <v>1876</v>
+        <v>1880</v>
       </c>
       <c r="C528" t="s">
-        <v>1877</v>
+        <v>1881</v>
       </c>
       <c r="D528" t="s">
         <v>118</v>
       </c>
       <c r="E528" t="s">
-        <v>1878</v>
+        <v>1882</v>
       </c>
       <c r="F528" t="s">
         <v>59</v>
@@ -41811,19 +41843,19 @@
     </row>
     <row r="529" spans="1:6">
       <c r="A529" t="s">
-        <v>1879</v>
+        <v>1883</v>
       </c>
       <c r="B529" t="s">
-        <v>1880</v>
+        <v>1884</v>
       </c>
       <c r="C529" t="s">
-        <v>1881</v>
+        <v>1885</v>
       </c>
       <c r="D529" t="s">
         <v>118</v>
       </c>
       <c r="E529" t="s">
-        <v>1878</v>
+        <v>1882</v>
       </c>
       <c r="F529" t="s">
         <v>59</v>
@@ -41831,19 +41863,19 @@
     </row>
     <row r="530" spans="1:6">
       <c r="A530" t="s">
-        <v>1882</v>
+        <v>1886</v>
       </c>
       <c r="B530" t="s">
-        <v>1883</v>
+        <v>1887</v>
       </c>
       <c r="C530" t="s">
-        <v>1884</v>
+        <v>1888</v>
       </c>
       <c r="D530" t="s">
         <v>118</v>
       </c>
       <c r="E530" t="s">
-        <v>1878</v>
+        <v>1882</v>
       </c>
       <c r="F530" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Fix permission not synced
</commit_message>
<xml_diff>
--- a/apps/core/fixtures/core_permission.xlsx
+++ b/apps/core/fixtures/core_permission.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16260" tabRatio="894" activeTab="8"/>
+    <workbookView windowHeight="15300" tabRatio="894" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="core_permission" sheetId="1" r:id="rId1"/>
@@ -6142,49 +6142,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -6422,7 +6385,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
@@ -6434,34 +6397,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="16">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="13">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="17">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="16">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="13">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="18">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="15">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0">
@@ -6546,7 +6509,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -6566,49 +6529,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -7132,7 +7086,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="S_NV_CHUNG" displayName="S_NV_CHUNG" ref="A1:F107" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F107" etc:filterBottomFollowUsedRange="0"/>
-  <sortState ref="A2:F107">
+  <sortState ref="A1:F107">
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="6">
@@ -7546,121 +7500,121 @@
       </c>
     </row>
     <row r="2" ht="17" spans="1:5">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" ht="17" spans="1:5">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="15" t="s">
         <v>29</v>
       </c>
     </row>
@@ -9017,7 +8971,6 @@
     <row r="10" spans="1:5">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
     </row>
@@ -9104,7 +9057,6 @@
     <row r="15" spans="1:5">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
     </row>
@@ -9151,7 +9103,6 @@
     <row r="18" spans="1:5">
       <c r="A18"/>
       <c r="B18"/>
-      <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
     </row>
@@ -9183,7 +9134,6 @@
     <row r="21" spans="1:5">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
     </row>
@@ -9270,7 +9220,6 @@
     <row r="26" spans="1:5">
       <c r="A26"/>
       <c r="B26"/>
-      <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
     </row>
@@ -9317,7 +9266,6 @@
     <row r="29" spans="1:5">
       <c r="A29"/>
       <c r="B29"/>
-      <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
     </row>
@@ -9349,7 +9297,6 @@
     <row r="32" spans="1:5">
       <c r="A32"/>
       <c r="B32"/>
-      <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
     </row>
@@ -9436,7 +9383,6 @@
     <row r="37" spans="1:5">
       <c r="A37"/>
       <c r="B37"/>
-      <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
     </row>
@@ -9483,7 +9429,6 @@
     <row r="40" spans="1:5">
       <c r="A40"/>
       <c r="B40"/>
-      <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
     </row>
@@ -9515,7 +9460,6 @@
     <row r="43" spans="1:5">
       <c r="A43"/>
       <c r="B43"/>
-      <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
     </row>
@@ -9602,7 +9546,6 @@
     <row r="48" spans="1:5">
       <c r="A48"/>
       <c r="B48"/>
-      <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
     </row>
@@ -9649,7 +9592,6 @@
     <row r="51" spans="1:5">
       <c r="A51"/>
       <c r="B51"/>
-      <c r="C51"/>
       <c r="D51"/>
       <c r="E51"/>
     </row>
@@ -9681,7 +9623,6 @@
     <row r="54" spans="1:5">
       <c r="A54"/>
       <c r="B54"/>
-      <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
     </row>
@@ -9768,7 +9709,6 @@
     <row r="59" spans="1:5">
       <c r="A59"/>
       <c r="B59"/>
-      <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
     </row>
@@ -9815,7 +9755,6 @@
     <row r="62" spans="1:5">
       <c r="A62"/>
       <c r="B62"/>
-      <c r="C62"/>
       <c r="D62"/>
       <c r="E62"/>
     </row>
@@ -9847,7 +9786,6 @@
     <row r="65" spans="1:5">
       <c r="A65"/>
       <c r="B65"/>
-      <c r="C65"/>
       <c r="D65"/>
       <c r="E65"/>
     </row>
@@ -9934,7 +9872,6 @@
     <row r="70" spans="1:5">
       <c r="A70"/>
       <c r="B70"/>
-      <c r="C70"/>
       <c r="D70"/>
       <c r="E70"/>
     </row>
@@ -9981,7 +9918,6 @@
     <row r="73" spans="1:5">
       <c r="A73"/>
       <c r="B73"/>
-      <c r="C73"/>
       <c r="D73"/>
       <c r="E73"/>
     </row>
@@ -10008,7 +9944,6 @@
     <row r="76" spans="1:5">
       <c r="A76"/>
       <c r="B76"/>
-      <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
     </row>
@@ -10095,7 +10030,6 @@
     <row r="81" spans="1:5">
       <c r="A81"/>
       <c r="B81"/>
-      <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
     </row>
@@ -10142,7 +10076,6 @@
     <row r="84" spans="1:5">
       <c r="A84"/>
       <c r="B84"/>
-      <c r="C84"/>
       <c r="D84"/>
       <c r="E84"/>
     </row>
@@ -10169,7 +10102,6 @@
     <row r="86" spans="1:5">
       <c r="A86"/>
       <c r="B86"/>
-      <c r="C86"/>
       <c r="D86"/>
       <c r="E86"/>
     </row>
@@ -10256,7 +10188,6 @@
     <row r="91" spans="1:5">
       <c r="A91"/>
       <c r="B91"/>
-      <c r="C91"/>
       <c r="D91"/>
       <c r="E91"/>
     </row>
@@ -10303,7 +10234,6 @@
     <row r="94" spans="1:5">
       <c r="A94"/>
       <c r="B94"/>
-      <c r="C94"/>
       <c r="D94"/>
       <c r="E94"/>
     </row>
@@ -10330,7 +10260,6 @@
     <row r="96" spans="1:5">
       <c r="A96"/>
       <c r="B96"/>
-      <c r="C96"/>
       <c r="D96"/>
       <c r="E96"/>
     </row>
@@ -10417,7 +10346,6 @@
     <row r="101" spans="1:5">
       <c r="A101"/>
       <c r="B101"/>
-      <c r="C101"/>
       <c r="D101"/>
       <c r="E101"/>
     </row>
@@ -10464,7 +10392,6 @@
     <row r="104" spans="1:5">
       <c r="A104"/>
       <c r="B104"/>
-      <c r="C104"/>
       <c r="D104"/>
       <c r="E104"/>
     </row>
@@ -10491,7 +10418,6 @@
     <row r="106" spans="1:5">
       <c r="A106"/>
       <c r="B106"/>
-      <c r="C106"/>
       <c r="D106"/>
       <c r="E106"/>
     </row>
@@ -10578,7 +10504,6 @@
     <row r="111" spans="1:5">
       <c r="A111"/>
       <c r="B111"/>
-      <c r="C111"/>
       <c r="D111"/>
       <c r="E111"/>
     </row>
@@ -10625,7 +10550,6 @@
     <row r="114" spans="1:5">
       <c r="A114"/>
       <c r="B114"/>
-      <c r="C114"/>
       <c r="D114"/>
       <c r="E114"/>
     </row>
@@ -34467,10 +34391,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:F110"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -36631,56 +36555,26 @@
       <c r="B109"/>
       <c r="C109"/>
     </row>
-    <row r="110" spans="1:6">
-      <c r="A110" t="str">
-        <f t="array" ref="A110:F147">S_TRUONGPHONG[]</f>
+    <row r="110" spans="1:3">
+      <c r="A110"/>
+      <c r="B110"/>
+      <c r="C110"/>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111"/>
+      <c r="B111"/>
+      <c r="C111"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="str" cm="1">
+        <f t="array" ref="A112:F153">S_TRUONGPHONG[]</f>
         <v>recruitment_request.create</v>
       </c>
-      <c r="B110" t="str">
+      <c r="B112" t="str">
         <v>[HCNS] [Tuyển dụng] Quyền tạo Phiếu yêu cầu tuyển dụng</v>
       </c>
-      <c r="C110" t="str">
+      <c r="C112" t="str">
         <v>Quyền tạo mới một Phiếu yêu cầu tuyển dụng</v>
-      </c>
-      <c r="D110" t="str">
-        <v>HCNS</v>
-      </c>
-      <c r="E110" t="str">
-        <v>Tuyển dụng</v>
-      </c>
-      <c r="F110" t="str">
-        <v>S_TRUONGPHONG</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" t="str">
-        <v>recruitment_request.destroy</v>
-      </c>
-      <c r="B111" t="str">
-        <v>[HCNS] [Tuyển dụng] Quyền xóa Phiếu yêu cầu tuyển dụng</v>
-      </c>
-      <c r="C111" t="str">
-        <v>Quyền xóa Phiếu yêu cầu tuyển dụng</v>
-      </c>
-      <c r="D111" t="str">
-        <v>HCNS</v>
-      </c>
-      <c r="E111" t="str">
-        <v>Tuyển dụng</v>
-      </c>
-      <c r="F111" t="str">
-        <v>S_TRUONGPHONG</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112" t="str">
-        <v>recruitment_request.export_detail_document</v>
-      </c>
-      <c r="B112" t="str">
-        <v>[HCNS] [Tuyển dụng] UNREGISTERED Export Detail Document Phiếu yêu cầu tuyển dụng</v>
-      </c>
-      <c r="C112" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Export Detail Document a Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D112" t="str">
         <v>HCNS</v>
@@ -36694,13 +36588,13 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="str">
-        <v>recruitment_request.histories</v>
+        <v>recruitment_request.destroy</v>
       </c>
       <c r="B113" t="str">
-        <v>[HCNS] [Tuyển dụng] Xem lịch sử Phiếu yêu cầu tuyển dụng</v>
+        <v>[HCNS] [Tuyển dụng] Quyền xóa Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="C113" t="str">
-        <v>Xem lịch sử Phiếu yêu cầu tuyển dụng</v>
+        <v>Quyền xóa Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D113" t="str">
         <v>HCNS</v>
@@ -36714,13 +36608,13 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="str">
-        <v>recruitment_request.history_detail</v>
+        <v>recruitment_request.export_detail_document</v>
       </c>
       <c r="B114" t="str">
-        <v>[HCNS] [Tuyển dụng] Xem chi tiết lịch sử của Phiếu yêu cầu tuyển dụng</v>
+        <v>[HCNS] [Tuyển dụng] UNREGISTERED Export Detail Document Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="C114" t="str">
-        <v>Xem chi tiết lịch sử của Phiếu yêu cầu tuyển dụng</v>
+        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Export Detail Document a Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D114" t="str">
         <v>HCNS</v>
@@ -36734,13 +36628,13 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="str">
-        <v>recruitment_request.list</v>
+        <v>recruitment_request.histories</v>
       </c>
       <c r="B115" t="str">
-        <v>[HCNS] [Tuyển dụng] Danh sách Phiếu Yêu Cầu Tuyển Dụng</v>
+        <v>[HCNS] [Tuyển dụng] Xem lịch sử Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="C115" t="str">
-        <v>Xem danh sách Phiếu Yêu Cầu Tuyển Dụng</v>
+        <v>Xem lịch sử Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D115" t="str">
         <v>HCNS</v>
@@ -36754,13 +36648,13 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="str">
-        <v>recruitment_request.partial_update</v>
+        <v>recruitment_request.history_detail</v>
       </c>
       <c r="B116" t="str">
-        <v>[HCNS] [Tuyển dụng] Quyền cập nhật một phần Phiếu yêu cầu tuyển dụng</v>
+        <v>[HCNS] [Tuyển dụng] Xem chi tiết lịch sử của Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="C116" t="str">
-        <v>Quyền cập nhật một phần Phiếu yêu cầu tuyển dụng</v>
+        <v>Xem chi tiết lịch sử của Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D116" t="str">
         <v>HCNS</v>
@@ -36774,13 +36668,13 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="str">
-        <v>recruitment_request.retrieve</v>
+        <v>recruitment_request.list</v>
       </c>
       <c r="B117" t="str">
-        <v>[HCNS] [Tuyển dụng] Xem Phiếu yêu cầu tuyển dụng</v>
+        <v>[HCNS] [Tuyển dụng] Danh sách Phiếu Yêu Cầu Tuyển Dụng</v>
       </c>
       <c r="C117" t="str">
-        <v>Xem chi tiết của Phiếu yêu cầu tuyển dụng</v>
+        <v>Xem danh sách Phiếu Yêu Cầu Tuyển Dụng</v>
       </c>
       <c r="D117" t="str">
         <v>HCNS</v>
@@ -36794,19 +36688,19 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="str">
-        <v>proposal_verifier.histories</v>
+        <v>recruitment_request.partial_update</v>
       </c>
       <c r="B118" t="str">
-        <v>[HRM] [Đề xuất] Xem lịch sử Người xác minh</v>
+        <v>[HCNS] [Tuyển dụng] Quyền cập nhật một phần Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="C118" t="str">
-        <v>Xem lịch sử Người xác minh</v>
+        <v>Quyền cập nhật một phần Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D118" t="str">
-        <v>HRM</v>
+        <v>HCNS</v>
       </c>
       <c r="E118" t="str">
-        <v>Đề xuất</v>
+        <v>Tuyển dụng</v>
       </c>
       <c r="F118" t="str">
         <v>S_TRUONGPHONG</v>
@@ -36814,19 +36708,19 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="str">
-        <v>proposal_verifier.history_detail</v>
+        <v>recruitment_request.retrieve</v>
       </c>
       <c r="B119" t="str">
-        <v>[HRM] [Đề xuất] Xem chi tiết lịch sử của Người xác minh</v>
+        <v>[HCNS] [Tuyển dụng] Xem Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="C119" t="str">
-        <v>Xem chi tiết lịch sử của Người xác minh</v>
+        <v>Xem chi tiết của Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D119" t="str">
-        <v>HRM</v>
+        <v>HCNS</v>
       </c>
       <c r="E119" t="str">
-        <v>Đề xuất</v>
+        <v>Tuyển dụng</v>
       </c>
       <c r="F119" t="str">
         <v>S_TRUONGPHONG</v>
@@ -36834,13 +36728,13 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="str">
-        <v>proposal_verifier.mine</v>
+        <v>proposal_verifier.histories</v>
       </c>
       <c r="B120" t="str">
-        <v>[HRM] [Đề xuất] UNREGISTERED Mine Người xác minh</v>
+        <v>[HRM] [Đề xuất] Xem lịch sử Người xác minh</v>
       </c>
       <c r="C120" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Mine a Người xác minh</v>
+        <v>Xem lịch sử Người xác minh</v>
       </c>
       <c r="D120" t="str">
         <v>HRM</v>
@@ -36854,13 +36748,13 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="str">
-        <v>proposal_verifier.reject</v>
+        <v>proposal_verifier.history_detail</v>
       </c>
       <c r="B121" t="str">
-        <v>[HRM] [Đề xuất] UNREGISTERED Reject Người xác minh</v>
+        <v>[HRM] [Đề xuất] Xem chi tiết lịch sử của Người xác minh</v>
       </c>
       <c r="C121" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Reject a Người xác minh</v>
+        <v>Xem chi tiết lịch sử của Người xác minh</v>
       </c>
       <c r="D121" t="str">
         <v>HRM</v>
@@ -36874,13 +36768,13 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="str">
-        <v>proposal_verifier.retrieve</v>
+        <v>proposal_verifier.mine</v>
       </c>
       <c r="B122" t="str">
-        <v>[HRM] [Đề xuất] Xem Người xác minh</v>
+        <v>[HRM] [Đề xuất] UNREGISTERED Mine Người xác minh</v>
       </c>
       <c r="C122" t="str">
-        <v>Xem chi tiết của Người xác minh</v>
+        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Mine a Người xác minh</v>
       </c>
       <c r="D122" t="str">
         <v>HRM</v>
@@ -36894,13 +36788,13 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="str">
-        <v>proposal_verifier.verify</v>
+        <v>proposal_verifier.reject</v>
       </c>
       <c r="B123" t="str">
-        <v>[HRM] [Đề xuất] UNREGISTERED Verify Người xác minh</v>
+        <v>[HRM] [Đề xuất] UNREGISTERED Reject Người xác minh</v>
       </c>
       <c r="C123" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Verify a Người xác minh</v>
+        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Reject a Người xác minh</v>
       </c>
       <c r="D123" t="str">
         <v>HRM</v>
@@ -36914,19 +36808,19 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="str">
-        <v>recruitment_request.update</v>
+        <v>proposal_verifier.retrieve</v>
       </c>
       <c r="B124" t="str">
-        <v>[HCNS] [Tuyển dụng] Quyền cập nhật Phiếu yêu cầu tuyển dụng</v>
+        <v>[HRM] [Đề xuất] Xem Người xác minh</v>
       </c>
       <c r="C124" t="str">
-        <v>Quyền cập nhật Phiếu yêu cầu tuyển dụng</v>
+        <v>Xem chi tiết của Người xác minh</v>
       </c>
       <c r="D124" t="str">
-        <v>HCNS</v>
+        <v>HRM</v>
       </c>
       <c r="E124" t="str">
-        <v>Tuyển dụng</v>
+        <v>Đề xuất</v>
       </c>
       <c r="F124" t="str">
         <v>S_TRUONGPHONG</v>
@@ -36934,19 +36828,19 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="str">
-        <v>department_kpi_assessment.list</v>
+        <v>proposal_verifier.verify</v>
       </c>
       <c r="B125" t="str">
-        <v>[Payroll] [KPI Management] Danh sách Department Kpi Assessments</v>
+        <v>[HRM] [Đề xuất] UNREGISTERED Verify Người xác minh</v>
       </c>
       <c r="C125" t="str">
-        <v>Xem danh sách Department Kpi Assessments</v>
+        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Verify a Người xác minh</v>
       </c>
       <c r="D125" t="str">
-        <v>Payroll</v>
+        <v>HRM</v>
       </c>
       <c r="E125" t="str">
-        <v>KPI Management</v>
+        <v>Đề xuất</v>
       </c>
       <c r="F125" t="str">
         <v>S_TRUONGPHONG</v>
@@ -36954,19 +36848,19 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="str">
-        <v>department_kpi_assessment.retrieve</v>
+        <v>recruitment_request.update</v>
       </c>
       <c r="B126" t="str">
-        <v>[Payroll] [KPI Management] Xem Department KPI Assessment</v>
+        <v>[HCNS] [Tuyển dụng] Quyền cập nhật Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="C126" t="str">
-        <v>Xem chi tiết của Department KPI Assessment</v>
+        <v>Quyền cập nhật Phiếu yêu cầu tuyển dụng</v>
       </c>
       <c r="D126" t="str">
-        <v>Payroll</v>
+        <v>HCNS</v>
       </c>
       <c r="E126" t="str">
-        <v>KPI Management</v>
+        <v>Tuyển dụng</v>
       </c>
       <c r="F126" t="str">
         <v>S_TRUONGPHONG</v>
@@ -36974,13 +36868,13 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="str">
-        <v>employee_kpi_assessment.histories</v>
+        <v>department_kpi_assessment.list</v>
       </c>
       <c r="B127" t="str">
-        <v>[Payroll] [KPI Management] Xem lịch sử Employee KPI Assessment</v>
+        <v>[Payroll] [KPI Management] Danh sách Department Kpi Assessments</v>
       </c>
       <c r="C127" t="str">
-        <v>Xem lịch sử Employee KPI Assessment</v>
+        <v>Xem danh sách Department Kpi Assessments</v>
       </c>
       <c r="D127" t="str">
         <v>Payroll</v>
@@ -36994,13 +36888,13 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="str">
-        <v>employee_kpi_assessment.history_detail</v>
+        <v>department_kpi_assessment.retrieve</v>
       </c>
       <c r="B128" t="str">
-        <v>[Payroll] [KPI Management] Xem chi tiết lịch sử của Employee KPI Assessment</v>
+        <v>[Payroll] [KPI Management] Xem Department KPI Assessment</v>
       </c>
       <c r="C128" t="str">
-        <v>Xem chi tiết lịch sử của Employee KPI Assessment</v>
+        <v>Xem chi tiết của Department KPI Assessment</v>
       </c>
       <c r="D128" t="str">
         <v>Payroll</v>
@@ -37014,13 +36908,13 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="str">
-        <v>employee_kpi_assessment.list</v>
+        <v>employee_kpi_assessment.histories</v>
       </c>
       <c r="B129" t="str">
-        <v>[Payroll] [KPI Management] Danh sách Employee Kpi Assessments</v>
+        <v>[Payroll] [KPI Management] Xem lịch sử Employee KPI Assessment</v>
       </c>
       <c r="C129" t="str">
-        <v>Xem danh sách Employee Kpi Assessments</v>
+        <v>Xem lịch sử Employee KPI Assessment</v>
       </c>
       <c r="D129" t="str">
         <v>Payroll</v>
@@ -37034,13 +36928,13 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="str">
-        <v>employee_kpi_assessment.partial_update</v>
+        <v>employee_kpi_assessment.history_detail</v>
       </c>
       <c r="B130" t="str">
-        <v>[Payroll] [KPI Management] Quyền cập nhật một phần Employee KPI Assessment</v>
+        <v>[Payroll] [KPI Management] Xem chi tiết lịch sử của Employee KPI Assessment</v>
       </c>
       <c r="C130" t="str">
-        <v>Quyền cập nhật một phần Employee KPI Assessment</v>
+        <v>Xem chi tiết lịch sử của Employee KPI Assessment</v>
       </c>
       <c r="D130" t="str">
         <v>Payroll</v>
@@ -37054,13 +36948,13 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="str">
-        <v>employee_kpi_assessment.retrieve</v>
+        <v>employee_kpi_assessment.list</v>
       </c>
       <c r="B131" t="str">
-        <v>[Payroll] [KPI Management] Xem Employee KPI Assessment</v>
+        <v>[Payroll] [KPI Management] Danh sách Employee Kpi Assessments</v>
       </c>
       <c r="C131" t="str">
-        <v>Xem chi tiết của Employee KPI Assessment</v>
+        <v>Xem danh sách Employee Kpi Assessments</v>
       </c>
       <c r="D131" t="str">
         <v>Payroll</v>
@@ -37074,13 +36968,13 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="str">
-        <v>employee_kpi_assessment.update</v>
+        <v>employee_kpi_assessment.partial_update</v>
       </c>
       <c r="B132" t="str">
-        <v>[Payroll] [KPI Management] Quyền cập nhật Employee KPI Assessment</v>
+        <v>[Payroll] [KPI Management] Quyền cập nhật một phần Employee KPI Assessment</v>
       </c>
       <c r="C132" t="str">
-        <v>Quyền cập nhật Employee KPI Assessment</v>
+        <v>Quyền cập nhật một phần Employee KPI Assessment</v>
       </c>
       <c r="D132" t="str">
         <v>Payroll</v>
@@ -37094,19 +36988,19 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="str">
-        <v>employee_manager_assessment.list</v>
+        <v>employee_kpi_assessment.retrieve</v>
       </c>
       <c r="B133" t="str">
-        <v>[Payroll] [Manager Assessment] Danh sách ManagerAssessments</v>
+        <v>[Payroll] [KPI Management] Xem Employee KPI Assessment</v>
       </c>
       <c r="C133" t="str">
-        <v>Xem danh sách ManagerAssessments</v>
+        <v>Xem chi tiết của Employee KPI Assessment</v>
       </c>
       <c r="D133" t="str">
         <v>Payroll</v>
       </c>
       <c r="E133" t="str">
-        <v>Manager Assessment</v>
+        <v>KPI Management</v>
       </c>
       <c r="F133" t="str">
         <v>S_TRUONGPHONG</v>
@@ -37114,19 +37008,19 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="str">
-        <v>employee_self_assessment.list</v>
+        <v>employee_kpi_assessment.update</v>
       </c>
       <c r="B134" t="str">
-        <v>[Payroll] [Employee Self-Assessment] Danh sách EmployeeSelfAssessments</v>
+        <v>[Payroll] [KPI Management] Quyền cập nhật Employee KPI Assessment</v>
       </c>
       <c r="C134" t="str">
-        <v>Xem danh sách EmployeeSelfAssessments</v>
+        <v>Quyền cập nhật Employee KPI Assessment</v>
       </c>
       <c r="D134" t="str">
         <v>Payroll</v>
       </c>
       <c r="E134" t="str">
-        <v>Employee Self-Assessment</v>
+        <v>KPI Management</v>
       </c>
       <c r="F134" t="str">
         <v>S_TRUONGPHONG</v>
@@ -37134,13 +37028,13 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="str">
-        <v>employee_manager_assessment.partial_update</v>
+        <v>employee_manager_assessment.list</v>
       </c>
       <c r="B135" t="str">
-        <v>[Payroll] [Manager Assessment] Quyền cập nhật một phần ManagerAssessment</v>
+        <v>[Payroll] [Manager Assessment] Danh sách ManagerAssessments</v>
       </c>
       <c r="C135" t="str">
-        <v>Quyền cập nhật một phần ManagerAssessment</v>
+        <v>Xem danh sách ManagerAssessments</v>
       </c>
       <c r="D135" t="str">
         <v>Payroll</v>
@@ -37154,19 +37048,19 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="str">
-        <v>employee_manager_assessment.retrieve</v>
+        <v>employee_self_assessment.list</v>
       </c>
       <c r="B136" t="str">
-        <v>[Payroll] [Manager Assessment] Xem ManagerAssessment</v>
+        <v>[Payroll] [Employee Self-Assessment] Danh sách EmployeeSelfAssessments</v>
       </c>
       <c r="C136" t="str">
-        <v>Xem chi tiết của ManagerAssessment</v>
+        <v>Xem danh sách EmployeeSelfAssessments</v>
       </c>
       <c r="D136" t="str">
         <v>Payroll</v>
       </c>
       <c r="E136" t="str">
-        <v>Manager Assessment</v>
+        <v>Employee Self-Assessment</v>
       </c>
       <c r="F136" t="str">
         <v>S_TRUONGPHONG</v>
@@ -37174,13 +37068,13 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="str">
-        <v>employee_manager_assessment.current_assessments</v>
+        <v>employee_manager_assessment.partial_update</v>
       </c>
       <c r="B137" t="str">
-        <v>[Payroll] [Manager Assessment] UNREGISTERED Current Assessments ManagerAssessment</v>
+        <v>[Payroll] [Manager Assessment] Quyền cập nhật một phần ManagerAssessment</v>
       </c>
       <c r="C137" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Current Assessments a ManagerAssessment</v>
+        <v>Quyền cập nhật một phần ManagerAssessment</v>
       </c>
       <c r="D137" t="str">
         <v>Payroll</v>
@@ -37214,13 +37108,13 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="str">
-        <v>employee_manager_assessment.create</v>
+        <v>employee_manager_assessment.current_assessments</v>
       </c>
       <c r="B139" t="str">
-        <v>[Payroll] [Manager Assessment] Quyền tạo ManagerAssessment</v>
+        <v>[Payroll] [Manager Assessment] UNREGISTERED Current Assessments ManagerAssessment</v>
       </c>
       <c r="C139" t="str">
-        <v>Quyền tạo mới một ManagerAssessment</v>
+        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Current Assessments a ManagerAssessment</v>
       </c>
       <c r="D139" t="str">
         <v>Payroll</v>
@@ -37234,13 +37128,13 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="str">
-        <v>employee_manager_assessment.destroy</v>
+        <v>employee_manager_assessment.retrieve</v>
       </c>
       <c r="B140" t="str">
-        <v>[Payroll] [Manager Assessment] Quyền xóa ManagerAssessment</v>
+        <v>[Payroll] [Manager Assessment] Xem ManagerAssessment</v>
       </c>
       <c r="C140" t="str">
-        <v>Quyền xóa ManagerAssessment</v>
+        <v>Xem chi tiết của ManagerAssessment</v>
       </c>
       <c r="D140" t="str">
         <v>Payroll</v>
@@ -37254,13 +37148,13 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="str">
-        <v>employee_manager_assessment.list</v>
+        <v>employee_manager_assessment.create</v>
       </c>
       <c r="B141" t="str">
-        <v>[Payroll] [Manager Assessment] Danh sách ManagerAssessments</v>
+        <v>[Payroll] [Manager Assessment] Quyền tạo ManagerAssessment</v>
       </c>
       <c r="C141" t="str">
-        <v>Xem danh sách ManagerAssessments</v>
+        <v>Quyền tạo mới một ManagerAssessment</v>
       </c>
       <c r="D141" t="str">
         <v>Payroll</v>
@@ -37274,13 +37168,13 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="str">
-        <v>employee_manager_assessment.partial_update</v>
+        <v>employee_manager_assessment.destroy</v>
       </c>
       <c r="B142" t="str">
-        <v>[Payroll] [Manager Assessment] Quyền cập nhật một phần ManagerAssessment</v>
+        <v>[Payroll] [Manager Assessment] Quyền xóa ManagerAssessment</v>
       </c>
       <c r="C142" t="str">
-        <v>Quyền cập nhật một phần ManagerAssessment</v>
+        <v>Quyền xóa ManagerAssessment</v>
       </c>
       <c r="D142" t="str">
         <v>Payroll</v>
@@ -37294,13 +37188,13 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="str">
-        <v>employee_manager_assessment.update</v>
+        <v>employee_manager_assessment.list</v>
       </c>
       <c r="B143" t="str">
-        <v>[Payroll] [Manager Assessment] Quyền cập nhật ManagerAssessment</v>
+        <v>[Payroll] [Manager Assessment] Danh sách ManagerAssessments</v>
       </c>
       <c r="C143" t="str">
-        <v>Quyền cập nhật ManagerAssessment</v>
+        <v>Xem danh sách ManagerAssessments</v>
       </c>
       <c r="D143" t="str">
         <v>Payroll</v>
@@ -37314,19 +37208,19 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="str">
-        <v>hrm.dashboard.manager.realtime</v>
+        <v>employee_manager_assessment.partial_update</v>
       </c>
       <c r="B144" t="str">
-        <v>[HCNS] [Manager Dashboard] Xem thống kê các vấn đề HCNS cần xử lý</v>
+        <v>[Payroll] [Manager Assessment] Quyền cập nhật một phần ManagerAssessment</v>
       </c>
       <c r="C144" t="str">
-        <v>Xem thống kê các đề xuất cần xác nhận và đánh giá KPI</v>
+        <v>Quyền cập nhật một phần ManagerAssessment</v>
       </c>
       <c r="D144" t="str">
-        <v>HCNS</v>
+        <v>Payroll</v>
       </c>
       <c r="E144" t="str">
-        <v>Manager Dashboard</v>
+        <v>Manager Assessment</v>
       </c>
       <c r="F144" t="str">
         <v>S_TRUONGPHONG</v>
@@ -37334,19 +37228,19 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="str">
-        <v>my_team_kpi_assessment.create</v>
+        <v>employee_manager_assessment.update</v>
       </c>
       <c r="B145" t="str">
-        <v>[Phiếu lương] [Team KPI] Quyền tạo Employee KPI Assessment</v>
+        <v>[Payroll] [Manager Assessment] Quyền cập nhật ManagerAssessment</v>
       </c>
       <c r="C145" t="str">
-        <v>Quyền tạo mới một Employee KPI Assessment</v>
+        <v>Quyền cập nhật ManagerAssessment</v>
       </c>
       <c r="D145" t="str">
-        <v>Phiếu lương</v>
+        <v>Payroll</v>
       </c>
       <c r="E145" t="str">
-        <v>Team KPI</v>
+        <v>Manager Assessment</v>
       </c>
       <c r="F145" t="str">
         <v>S_TRUONGPHONG</v>
@@ -37354,19 +37248,19 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="str">
-        <v>my_team_kpi_assessment.current</v>
+        <v>hrm.dashboard.manager.realtime</v>
       </c>
       <c r="B146" t="str">
-        <v>[Phiếu lương] [Team KPI] UNREGISTERED Current Employee KPI Assessment</v>
+        <v>[HCNS] [Manager Dashboard] Xem thống kê các vấn đề HCNS cần xử lý</v>
       </c>
       <c r="C146" t="str">
-        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Current a Employee KPI Assessment</v>
+        <v>Xem thống kê các đề xuất cần xác nhận và đánh giá KPI</v>
       </c>
       <c r="D146" t="str">
-        <v>Phiếu lương</v>
+        <v>HCNS</v>
       </c>
       <c r="E146" t="str">
-        <v>Team KPI</v>
+        <v>Manager Dashboard</v>
       </c>
       <c r="F146" t="str">
         <v>S_TRUONGPHONG</v>
@@ -37374,13 +37268,13 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="str">
-        <v>my_team_kpi_assessment.destroy</v>
+        <v>my_team_kpi_assessment.create</v>
       </c>
       <c r="B147" t="str">
-        <v>[Phiếu lương] [Team KPI] Quyền xóa Employee KPI Assessment</v>
+        <v>[Phiếu lương] [Team KPI] Quyền tạo Employee KPI Assessment</v>
       </c>
       <c r="C147" t="str">
-        <v>Quyền xóa Employee KPI Assessment</v>
+        <v>Quyền tạo mới một Employee KPI Assessment</v>
       </c>
       <c r="D147" t="str">
         <v>Phiếu lương</v>
@@ -37389,6 +37283,126 @@
         <v>Team KPI</v>
       </c>
       <c r="F147" t="str">
+        <v>S_TRUONGPHONG</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="1" t="str">
+        <v>my_team_kpi_assessment.current</v>
+      </c>
+      <c r="B148" s="1" t="str">
+        <v>[Phiếu lương] [Team KPI] UNREGISTERED Current Employee KPI Assessment</v>
+      </c>
+      <c r="C148" s="1" t="str">
+        <v>You need to add this action to PERMISSION_REGISTERED_ACTIONS to it's View Current a Employee KPI Assessment</v>
+      </c>
+      <c r="D148" t="str">
+        <v>Phiếu lương</v>
+      </c>
+      <c r="E148" t="str">
+        <v>Team KPI</v>
+      </c>
+      <c r="F148" t="str">
+        <v>S_TRUONGPHONG</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="1" t="str">
+        <v>my_team_kpi_assessment.destroy</v>
+      </c>
+      <c r="B149" s="1" t="str">
+        <v>[Phiếu lương] [Team KPI] Quyền xóa Employee KPI Assessment</v>
+      </c>
+      <c r="C149" s="1" t="str">
+        <v>Quyền xóa Employee KPI Assessment</v>
+      </c>
+      <c r="D149" t="str">
+        <v>Phiếu lương</v>
+      </c>
+      <c r="E149" t="str">
+        <v>Team KPI</v>
+      </c>
+      <c r="F149" t="str">
+        <v>S_TRUONGPHONG</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="1" t="str">
+        <v>my_team_kpi_assessment.list</v>
+      </c>
+      <c r="B150" s="1" t="str">
+        <v>[Phiếu lương] [Team KPI] Danh sách Employee Kpi Assessments</v>
+      </c>
+      <c r="C150" s="1" t="str">
+        <v>Xem danh sách Employee Kpi Assessments</v>
+      </c>
+      <c r="D150" t="str">
+        <v>Phiếu lương</v>
+      </c>
+      <c r="E150" t="str">
+        <v>Team KPI</v>
+      </c>
+      <c r="F150" t="str">
+        <v>S_TRUONGPHONG</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="1" t="str">
+        <v>my_team_kpi_assessment.partial_update</v>
+      </c>
+      <c r="B151" s="1" t="str">
+        <v>[Phiếu lương] [Team KPI] Quyền cập nhật một phần Employee KPI Assessment</v>
+      </c>
+      <c r="C151" s="1" t="str">
+        <v>Quyền cập nhật một phần Employee KPI Assessment</v>
+      </c>
+      <c r="D151" t="str">
+        <v>Phiếu lương</v>
+      </c>
+      <c r="E151" t="str">
+        <v>Team KPI</v>
+      </c>
+      <c r="F151" t="str">
+        <v>S_TRUONGPHONG</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="1" t="str">
+        <v>my_team_kpi_assessment.retrieve</v>
+      </c>
+      <c r="B152" s="1" t="str">
+        <v>[Phiếu lương] [Team KPI] Xem Employee KPI Assessment</v>
+      </c>
+      <c r="C152" s="1" t="str">
+        <v>Xem chi tiết của Employee KPI Assessment</v>
+      </c>
+      <c r="D152" t="str">
+        <v>Phiếu lương</v>
+      </c>
+      <c r="E152" t="str">
+        <v>Team KPI</v>
+      </c>
+      <c r="F152" t="str">
+        <v>S_TRUONGPHONG</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="1" t="str">
+        <v>my_team_kpi_assessment.update</v>
+      </c>
+      <c r="B153" s="1" t="str">
+        <v>[Phiếu lương] [Team KPI] Quyền cập nhật Employee KPI Assessment</v>
+      </c>
+      <c r="C153" s="1" t="str">
+        <v>Quyền cập nhật Employee KPI Assessment</v>
+      </c>
+      <c r="D153" t="str">
+        <v>Phiếu lương</v>
+      </c>
+      <c r="E153" t="str">
+        <v>Team KPI</v>
+      </c>
+      <c r="F153" t="str">
         <v>S_TRUONGPHONG</v>
       </c>
     </row>
@@ -48826,10 +48840,10 @@
       <c r="A12" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>107</v>
       </c>
       <c r="D12" t="s">
@@ -48843,7 +48857,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B13" t="s">
@@ -58337,19 +58351,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -59098,8 +59112,8 @@
   <sheetPr/>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Add more fields to proposal serializer (#688)
Co-authored-by: Cong Khoa <khoabk.nc@gmail.com>
</commit_message>
<xml_diff>
--- a/apps/core/fixtures/core_permission.xlsx
+++ b/apps/core/fixtures/core_permission.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16260" tabRatio="894" firstSheet="13" activeTab="17"/>
+    <workbookView windowHeight="15300" tabRatio="894" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="core_permission" sheetId="1" r:id="rId1"/>
@@ -8001,7 +8001,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -8750,7 +8750,7 @@
         <v>29</v>
       </c>
       <c r="F37" t="s">
-        <v>59</v>
+        <v>1562</v>
       </c>
     </row>
   </sheetData>
@@ -8768,7 +8768,7 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="A70" sqref="A70:F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -10354,7 +10354,7 @@
   <sheetPr/>
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A83" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -12460,7 +12460,7 @@
   <sheetPr/>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
@@ -14553,7 +14553,6 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105"/>
-      <c r="B105"/>
       <c r="C105"/>
     </row>
     <row r="106" spans="1:3">
@@ -37307,8 +37306,8 @@
   <sheetPr/>
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -40292,7 +40291,7 @@
         <v>KPI Period Management</v>
       </c>
       <c r="F154" t="str">
-        <v>S_HRM_LUONG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -40312,7 +40311,7 @@
         <v>KPI Period Management</v>
       </c>
       <c r="F155" t="str">
-        <v>S_HRM_LUONG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -40332,7 +40331,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F156" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -40352,7 +40351,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F157" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -40372,7 +40371,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F158" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -40392,7 +40391,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F159" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -40412,7 +40411,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F160" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -40432,7 +40431,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F161" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -40452,7 +40451,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F162" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -40472,7 +40471,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F163" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -40492,7 +40491,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F164" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -40512,7 +40511,7 @@
         <v>Đề xuất</v>
       </c>
       <c r="F165" t="str">
-        <v>S_NV_CHUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
   </sheetData>
@@ -40526,8 +40525,8 @@
   <sheetPr/>
   <dimension ref="A1:F754"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A658" workbookViewId="0">
-      <selection activeCell="B671" sqref="B671"/>
+    <sheetView topLeftCell="A711" workbookViewId="0">
+      <selection activeCell="A746" sqref="A746:G746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -52310,7 +52309,7 @@
         <v>KPI Period Management</v>
       </c>
       <c r="F652" t="str">
-        <v>S_HRM_LUONG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="653" spans="1:6">
@@ -52330,7 +52329,7 @@
         <v>KPI Period Management</v>
       </c>
       <c r="F653" t="str">
-        <v>S_HRM_LUONG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="654" spans="1:6">
@@ -52350,7 +52349,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F654" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="655" spans="1:6">
@@ -52370,7 +52369,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F655" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="656" spans="1:6">
@@ -52390,7 +52389,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F656" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="657" spans="1:6">
@@ -52410,7 +52409,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F657" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="658" spans="1:6">
@@ -52430,7 +52429,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F658" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="659" spans="1:6">
@@ -52450,7 +52449,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F659" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="660" spans="1:6">
@@ -52470,7 +52469,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F660" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="661" spans="1:6">
@@ -52490,7 +52489,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F661" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="662" spans="1:6">
@@ -52510,7 +52509,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F662" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="663" spans="1:6">
@@ -52530,7 +52529,7 @@
         <v>Đề xuất</v>
       </c>
       <c r="F663" t="str">
-        <v>S_NV_CHUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="664" spans="1:2">
@@ -62564,7 +62563,7 @@
         <v>KPI Management</v>
       </c>
       <c r="F525" t="str">
-        <v/>
+        <v>S_HRM_TONG</v>
       </c>
     </row>
     <row r="533" spans="1:6">
@@ -67427,7 +67426,7 @@
         <v>KPI Period Management</v>
       </c>
       <c r="F789" t="str">
-        <v>S_HRM_LUONG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="790" spans="1:6">
@@ -67447,7 +67446,7 @@
         <v>KPI Period Management</v>
       </c>
       <c r="F790" t="str">
-        <v>S_HRM_LUONG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="791" spans="1:6">
@@ -67467,7 +67466,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F791" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="792" spans="1:6">
@@ -67487,7 +67486,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F792" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="793" spans="1:6">
@@ -67507,7 +67506,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F793" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="794" spans="1:6">
@@ -67527,7 +67526,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F794" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="795" spans="1:6">
@@ -67547,7 +67546,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F795" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="796" spans="1:6">
@@ -67567,7 +67566,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F796" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="797" spans="1:6">
@@ -67587,7 +67586,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F797" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="798" spans="1:6">
@@ -67607,7 +67606,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F798" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="799" spans="1:6">
@@ -67627,7 +67626,7 @@
         <v>Tuyển dụng</v>
       </c>
       <c r="F799" t="str">
-        <v>S_HRM_TUYENDUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="800" spans="1:6">
@@ -67647,7 +67646,7 @@
         <v>Đề xuất</v>
       </c>
       <c r="F800" t="str">
-        <v>S_NV_CHUNG</v>
+        <v>S_TRUONGPHONG</v>
       </c>
     </row>
     <row r="821" spans="1:6">
@@ -70330,7 +70329,7 @@
   <sheetPr/>
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A71" workbookViewId="0">
       <selection activeCell="A30" sqref="A22:F30"/>
     </sheetView>
   </sheetViews>
@@ -78684,8 +78683,8 @@
   <sheetPr/>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -79575,7 +79574,7 @@
         <v>1130</v>
       </c>
       <c r="F44" t="s">
-        <v>932</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -79595,7 +79594,7 @@
         <v>1130</v>
       </c>
       <c r="F45" t="s">
-        <v>932</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -79615,7 +79614,7 @@
         <v>287</v>
       </c>
       <c r="F46" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -79635,7 +79634,7 @@
         <v>287</v>
       </c>
       <c r="F47" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -79655,7 +79654,7 @@
         <v>287</v>
       </c>
       <c r="F48" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -79675,7 +79674,7 @@
         <v>287</v>
       </c>
       <c r="F49" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -79695,7 +79694,7 @@
         <v>287</v>
       </c>
       <c r="F50" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -79715,7 +79714,7 @@
         <v>287</v>
       </c>
       <c r="F51" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -79735,7 +79734,7 @@
         <v>287</v>
       </c>
       <c r="F52" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -79755,7 +79754,7 @@
         <v>287</v>
       </c>
       <c r="F53" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -79775,7 +79774,7 @@
         <v>287</v>
       </c>
       <c r="F54" t="s">
-        <v>288</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -79795,7 +79794,7 @@
         <v>167</v>
       </c>
       <c r="F55" t="s">
-        <v>70</v>
+        <v>1477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>